<commit_message>
Ajusta dias e acrescenta feriados no cronograma modelo
</commit_message>
<xml_diff>
--- a/Cronograma/Projeto-Cronograma - Acompanhamento.xlsx
+++ b/Cronograma/Projeto-Cronograma - Acompanhamento.xlsx
@@ -833,35 +833,7 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -885,12 +857,40 @@
       <alignment textRotation="255"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1174,7 +1174,7 @@
   <dimension ref="A1:DL942"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="BU4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
       <selection pane="bottomRight" activeCell="Q11" sqref="Q11"/>
@@ -1192,7 +1192,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:116" ht="14.25" customHeight="1">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="91" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -1532,7 +1532,7 @@
       </c>
     </row>
     <row r="2" spans="1:116" ht="14.25" customHeight="1">
-      <c r="A2" s="79"/>
+      <c r="A2" s="90"/>
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
@@ -1858,15 +1858,15 @@
         <v>12</v>
       </c>
       <c r="DF2" s="11"/>
-      <c r="DG2" s="81"/>
-      <c r="DH2" s="79"/>
-      <c r="DI2" s="79"/>
-      <c r="DJ2" s="79"/>
+      <c r="DG2" s="92"/>
+      <c r="DH2" s="90"/>
+      <c r="DI2" s="90"/>
+      <c r="DJ2" s="90"/>
       <c r="DK2" s="77"/>
       <c r="DL2" s="77"/>
     </row>
     <row r="3" spans="1:116" ht="14.25" customHeight="1">
-      <c r="A3" s="79"/>
+      <c r="A3" s="90"/>
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
@@ -2203,7 +2203,7 @@
       <c r="A4" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="82" t="s">
+      <c r="B4" s="93" t="s">
         <v>38</v>
       </c>
       <c r="C4" s="19" t="s">
@@ -2345,7 +2345,7 @@
       <c r="A5" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="79"/>
+      <c r="B5" s="90"/>
       <c r="C5" s="21"/>
       <c r="D5" s="21"/>
       <c r="E5" s="21"/>
@@ -2485,7 +2485,7 @@
       <c r="A6" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="B6" s="79"/>
+      <c r="B6" s="90"/>
       <c r="C6" s="21"/>
       <c r="D6" s="21"/>
       <c r="E6" s="21"/>
@@ -2625,7 +2625,7 @@
       <c r="A7" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="B7" s="79"/>
+      <c r="B7" s="90"/>
       <c r="C7" s="21"/>
       <c r="D7" s="21"/>
       <c r="E7" s="21"/>
@@ -2763,7 +2763,7 @@
       <c r="A8" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="B8" s="79"/>
+      <c r="B8" s="90"/>
       <c r="C8" s="21"/>
       <c r="D8" s="21"/>
       <c r="E8" s="21"/>
@@ -2903,7 +2903,7 @@
       <c r="A9" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="B9" s="83" t="s">
+      <c r="B9" s="94" t="s">
         <v>58</v>
       </c>
       <c r="C9" s="21"/>
@@ -3045,7 +3045,7 @@
       <c r="A10" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="B10" s="79"/>
+      <c r="B10" s="90"/>
       <c r="C10" s="21"/>
       <c r="D10" s="21"/>
       <c r="E10" s="21"/>
@@ -3185,7 +3185,7 @@
       <c r="A11" s="32" t="s">
         <v>65</v>
       </c>
-      <c r="B11" s="84" t="s">
+      <c r="B11" s="95" t="s">
         <v>66</v>
       </c>
       <c r="C11" s="21"/>
@@ -3315,7 +3315,7 @@
       <c r="A12" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="B12" s="79"/>
+      <c r="B12" s="90"/>
       <c r="C12" s="21"/>
       <c r="D12" s="21"/>
       <c r="E12" s="21"/>
@@ -3453,7 +3453,7 @@
       <c r="A13" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="B13" s="79"/>
+      <c r="B13" s="90"/>
       <c r="C13" s="21"/>
       <c r="D13" s="21"/>
       <c r="E13" s="21"/>
@@ -3593,7 +3593,7 @@
       <c r="A14" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="B14" s="79"/>
+      <c r="B14" s="90"/>
       <c r="C14" s="21"/>
       <c r="D14" s="21"/>
       <c r="E14" s="21"/>
@@ -3729,7 +3729,7 @@
       <c r="A15" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="79"/>
+      <c r="B15" s="90"/>
       <c r="C15" s="21"/>
       <c r="D15" s="21"/>
       <c r="E15" s="21"/>
@@ -3865,7 +3865,7 @@
       <c r="A16" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="B16" s="79"/>
+      <c r="B16" s="90"/>
       <c r="C16" s="21"/>
       <c r="D16" s="21"/>
       <c r="E16" s="21"/>
@@ -4001,7 +4001,7 @@
       <c r="A17" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="B17" s="79"/>
+      <c r="B17" s="90"/>
       <c r="C17" s="21"/>
       <c r="D17" s="21"/>
       <c r="E17" s="21"/>
@@ -4137,7 +4137,7 @@
       <c r="A18" s="34" t="s">
         <v>79</v>
       </c>
-      <c r="B18" s="79"/>
+      <c r="B18" s="90"/>
       <c r="C18" s="21"/>
       <c r="D18" s="21"/>
       <c r="E18" s="21"/>
@@ -4277,7 +4277,7 @@
       <c r="A19" s="39" t="s">
         <v>81</v>
       </c>
-      <c r="B19" s="79"/>
+      <c r="B19" s="90"/>
       <c r="C19" s="21"/>
       <c r="D19" s="21"/>
       <c r="E19" s="21"/>
@@ -4413,7 +4413,7 @@
       <c r="A20" s="42" t="s">
         <v>82</v>
       </c>
-      <c r="B20" s="79"/>
+      <c r="B20" s="90"/>
       <c r="C20" s="21"/>
       <c r="D20" s="21"/>
       <c r="E20" s="21"/>
@@ -4549,7 +4549,7 @@
       <c r="A21" s="45" t="s">
         <v>85</v>
       </c>
-      <c r="B21" s="85" t="s">
+      <c r="B21" s="96" t="s">
         <v>86</v>
       </c>
       <c r="C21" s="21"/>
@@ -4683,7 +4683,7 @@
       <c r="A22" s="49" t="s">
         <v>88</v>
       </c>
-      <c r="B22" s="79"/>
+      <c r="B22" s="90"/>
       <c r="C22" s="21"/>
       <c r="D22" s="21"/>
       <c r="E22" s="21"/>
@@ -4819,7 +4819,7 @@
       <c r="A23" s="53" t="s">
         <v>89</v>
       </c>
-      <c r="B23" s="79"/>
+      <c r="B23" s="90"/>
       <c r="C23" s="21"/>
       <c r="D23" s="21"/>
       <c r="E23" s="21"/>
@@ -4951,7 +4951,7 @@
       <c r="A24" s="56" t="s">
         <v>90</v>
       </c>
-      <c r="B24" s="79"/>
+      <c r="B24" s="90"/>
       <c r="C24" s="21"/>
       <c r="D24" s="21"/>
       <c r="E24" s="21"/>
@@ -5085,7 +5085,7 @@
       <c r="A25" s="59" t="s">
         <v>92</v>
       </c>
-      <c r="B25" s="79"/>
+      <c r="B25" s="90"/>
       <c r="C25" s="21"/>
       <c r="D25" s="21"/>
       <c r="E25" s="21"/>
@@ -5229,7 +5229,7 @@
       <c r="A26" s="61" t="s">
         <v>93</v>
       </c>
-      <c r="B26" s="78" t="s">
+      <c r="B26" s="89" t="s">
         <v>58</v>
       </c>
       <c r="C26" s="21"/>
@@ -5363,7 +5363,7 @@
       <c r="A27" s="64" t="s">
         <v>95</v>
       </c>
-      <c r="B27" s="79"/>
+      <c r="B27" s="90"/>
       <c r="C27" s="21"/>
       <c r="D27" s="21"/>
       <c r="E27" s="21"/>
@@ -5503,7 +5503,7 @@
       <c r="A28" s="67" t="s">
         <v>97</v>
       </c>
-      <c r="B28" s="79"/>
+      <c r="B28" s="90"/>
       <c r="C28" s="21"/>
       <c r="D28" s="21"/>
       <c r="E28" s="21"/>
@@ -5635,7 +5635,7 @@
       <c r="A29" s="70" t="s">
         <v>99</v>
       </c>
-      <c r="B29" s="79"/>
+      <c r="B29" s="90"/>
       <c r="C29" s="21"/>
       <c r="D29" s="21"/>
       <c r="E29" s="21"/>
@@ -5763,7 +5763,7 @@
       <c r="A30" s="73" t="s">
         <v>100</v>
       </c>
-      <c r="B30" s="79"/>
+      <c r="B30" s="90"/>
       <c r="C30" s="21"/>
       <c r="D30" s="21"/>
       <c r="E30" s="21"/>
@@ -5889,7 +5889,7 @@
       <c r="A31" s="61" t="s">
         <v>101</v>
       </c>
-      <c r="B31" s="79"/>
+      <c r="B31" s="90"/>
       <c r="C31" s="21"/>
       <c r="D31" s="21"/>
       <c r="E31" s="21"/>
@@ -6983,989 +6983,989 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CR39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AF1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="CO3" sqref="CO3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
     <col min="1" max="1" width="16.21875" customWidth="1"/>
-    <col min="3" max="17" width="5.77734375" style="86" customWidth="1"/>
+    <col min="3" max="17" width="5.77734375" style="78" customWidth="1"/>
     <col min="18" max="47" width="5.77734375" customWidth="1"/>
-    <col min="48" max="48" width="3.77734375" style="95" customWidth="1"/>
-    <col min="49" max="49" width="3.77734375" style="94" customWidth="1"/>
+    <col min="48" max="48" width="3.77734375" style="85" customWidth="1"/>
+    <col min="49" max="49" width="3.77734375" style="84" customWidth="1"/>
     <col min="50" max="71" width="5.77734375" customWidth="1"/>
-    <col min="72" max="72" width="3.77734375" style="94" customWidth="1"/>
+    <col min="72" max="72" width="3.77734375" style="84" customWidth="1"/>
     <col min="73" max="74" width="5.77734375" customWidth="1"/>
-    <col min="75" max="75" width="3.77734375" style="94" customWidth="1"/>
+    <col min="75" max="75" width="3.77734375" style="84" customWidth="1"/>
     <col min="76" max="92" width="5.77734375" customWidth="1"/>
-    <col min="93" max="93" width="5.77734375" style="99" customWidth="1"/>
+    <col min="93" max="93" width="5.77734375" style="88" customWidth="1"/>
     <col min="94" max="96" width="5.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:96">
-      <c r="A1" s="88" t="s">
+      <c r="A1" s="97" t="s">
         <v>110</v>
       </c>
-      <c r="B1" s="86" t="s">
+      <c r="B1" s="78" t="s">
         <v>105</v>
       </c>
-      <c r="C1" s="86">
+      <c r="C1" s="78">
         <v>14</v>
       </c>
-      <c r="D1" s="86">
+      <c r="D1" s="78">
         <v>15</v>
       </c>
-      <c r="E1" s="86">
+      <c r="E1" s="78">
         <v>16</v>
       </c>
-      <c r="F1" s="86">
+      <c r="F1" s="78">
         <v>17</v>
       </c>
-      <c r="G1" s="86">
+      <c r="G1" s="78">
         <v>18</v>
       </c>
-      <c r="H1" s="86">
+      <c r="H1" s="78">
         <v>19</v>
       </c>
-      <c r="I1" s="86">
+      <c r="I1" s="78">
         <v>20</v>
       </c>
-      <c r="J1" s="86">
+      <c r="J1" s="78">
         <v>21</v>
       </c>
-      <c r="K1" s="86">
+      <c r="K1" s="78">
         <v>22</v>
       </c>
-      <c r="L1" s="86">
+      <c r="L1" s="78">
         <v>23</v>
       </c>
-      <c r="M1" s="86">
+      <c r="M1" s="78">
         <v>24</v>
       </c>
-      <c r="N1" s="86">
+      <c r="N1" s="78">
         <v>25</v>
       </c>
-      <c r="O1" s="86">
+      <c r="O1" s="78">
         <v>26</v>
       </c>
-      <c r="P1" s="86">
+      <c r="P1" s="78">
         <v>27</v>
       </c>
-      <c r="Q1" s="86">
+      <c r="Q1" s="78">
         <v>28</v>
       </c>
-      <c r="R1" s="86">
+      <c r="R1" s="78">
         <v>29</v>
       </c>
-      <c r="S1" s="86">
+      <c r="S1" s="78">
         <v>30</v>
       </c>
-      <c r="T1" s="86">
+      <c r="T1" s="78">
         <v>31</v>
       </c>
-      <c r="U1" s="86">
+      <c r="U1" s="78">
         <v>32</v>
       </c>
-      <c r="V1" s="86">
+      <c r="V1" s="78">
         <v>33</v>
       </c>
-      <c r="W1" s="86">
+      <c r="W1" s="78">
         <v>34</v>
       </c>
-      <c r="X1" s="86">
+      <c r="X1" s="78">
         <v>35</v>
       </c>
-      <c r="Y1" s="86">
+      <c r="Y1" s="78">
         <v>36</v>
       </c>
-      <c r="Z1" s="86">
+      <c r="Z1" s="78">
         <v>37</v>
       </c>
-      <c r="AA1" s="86">
+      <c r="AA1" s="78">
         <v>38</v>
       </c>
-      <c r="AB1" s="86">
+      <c r="AB1" s="78">
         <v>39</v>
       </c>
-      <c r="AC1" s="86">
+      <c r="AC1" s="78">
         <v>40</v>
       </c>
-      <c r="AD1" s="86">
+      <c r="AD1" s="78">
         <v>41</v>
       </c>
-      <c r="AE1" s="86">
+      <c r="AE1" s="78">
         <v>42</v>
       </c>
-      <c r="AF1" s="86">
+      <c r="AF1" s="78">
         <v>43</v>
       </c>
-      <c r="AG1" s="86">
+      <c r="AG1" s="78">
         <v>44</v>
       </c>
-      <c r="AH1" s="86">
+      <c r="AH1" s="78">
         <v>45</v>
       </c>
-      <c r="AI1" s="86">
+      <c r="AI1" s="78">
         <v>46</v>
       </c>
-      <c r="AJ1" s="86">
+      <c r="AJ1" s="78">
         <v>47</v>
       </c>
-      <c r="AK1" s="86">
+      <c r="AK1" s="78">
         <v>48</v>
       </c>
-      <c r="AL1" s="86">
+      <c r="AL1" s="78">
         <v>49</v>
       </c>
-      <c r="AM1" s="86">
+      <c r="AM1" s="78">
         <v>50</v>
       </c>
-      <c r="AN1" s="86">
+      <c r="AN1" s="78">
         <v>51</v>
       </c>
-      <c r="AO1" s="86">
+      <c r="AO1" s="78">
         <v>52</v>
       </c>
-      <c r="AP1" s="86">
+      <c r="AP1" s="78">
         <v>53</v>
       </c>
-      <c r="AQ1" s="86">
+      <c r="AQ1" s="78">
         <v>54</v>
       </c>
-      <c r="AR1" s="86">
+      <c r="AR1" s="78">
         <v>55</v>
       </c>
-      <c r="AS1" s="86">
+      <c r="AS1" s="78">
         <v>56</v>
       </c>
-      <c r="AT1" s="86">
+      <c r="AT1" s="78">
         <v>57</v>
       </c>
-      <c r="AU1" s="86">
+      <c r="AU1" s="78">
         <v>58</v>
       </c>
-      <c r="AV1" s="93"/>
-      <c r="AW1" s="93"/>
-      <c r="AX1" s="86">
+      <c r="AV1" s="83"/>
+      <c r="AW1" s="83"/>
+      <c r="AX1" s="78">
         <v>59</v>
       </c>
-      <c r="AY1" s="86">
+      <c r="AY1" s="78">
         <v>60</v>
       </c>
-      <c r="AZ1" s="86">
+      <c r="AZ1" s="78">
         <v>61</v>
       </c>
-      <c r="BA1" s="86">
+      <c r="BA1" s="78">
         <v>62</v>
       </c>
-      <c r="BB1" s="86">
+      <c r="BB1" s="78">
         <v>63</v>
       </c>
-      <c r="BC1" s="86">
+      <c r="BC1" s="78">
         <v>64</v>
       </c>
-      <c r="BD1" s="86">
+      <c r="BD1" s="78">
         <v>65</v>
       </c>
-      <c r="BE1" s="86">
+      <c r="BE1" s="78">
         <v>66</v>
       </c>
-      <c r="BF1" s="86">
+      <c r="BF1" s="78">
         <v>67</v>
       </c>
-      <c r="BG1" s="86">
+      <c r="BG1" s="78">
         <v>68</v>
       </c>
-      <c r="BH1" s="86">
+      <c r="BH1" s="78">
         <v>69</v>
       </c>
-      <c r="BI1" s="86">
+      <c r="BI1" s="78">
         <v>70</v>
       </c>
-      <c r="BJ1" s="86">
+      <c r="BJ1" s="78">
         <v>71</v>
       </c>
-      <c r="BK1" s="86">
+      <c r="BK1" s="78">
         <v>72</v>
       </c>
-      <c r="BL1" s="86">
+      <c r="BL1" s="78">
         <v>73</v>
       </c>
-      <c r="BM1" s="86">
+      <c r="BM1" s="78">
         <v>74</v>
       </c>
-      <c r="BN1" s="86">
+      <c r="BN1" s="78">
         <v>75</v>
       </c>
-      <c r="BO1" s="86">
+      <c r="BO1" s="78">
         <v>76</v>
       </c>
-      <c r="BP1" s="86">
+      <c r="BP1" s="78">
         <v>77</v>
       </c>
-      <c r="BQ1" s="86">
+      <c r="BQ1" s="78">
         <v>78</v>
       </c>
-      <c r="BR1" s="86">
+      <c r="BR1" s="78">
         <v>79</v>
       </c>
-      <c r="BS1" s="86">
+      <c r="BS1" s="78">
         <v>80</v>
       </c>
-      <c r="BT1" s="93"/>
-      <c r="BU1" s="86">
+      <c r="BT1" s="83"/>
+      <c r="BU1" s="78">
         <v>81</v>
       </c>
-      <c r="BV1" s="86">
+      <c r="BV1" s="78">
         <v>82</v>
       </c>
-      <c r="BW1" s="93"/>
-      <c r="BX1" s="86">
+      <c r="BW1" s="83"/>
+      <c r="BX1" s="78">
         <v>83</v>
       </c>
-      <c r="BY1" s="86">
+      <c r="BY1" s="78">
         <v>84</v>
       </c>
-      <c r="BZ1" s="86">
+      <c r="BZ1" s="78">
         <v>85</v>
       </c>
-      <c r="CA1" s="86">
+      <c r="CA1" s="78">
         <v>86</v>
       </c>
-      <c r="CB1" s="86">
+      <c r="CB1" s="78">
         <v>87</v>
       </c>
-      <c r="CC1" s="86">
+      <c r="CC1" s="78">
         <v>88</v>
       </c>
-      <c r="CD1" s="86">
+      <c r="CD1" s="78">
         <v>89</v>
       </c>
-      <c r="CE1" s="86">
+      <c r="CE1" s="78">
         <v>90</v>
       </c>
-      <c r="CF1" s="86">
+      <c r="CF1" s="78">
         <v>91</v>
       </c>
-      <c r="CG1" s="86">
+      <c r="CG1" s="78">
         <v>92</v>
       </c>
-      <c r="CH1" s="86">
+      <c r="CH1" s="78">
         <v>93</v>
       </c>
-      <c r="CI1" s="86">
+      <c r="CI1" s="78">
         <v>94</v>
       </c>
-      <c r="CJ1" s="86">
+      <c r="CJ1" s="78">
         <v>95</v>
       </c>
-      <c r="CK1" s="86">
+      <c r="CK1" s="78">
         <v>96</v>
       </c>
-      <c r="CL1" s="86">
+      <c r="CL1" s="78">
         <v>97</v>
       </c>
-      <c r="CM1" s="86">
+      <c r="CM1" s="78">
         <v>98</v>
       </c>
-      <c r="CN1" s="86">
+      <c r="CN1" s="78">
         <v>99</v>
       </c>
-      <c r="CO1" s="98"/>
-      <c r="CP1" s="86">
+      <c r="CO1" s="87"/>
+      <c r="CP1" s="78">
         <v>100</v>
       </c>
-      <c r="CQ1" s="86">
+      <c r="CQ1" s="78">
         <v>101</v>
       </c>
-      <c r="CR1" s="86">
+      <c r="CR1" s="78">
         <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:96" ht="19.95" customHeight="1">
-      <c r="A2" s="87"/>
-      <c r="B2" s="86" t="s">
+      <c r="A2" s="98"/>
+      <c r="B2" s="78" t="s">
         <v>104</v>
       </c>
-      <c r="C2" s="87" t="s">
+      <c r="C2" s="98" t="s">
         <v>109</v>
       </c>
-      <c r="D2" s="87"/>
-      <c r="E2" s="87"/>
-      <c r="F2" s="87"/>
-      <c r="G2" s="87"/>
-      <c r="H2" s="87"/>
-      <c r="I2" s="87"/>
-      <c r="J2" s="87"/>
-      <c r="K2" s="87"/>
-      <c r="L2" s="87"/>
-      <c r="M2" s="87"/>
-      <c r="N2" s="87"/>
-      <c r="O2" s="87"/>
-      <c r="P2" s="87"/>
-      <c r="Q2" s="87"/>
-      <c r="R2" s="88" t="s">
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="98"/>
+      <c r="H2" s="98"/>
+      <c r="I2" s="98"/>
+      <c r="J2" s="98"/>
+      <c r="K2" s="98"/>
+      <c r="L2" s="98"/>
+      <c r="M2" s="98"/>
+      <c r="N2" s="98"/>
+      <c r="O2" s="98"/>
+      <c r="P2" s="98"/>
+      <c r="Q2" s="98"/>
+      <c r="R2" s="97" t="s">
         <v>111</v>
       </c>
-      <c r="S2" s="87"/>
-      <c r="T2" s="87"/>
-      <c r="U2" s="87"/>
-      <c r="V2" s="87"/>
-      <c r="W2" s="87"/>
-      <c r="X2" s="87"/>
-      <c r="Y2" s="87"/>
-      <c r="Z2" s="87"/>
-      <c r="AA2" s="87"/>
-      <c r="AB2" s="87"/>
-      <c r="AC2" s="87"/>
-      <c r="AD2" s="87"/>
-      <c r="AE2" s="87"/>
-      <c r="AF2" s="87"/>
-      <c r="AG2" s="87"/>
-      <c r="AH2" s="87"/>
-      <c r="AI2" s="87"/>
-      <c r="AJ2" s="87"/>
-      <c r="AK2" s="87"/>
-      <c r="AL2" s="87"/>
-      <c r="AM2" s="88" t="s">
+      <c r="S2" s="98"/>
+      <c r="T2" s="98"/>
+      <c r="U2" s="98"/>
+      <c r="V2" s="98"/>
+      <c r="W2" s="98"/>
+      <c r="X2" s="98"/>
+      <c r="Y2" s="98"/>
+      <c r="Z2" s="98"/>
+      <c r="AA2" s="98"/>
+      <c r="AB2" s="98"/>
+      <c r="AC2" s="98"/>
+      <c r="AD2" s="98"/>
+      <c r="AE2" s="98"/>
+      <c r="AF2" s="98"/>
+      <c r="AG2" s="98"/>
+      <c r="AH2" s="98"/>
+      <c r="AI2" s="98"/>
+      <c r="AJ2" s="98"/>
+      <c r="AK2" s="98"/>
+      <c r="AL2" s="98"/>
+      <c r="AM2" s="97" t="s">
         <v>112</v>
       </c>
-      <c r="AN2" s="87"/>
-      <c r="AO2" s="87"/>
-      <c r="AP2" s="87"/>
-      <c r="AQ2" s="87"/>
-      <c r="AR2" s="87"/>
-      <c r="AS2" s="87"/>
-      <c r="AT2" s="87"/>
-      <c r="AU2" s="87"/>
-      <c r="AV2" s="87"/>
-      <c r="AW2" s="87"/>
-      <c r="AX2" s="87"/>
-      <c r="AY2" s="87"/>
-      <c r="AZ2" s="87"/>
-      <c r="BA2" s="87"/>
-      <c r="BB2" s="87"/>
-      <c r="BC2" s="87"/>
-      <c r="BD2" s="87"/>
-      <c r="BE2" s="87"/>
-      <c r="BF2" s="87"/>
-      <c r="BG2" s="87"/>
-      <c r="BH2" s="87"/>
-      <c r="BI2" s="87"/>
-      <c r="BJ2" s="88" t="s">
+      <c r="AN2" s="98"/>
+      <c r="AO2" s="98"/>
+      <c r="AP2" s="98"/>
+      <c r="AQ2" s="98"/>
+      <c r="AR2" s="98"/>
+      <c r="AS2" s="98"/>
+      <c r="AT2" s="98"/>
+      <c r="AU2" s="98"/>
+      <c r="AV2" s="98"/>
+      <c r="AW2" s="98"/>
+      <c r="AX2" s="98"/>
+      <c r="AY2" s="98"/>
+      <c r="AZ2" s="98"/>
+      <c r="BA2" s="98"/>
+      <c r="BB2" s="98"/>
+      <c r="BC2" s="98"/>
+      <c r="BD2" s="98"/>
+      <c r="BE2" s="98"/>
+      <c r="BF2" s="98"/>
+      <c r="BG2" s="98"/>
+      <c r="BH2" s="98"/>
+      <c r="BI2" s="98"/>
+      <c r="BJ2" s="97" t="s">
         <v>113</v>
       </c>
-      <c r="BK2" s="87"/>
-      <c r="BL2" s="87"/>
-      <c r="BM2" s="87"/>
-      <c r="BN2" s="87"/>
-      <c r="BO2" s="87"/>
-      <c r="BP2" s="87"/>
-      <c r="BQ2" s="87"/>
-      <c r="BR2" s="87"/>
-      <c r="BS2" s="87"/>
-      <c r="BT2" s="87"/>
-      <c r="BU2" s="87"/>
-      <c r="BV2" s="87"/>
-      <c r="BW2" s="87"/>
-      <c r="BX2" s="87"/>
-      <c r="BY2" s="87"/>
-      <c r="BZ2" s="87"/>
-      <c r="CA2" s="87"/>
-      <c r="CB2" s="87"/>
-      <c r="CC2" s="87"/>
-      <c r="CD2" s="87"/>
-      <c r="CE2" s="88" t="s">
+      <c r="BK2" s="98"/>
+      <c r="BL2" s="98"/>
+      <c r="BM2" s="98"/>
+      <c r="BN2" s="98"/>
+      <c r="BO2" s="98"/>
+      <c r="BP2" s="98"/>
+      <c r="BQ2" s="98"/>
+      <c r="BR2" s="98"/>
+      <c r="BS2" s="98"/>
+      <c r="BT2" s="98"/>
+      <c r="BU2" s="98"/>
+      <c r="BV2" s="98"/>
+      <c r="BW2" s="98"/>
+      <c r="BX2" s="98"/>
+      <c r="BY2" s="98"/>
+      <c r="BZ2" s="98"/>
+      <c r="CA2" s="98"/>
+      <c r="CB2" s="98"/>
+      <c r="CC2" s="98"/>
+      <c r="CD2" s="98"/>
+      <c r="CE2" s="97" t="s">
         <v>114</v>
       </c>
-      <c r="CF2" s="88"/>
-      <c r="CG2" s="88"/>
-      <c r="CH2" s="88"/>
-      <c r="CI2" s="88"/>
-      <c r="CJ2" s="88"/>
-      <c r="CK2" s="88"/>
-      <c r="CL2" s="88"/>
-      <c r="CM2" s="88"/>
-      <c r="CN2" s="88"/>
-      <c r="CO2" s="88"/>
-      <c r="CP2" s="88"/>
-      <c r="CQ2" s="88"/>
-      <c r="CR2" s="88"/>
+      <c r="CF2" s="97"/>
+      <c r="CG2" s="97"/>
+      <c r="CH2" s="97"/>
+      <c r="CI2" s="97"/>
+      <c r="CJ2" s="97"/>
+      <c r="CK2" s="97"/>
+      <c r="CL2" s="97"/>
+      <c r="CM2" s="97"/>
+      <c r="CN2" s="97"/>
+      <c r="CO2" s="97"/>
+      <c r="CP2" s="97"/>
+      <c r="CQ2" s="97"/>
+      <c r="CR2" s="97"/>
     </row>
     <row r="3" spans="1:96">
-      <c r="A3" s="87"/>
-      <c r="B3" s="86" t="s">
+      <c r="A3" s="98"/>
+      <c r="B3" s="78" t="s">
         <v>103</v>
       </c>
-      <c r="C3" s="86">
+      <c r="C3" s="78">
         <v>12</v>
       </c>
-      <c r="D3" s="86">
+      <c r="D3" s="78">
         <v>13</v>
       </c>
-      <c r="E3" s="86">
+      <c r="E3" s="78">
         <v>14</v>
       </c>
-      <c r="F3" s="86">
+      <c r="F3" s="78">
         <v>15</v>
       </c>
-      <c r="G3" s="86">
+      <c r="G3" s="78">
         <v>16</v>
       </c>
-      <c r="H3" s="86">
+      <c r="H3" s="78">
         <v>19</v>
       </c>
-      <c r="I3" s="86">
+      <c r="I3" s="78">
         <v>20</v>
       </c>
-      <c r="J3" s="86">
+      <c r="J3" s="78">
         <v>21</v>
       </c>
-      <c r="K3" s="86">
+      <c r="K3" s="78">
         <v>22</v>
       </c>
-      <c r="L3" s="86">
+      <c r="L3" s="78">
         <v>23</v>
       </c>
-      <c r="M3" s="86">
+      <c r="M3" s="78">
         <v>26</v>
       </c>
-      <c r="N3" s="86">
+      <c r="N3" s="78">
         <v>27</v>
       </c>
-      <c r="O3" s="86">
+      <c r="O3" s="78">
         <v>28</v>
       </c>
-      <c r="P3" s="86">
+      <c r="P3" s="78">
         <v>29</v>
       </c>
-      <c r="Q3" s="86">
+      <c r="Q3" s="78">
         <v>30</v>
       </c>
-      <c r="R3" s="86">
+      <c r="R3" s="78">
         <v>2</v>
       </c>
-      <c r="S3" s="86">
+      <c r="S3" s="78">
         <v>3</v>
       </c>
-      <c r="T3" s="86">
+      <c r="T3" s="78">
         <v>4</v>
       </c>
-      <c r="U3" s="86">
+      <c r="U3" s="78">
         <v>5</v>
       </c>
-      <c r="V3" s="86">
+      <c r="V3" s="78">
         <v>6</v>
       </c>
-      <c r="W3" s="86">
+      <c r="W3" s="78">
         <v>9</v>
       </c>
-      <c r="X3" s="86">
+      <c r="X3" s="78">
         <v>10</v>
       </c>
-      <c r="Y3" s="86">
+      <c r="Y3" s="78">
         <v>11</v>
       </c>
-      <c r="Z3" s="86">
+      <c r="Z3" s="78">
         <v>12</v>
       </c>
-      <c r="AA3" s="86">
+      <c r="AA3" s="78">
         <v>13</v>
       </c>
-      <c r="AB3" s="86">
+      <c r="AB3" s="78">
         <v>16</v>
       </c>
-      <c r="AC3" s="86">
+      <c r="AC3" s="78">
         <v>17</v>
       </c>
-      <c r="AD3" s="86">
+      <c r="AD3" s="78">
         <v>18</v>
       </c>
-      <c r="AE3" s="86">
+      <c r="AE3" s="78">
         <v>19</v>
       </c>
-      <c r="AF3" s="86">
+      <c r="AF3" s="78">
         <v>20</v>
       </c>
-      <c r="AG3" s="86">
+      <c r="AG3" s="78">
         <v>23</v>
       </c>
-      <c r="AH3" s="86">
+      <c r="AH3" s="78">
         <v>24</v>
       </c>
-      <c r="AI3" s="86">
+      <c r="AI3" s="78">
         <v>25</v>
       </c>
-      <c r="AJ3" s="86">
+      <c r="AJ3" s="78">
         <v>26</v>
       </c>
-      <c r="AK3" s="86">
+      <c r="AK3" s="78">
         <v>27</v>
       </c>
-      <c r="AL3" s="86">
+      <c r="AL3" s="78">
         <v>30</v>
       </c>
-      <c r="AM3" s="86">
+      <c r="AM3" s="78">
         <v>1</v>
       </c>
-      <c r="AN3" s="86">
+      <c r="AN3" s="78">
         <v>2</v>
       </c>
-      <c r="AO3" s="86">
+      <c r="AO3" s="78">
         <v>3</v>
       </c>
-      <c r="AP3" s="86">
+      <c r="AP3" s="78">
         <v>4</v>
       </c>
-      <c r="AQ3" s="86">
+      <c r="AQ3" s="78">
         <v>7</v>
       </c>
-      <c r="AR3" s="86">
+      <c r="AR3" s="78">
         <v>8</v>
       </c>
-      <c r="AS3" s="86">
+      <c r="AS3" s="78">
         <v>9</v>
       </c>
-      <c r="AT3" s="86">
+      <c r="AT3" s="78">
         <v>10</v>
       </c>
-      <c r="AU3" s="86">
+      <c r="AU3" s="78">
         <v>11</v>
       </c>
-      <c r="AV3" s="98">
+      <c r="AV3" s="87">
         <v>14</v>
       </c>
-      <c r="AW3" s="98">
+      <c r="AW3" s="87">
         <v>15</v>
       </c>
-      <c r="AX3" s="86">
+      <c r="AX3" s="78">
         <v>16</v>
       </c>
-      <c r="AY3" s="86">
+      <c r="AY3" s="78">
         <v>17</v>
       </c>
-      <c r="AZ3" s="86">
+      <c r="AZ3" s="78">
         <v>18</v>
       </c>
-      <c r="BA3" s="86">
+      <c r="BA3" s="78">
         <v>21</v>
       </c>
-      <c r="BB3" s="86">
+      <c r="BB3" s="78">
         <v>22</v>
       </c>
-      <c r="BC3" s="86">
+      <c r="BC3" s="78">
         <v>23</v>
       </c>
-      <c r="BD3" s="86">
+      <c r="BD3" s="78">
         <v>24</v>
       </c>
-      <c r="BE3" s="86">
+      <c r="BE3" s="78">
         <v>25</v>
       </c>
-      <c r="BF3" s="86">
+      <c r="BF3" s="78">
         <v>28</v>
       </c>
-      <c r="BG3" s="86">
+      <c r="BG3" s="78">
         <v>29</v>
       </c>
-      <c r="BH3" s="86">
+      <c r="BH3" s="78">
         <v>30</v>
       </c>
-      <c r="BI3" s="86">
+      <c r="BI3" s="78">
         <v>31</v>
       </c>
-      <c r="BJ3" s="86">
+      <c r="BJ3" s="78">
         <v>1</v>
       </c>
-      <c r="BK3" s="86">
+      <c r="BK3" s="78">
         <v>4</v>
       </c>
-      <c r="BL3" s="86">
+      <c r="BL3" s="78">
         <v>5</v>
       </c>
-      <c r="BM3" s="86">
+      <c r="BM3" s="78">
         <v>6</v>
       </c>
-      <c r="BN3" s="86">
+      <c r="BN3" s="78">
         <v>7</v>
       </c>
-      <c r="BO3" s="86">
+      <c r="BO3" s="78">
         <v>8</v>
       </c>
-      <c r="BP3" s="86">
+      <c r="BP3" s="78">
         <v>11</v>
       </c>
-      <c r="BQ3" s="86">
+      <c r="BQ3" s="78">
         <v>12</v>
       </c>
-      <c r="BR3" s="86">
+      <c r="BR3" s="78">
         <v>13</v>
       </c>
-      <c r="BS3" s="86">
+      <c r="BS3" s="78">
         <v>14</v>
       </c>
-      <c r="BT3" s="98">
+      <c r="BT3" s="87">
         <v>15</v>
       </c>
-      <c r="BU3" s="86">
+      <c r="BU3" s="78">
         <v>18</v>
       </c>
-      <c r="BV3" s="86">
+      <c r="BV3" s="78">
         <v>19</v>
       </c>
-      <c r="BW3" s="98">
+      <c r="BW3" s="87">
         <v>20</v>
       </c>
-      <c r="BX3" s="86">
+      <c r="BX3" s="78">
         <v>21</v>
       </c>
-      <c r="BY3" s="86">
+      <c r="BY3" s="78">
         <v>22</v>
       </c>
-      <c r="BZ3" s="86">
+      <c r="BZ3" s="78">
         <v>25</v>
       </c>
-      <c r="CA3" s="86">
+      <c r="CA3" s="78">
         <v>26</v>
       </c>
-      <c r="CB3" s="86">
+      <c r="CB3" s="78">
         <v>27</v>
       </c>
-      <c r="CC3" s="86">
+      <c r="CC3" s="78">
         <v>28</v>
       </c>
-      <c r="CD3" s="86">
+      <c r="CD3" s="78">
         <v>29</v>
       </c>
-      <c r="CE3" s="86">
+      <c r="CE3" s="78">
         <v>2</v>
       </c>
-      <c r="CF3" s="86">
+      <c r="CF3" s="78">
         <v>3</v>
       </c>
-      <c r="CG3" s="86">
+      <c r="CG3" s="78">
         <v>4</v>
       </c>
-      <c r="CH3" s="86">
+      <c r="CH3" s="78">
         <v>5</v>
       </c>
-      <c r="CI3" s="86">
+      <c r="CI3" s="78">
         <v>6</v>
       </c>
-      <c r="CJ3" s="86">
+      <c r="CJ3" s="78">
         <v>9</v>
       </c>
-      <c r="CK3" s="86">
+      <c r="CK3" s="78">
         <v>10</v>
       </c>
-      <c r="CL3" s="86">
+      <c r="CL3" s="78">
         <v>11</v>
       </c>
-      <c r="CM3" s="86">
+      <c r="CM3" s="78">
         <v>12</v>
       </c>
-      <c r="CN3" s="86">
+      <c r="CN3" s="78">
         <v>13</v>
       </c>
-      <c r="CO3" s="98">
+      <c r="CO3" s="87">
         <v>14</v>
       </c>
-      <c r="CP3" s="86">
+      <c r="CP3" s="78">
         <v>16</v>
       </c>
-      <c r="CQ3" s="86">
+      <c r="CQ3" s="78">
         <v>17</v>
       </c>
-      <c r="CR3" s="86">
+      <c r="CR3" s="78">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:96" s="91" customFormat="1" ht="13.2" customHeight="1">
-      <c r="A4" s="90" t="s">
+    <row r="4" spans="1:96" s="81" customFormat="1" ht="13.2" customHeight="1">
+      <c r="A4" s="80" t="s">
         <v>102</v>
       </c>
-      <c r="C4" s="89"/>
-      <c r="D4" s="92"/>
-      <c r="E4" s="92"/>
-      <c r="F4" s="92"/>
-      <c r="G4" s="92"/>
-      <c r="H4" s="92"/>
-      <c r="I4" s="92"/>
-      <c r="J4" s="92"/>
-      <c r="K4" s="92"/>
-      <c r="L4" s="92"/>
-      <c r="M4" s="92"/>
-      <c r="N4" s="92"/>
-      <c r="O4" s="92"/>
-      <c r="P4" s="92"/>
-      <c r="Q4" s="92"/>
-      <c r="AV4" s="97" t="s">
+      <c r="C4" s="79"/>
+      <c r="D4" s="82"/>
+      <c r="E4" s="82"/>
+      <c r="F4" s="82"/>
+      <c r="G4" s="82"/>
+      <c r="H4" s="82"/>
+      <c r="I4" s="82"/>
+      <c r="J4" s="82"/>
+      <c r="K4" s="82"/>
+      <c r="L4" s="82"/>
+      <c r="M4" s="82"/>
+      <c r="N4" s="82"/>
+      <c r="O4" s="82"/>
+      <c r="P4" s="82"/>
+      <c r="Q4" s="82"/>
+      <c r="AV4" s="99" t="s">
         <v>116</v>
       </c>
-      <c r="AW4" s="97" t="s">
+      <c r="AW4" s="99" t="s">
         <v>116</v>
       </c>
-      <c r="BT4" s="97" t="s">
+      <c r="BT4" s="99" t="s">
         <v>115</v>
       </c>
-      <c r="BW4" s="97" t="s">
+      <c r="BW4" s="99" t="s">
         <v>117</v>
       </c>
-      <c r="CO4" s="97" t="s">
+      <c r="CO4" s="99" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="5" spans="1:96" s="91" customFormat="1">
-      <c r="A5" s="90" t="s">
+    <row r="5" spans="1:96" s="81" customFormat="1">
+      <c r="A5" s="80" t="s">
         <v>106</v>
       </c>
-      <c r="C5" s="92"/>
-      <c r="D5" s="92"/>
-      <c r="E5" s="92"/>
-      <c r="F5" s="92"/>
-      <c r="G5" s="92"/>
-      <c r="H5" s="92"/>
-      <c r="I5" s="92"/>
-      <c r="J5" s="92"/>
-      <c r="K5" s="92"/>
-      <c r="L5" s="92"/>
-      <c r="M5" s="92"/>
-      <c r="N5" s="92"/>
-      <c r="O5" s="92"/>
-      <c r="P5" s="92"/>
-      <c r="Q5" s="92"/>
-      <c r="AV5" s="97"/>
-      <c r="AW5" s="97"/>
-      <c r="BT5" s="97"/>
-      <c r="BW5" s="97"/>
-      <c r="CO5" s="97"/>
-    </row>
-    <row r="6" spans="1:96" s="91" customFormat="1">
-      <c r="A6" s="90" t="s">
+      <c r="C5" s="82"/>
+      <c r="D5" s="82"/>
+      <c r="E5" s="82"/>
+      <c r="F5" s="82"/>
+      <c r="G5" s="82"/>
+      <c r="H5" s="82"/>
+      <c r="I5" s="82"/>
+      <c r="J5" s="82"/>
+      <c r="K5" s="82"/>
+      <c r="L5" s="82"/>
+      <c r="M5" s="82"/>
+      <c r="N5" s="82"/>
+      <c r="O5" s="82"/>
+      <c r="P5" s="82"/>
+      <c r="Q5" s="82"/>
+      <c r="AV5" s="99"/>
+      <c r="AW5" s="99"/>
+      <c r="BT5" s="99"/>
+      <c r="BW5" s="99"/>
+      <c r="CO5" s="99"/>
+    </row>
+    <row r="6" spans="1:96" s="81" customFormat="1">
+      <c r="A6" s="80" t="s">
         <v>107</v>
       </c>
-      <c r="C6" s="92"/>
-      <c r="D6" s="92"/>
-      <c r="E6" s="92"/>
-      <c r="F6" s="92"/>
-      <c r="G6" s="92"/>
-      <c r="H6" s="92"/>
-      <c r="I6" s="92"/>
-      <c r="J6" s="92"/>
-      <c r="K6" s="92"/>
-      <c r="L6" s="92"/>
-      <c r="M6" s="92"/>
-      <c r="N6" s="92"/>
-      <c r="O6" s="92"/>
-      <c r="P6" s="92"/>
-      <c r="Q6" s="92"/>
-      <c r="AV6" s="97"/>
-      <c r="AW6" s="97"/>
-      <c r="BT6" s="97"/>
-      <c r="BW6" s="97"/>
-      <c r="CO6" s="97"/>
-    </row>
-    <row r="7" spans="1:96" s="91" customFormat="1">
-      <c r="A7" s="90" t="s">
+      <c r="C6" s="82"/>
+      <c r="D6" s="82"/>
+      <c r="E6" s="82"/>
+      <c r="F6" s="82"/>
+      <c r="G6" s="82"/>
+      <c r="H6" s="82"/>
+      <c r="I6" s="82"/>
+      <c r="J6" s="82"/>
+      <c r="K6" s="82"/>
+      <c r="L6" s="82"/>
+      <c r="M6" s="82"/>
+      <c r="N6" s="82"/>
+      <c r="O6" s="82"/>
+      <c r="P6" s="82"/>
+      <c r="Q6" s="82"/>
+      <c r="AV6" s="99"/>
+      <c r="AW6" s="99"/>
+      <c r="BT6" s="99"/>
+      <c r="BW6" s="99"/>
+      <c r="CO6" s="99"/>
+    </row>
+    <row r="7" spans="1:96" s="81" customFormat="1">
+      <c r="A7" s="80" t="s">
         <v>108</v>
       </c>
-      <c r="C7" s="92"/>
-      <c r="D7" s="92"/>
-      <c r="E7" s="92"/>
-      <c r="F7" s="92"/>
-      <c r="G7" s="92"/>
-      <c r="H7" s="92"/>
-      <c r="I7" s="92"/>
-      <c r="J7" s="92"/>
-      <c r="K7" s="92"/>
-      <c r="L7" s="92"/>
-      <c r="M7" s="92"/>
-      <c r="N7" s="92"/>
-      <c r="O7" s="92"/>
-      <c r="P7" s="92"/>
-      <c r="Q7" s="92"/>
-      <c r="AV7" s="97"/>
-      <c r="AW7" s="97"/>
-      <c r="BT7" s="97"/>
-      <c r="BW7" s="97"/>
-      <c r="CO7" s="97"/>
+      <c r="C7" s="82"/>
+      <c r="D7" s="82"/>
+      <c r="E7" s="82"/>
+      <c r="F7" s="82"/>
+      <c r="G7" s="82"/>
+      <c r="H7" s="82"/>
+      <c r="I7" s="82"/>
+      <c r="J7" s="82"/>
+      <c r="K7" s="82"/>
+      <c r="L7" s="82"/>
+      <c r="M7" s="82"/>
+      <c r="N7" s="82"/>
+      <c r="O7" s="82"/>
+      <c r="P7" s="82"/>
+      <c r="Q7" s="82"/>
+      <c r="AV7" s="99"/>
+      <c r="AW7" s="99"/>
+      <c r="BT7" s="99"/>
+      <c r="BW7" s="99"/>
+      <c r="CO7" s="99"/>
     </row>
     <row r="8" spans="1:96">
-      <c r="AV8" s="97"/>
-      <c r="AW8" s="97"/>
-      <c r="BT8" s="97"/>
-      <c r="BW8" s="97"/>
-      <c r="CO8" s="97"/>
+      <c r="AV8" s="99"/>
+      <c r="AW8" s="99"/>
+      <c r="BT8" s="99"/>
+      <c r="BW8" s="99"/>
+      <c r="CO8" s="99"/>
     </row>
     <row r="9" spans="1:96">
-      <c r="AV9" s="97"/>
-      <c r="AW9" s="97"/>
-      <c r="BT9" s="97"/>
-      <c r="BW9" s="97"/>
-      <c r="CO9" s="97"/>
+      <c r="AV9" s="99"/>
+      <c r="AW9" s="99"/>
+      <c r="BT9" s="99"/>
+      <c r="BW9" s="99"/>
+      <c r="CO9" s="99"/>
     </row>
     <row r="10" spans="1:96">
-      <c r="AV10" s="97"/>
-      <c r="AW10" s="97"/>
-      <c r="BT10" s="97"/>
-      <c r="BW10" s="97"/>
-      <c r="CO10" s="97"/>
+      <c r="AV10" s="99"/>
+      <c r="AW10" s="99"/>
+      <c r="BT10" s="99"/>
+      <c r="BW10" s="99"/>
+      <c r="CO10" s="99"/>
     </row>
     <row r="11" spans="1:96">
-      <c r="AV11" s="97"/>
-      <c r="AW11" s="97"/>
-      <c r="BT11" s="97"/>
-      <c r="BW11" s="97"/>
-      <c r="CO11" s="97"/>
+      <c r="AV11" s="99"/>
+      <c r="AW11" s="99"/>
+      <c r="BT11" s="99"/>
+      <c r="BW11" s="99"/>
+      <c r="CO11" s="99"/>
     </row>
     <row r="12" spans="1:96">
-      <c r="AV12" s="97"/>
-      <c r="AW12" s="97"/>
-      <c r="BT12" s="97"/>
-      <c r="BW12" s="97"/>
-      <c r="CO12" s="97"/>
+      <c r="AV12" s="99"/>
+      <c r="AW12" s="99"/>
+      <c r="BT12" s="99"/>
+      <c r="BW12" s="99"/>
+      <c r="CO12" s="99"/>
     </row>
     <row r="13" spans="1:96">
-      <c r="AV13" s="97"/>
-      <c r="AW13" s="97"/>
-      <c r="BT13" s="97"/>
-      <c r="BW13" s="97"/>
-      <c r="CO13" s="97"/>
+      <c r="AV13" s="99"/>
+      <c r="AW13" s="99"/>
+      <c r="BT13" s="99"/>
+      <c r="BW13" s="99"/>
+      <c r="CO13" s="99"/>
     </row>
     <row r="14" spans="1:96">
-      <c r="AV14" s="97"/>
-      <c r="AW14" s="97"/>
-      <c r="BT14" s="97"/>
-      <c r="BW14" s="97"/>
-      <c r="CO14" s="97"/>
+      <c r="AV14" s="99"/>
+      <c r="AW14" s="99"/>
+      <c r="BT14" s="99"/>
+      <c r="BW14" s="99"/>
+      <c r="CO14" s="99"/>
     </row>
     <row r="15" spans="1:96">
-      <c r="AV15" s="97"/>
-      <c r="AW15" s="97"/>
-      <c r="BT15" s="97"/>
-      <c r="BW15" s="97"/>
-      <c r="CO15" s="97"/>
+      <c r="AV15" s="99"/>
+      <c r="AW15" s="99"/>
+      <c r="BT15" s="99"/>
+      <c r="BW15" s="99"/>
+      <c r="CO15" s="99"/>
     </row>
     <row r="16" spans="1:96">
-      <c r="AV16" s="97"/>
-      <c r="AW16" s="97"/>
-      <c r="BT16" s="97"/>
-      <c r="BW16" s="97"/>
-      <c r="CO16" s="97"/>
+      <c r="AV16" s="99"/>
+      <c r="AW16" s="99"/>
+      <c r="BT16" s="99"/>
+      <c r="BW16" s="99"/>
+      <c r="CO16" s="99"/>
     </row>
     <row r="17" spans="48:93">
-      <c r="AV17" s="97"/>
-      <c r="AW17" s="97"/>
-      <c r="BT17" s="97"/>
-      <c r="BW17" s="97"/>
-      <c r="CO17" s="97"/>
+      <c r="AV17" s="99"/>
+      <c r="AW17" s="99"/>
+      <c r="BT17" s="99"/>
+      <c r="BW17" s="99"/>
+      <c r="CO17" s="99"/>
     </row>
     <row r="18" spans="48:93">
-      <c r="AV18" s="97"/>
-      <c r="AW18" s="97"/>
-      <c r="BT18" s="97"/>
-      <c r="BW18" s="97"/>
-      <c r="CO18" s="97"/>
+      <c r="AV18" s="99"/>
+      <c r="AW18" s="99"/>
+      <c r="BT18" s="99"/>
+      <c r="BW18" s="99"/>
+      <c r="CO18" s="99"/>
     </row>
     <row r="19" spans="48:93">
-      <c r="AV19" s="97"/>
-      <c r="AW19" s="97"/>
-      <c r="BT19" s="97"/>
-      <c r="BW19" s="97"/>
-      <c r="CO19" s="97"/>
+      <c r="AV19" s="99"/>
+      <c r="AW19" s="99"/>
+      <c r="BT19" s="99"/>
+      <c r="BW19" s="99"/>
+      <c r="CO19" s="99"/>
     </row>
     <row r="20" spans="48:93">
-      <c r="AV20" s="97"/>
-      <c r="AW20" s="97"/>
-      <c r="BT20" s="97"/>
-      <c r="BW20" s="97"/>
-      <c r="CO20" s="97"/>
+      <c r="AV20" s="99"/>
+      <c r="AW20" s="99"/>
+      <c r="BT20" s="99"/>
+      <c r="BW20" s="99"/>
+      <c r="CO20" s="99"/>
     </row>
     <row r="21" spans="48:93">
-      <c r="AV21" s="97"/>
-      <c r="AW21" s="97"/>
-      <c r="BT21" s="97"/>
-      <c r="BW21" s="97"/>
-      <c r="CO21" s="97"/>
+      <c r="AV21" s="99"/>
+      <c r="AW21" s="99"/>
+      <c r="BT21" s="99"/>
+      <c r="BW21" s="99"/>
+      <c r="CO21" s="99"/>
     </row>
     <row r="22" spans="48:93">
-      <c r="AV22" s="97"/>
-      <c r="AW22" s="97"/>
-      <c r="BT22" s="97"/>
-      <c r="BW22" s="97"/>
-      <c r="CO22" s="97"/>
+      <c r="AV22" s="99"/>
+      <c r="AW22" s="99"/>
+      <c r="BT22" s="99"/>
+      <c r="BW22" s="99"/>
+      <c r="CO22" s="99"/>
     </row>
     <row r="23" spans="48:93">
-      <c r="AV23" s="97"/>
-      <c r="AW23" s="97"/>
-      <c r="BT23" s="97"/>
-      <c r="BW23" s="97"/>
-      <c r="CO23" s="97"/>
+      <c r="AV23" s="99"/>
+      <c r="AW23" s="99"/>
+      <c r="BT23" s="99"/>
+      <c r="BW23" s="99"/>
+      <c r="CO23" s="99"/>
     </row>
     <row r="24" spans="48:93">
-      <c r="AV24" s="97"/>
-      <c r="AW24" s="97"/>
-      <c r="BT24" s="97"/>
-      <c r="BW24" s="97"/>
-      <c r="CO24" s="97"/>
+      <c r="AV24" s="99"/>
+      <c r="AW24" s="99"/>
+      <c r="BT24" s="99"/>
+      <c r="BW24" s="99"/>
+      <c r="CO24" s="99"/>
     </row>
     <row r="25" spans="48:93">
-      <c r="AV25" s="97"/>
-      <c r="AW25" s="97"/>
-      <c r="BT25" s="97"/>
-      <c r="BW25" s="97"/>
-      <c r="CO25" s="97"/>
+      <c r="AV25" s="99"/>
+      <c r="AW25" s="99"/>
+      <c r="BT25" s="99"/>
+      <c r="BW25" s="99"/>
+      <c r="CO25" s="99"/>
     </row>
     <row r="26" spans="48:93">
-      <c r="AV26" s="97"/>
-      <c r="AW26" s="97"/>
-      <c r="BT26" s="97"/>
-      <c r="BW26" s="97"/>
-      <c r="CO26" s="97"/>
+      <c r="AV26" s="99"/>
+      <c r="AW26" s="99"/>
+      <c r="BT26" s="99"/>
+      <c r="BW26" s="99"/>
+      <c r="CO26" s="99"/>
     </row>
     <row r="27" spans="48:93">
-      <c r="AV27" s="97"/>
-      <c r="AW27" s="97"/>
-      <c r="BT27" s="97"/>
-      <c r="BW27" s="97"/>
-      <c r="CO27" s="97"/>
+      <c r="AV27" s="99"/>
+      <c r="AW27" s="99"/>
+      <c r="BT27" s="99"/>
+      <c r="BW27" s="99"/>
+      <c r="CO27" s="99"/>
     </row>
     <row r="28" spans="48:93">
-      <c r="AV28" s="96"/>
+      <c r="AV28" s="86"/>
     </row>
     <row r="29" spans="48:93">
-      <c r="AV29" s="96"/>
+      <c r="AV29" s="86"/>
     </row>
     <row r="30" spans="48:93">
-      <c r="AV30" s="96"/>
+      <c r="AV30" s="86"/>
     </row>
     <row r="31" spans="48:93">
-      <c r="AV31" s="96"/>
+      <c r="AV31" s="86"/>
     </row>
     <row r="32" spans="48:93">
-      <c r="AV32" s="96"/>
+      <c r="AV32" s="86"/>
     </row>
     <row r="33" spans="48:48">
-      <c r="AV33" s="96"/>
+      <c r="AV33" s="86"/>
     </row>
     <row r="34" spans="48:48">
-      <c r="AV34" s="96"/>
+      <c r="AV34" s="86"/>
     </row>
     <row r="35" spans="48:48">
-      <c r="AV35" s="96"/>
+      <c r="AV35" s="86"/>
     </row>
     <row r="36" spans="48:48">
-      <c r="AV36" s="96"/>
+      <c r="AV36" s="86"/>
     </row>
     <row r="37" spans="48:48">
-      <c r="AV37" s="96"/>
+      <c r="AV37" s="86"/>
     </row>
     <row r="38" spans="48:48">
-      <c r="AV38" s="96"/>
+      <c r="AV38" s="86"/>
     </row>
     <row r="39" spans="48:48">
-      <c r="AV39" s="96"/>
+      <c r="AV39" s="86"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -7974,12 +7974,12 @@
     <mergeCell ref="BW4:BW27"/>
     <mergeCell ref="CO4:CO27"/>
     <mergeCell ref="AV4:AV27"/>
+    <mergeCell ref="CE2:CR2"/>
     <mergeCell ref="C2:Q2"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="R2:AL2"/>
     <mergeCell ref="AM2:BI2"/>
     <mergeCell ref="BJ2:CD2"/>
-    <mergeCell ref="CE2:CR2"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Melhora estilização das planilhas e adiciona membros dos grupos do técnico
</commit_message>
<xml_diff>
--- a/Cronograma/Projeto-Cronograma - Acompanhamento.xlsx
+++ b/Cronograma/Projeto-Cronograma - Acompanhamento.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\39893838843\Downloads\2s2019-t3-mentoria\Cronograma\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Works\Cursos\senai_desenvolvimento\2s2019\2s2019-t3-mentoria\Cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E716B7FC-D120-4FDB-8BFE-15D7E59247EB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Proj-Cronograma" sheetId="1" r:id="rId1"/>
@@ -24,6 +25,86 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Saulo Santos</author>
+  </authors>
+  <commentList>
+    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{B823D240-44A1-4AA8-AD85-B98BE0488E33}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>Gabriel
+Guilherme
+Luana
+Ricardo Paulo</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{EFDCB323-A12C-4FE4-999F-BA8C5695F98E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>Davi
+Murilo
+Renato
+Ricardo Ribeiro</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{37BAB12C-F1E4-410F-9AC0-AAB1C84CED66}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>Artur
+Bárbara
+Carlos
+Cristian
+Jefferson</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{79CF17A7-FE5A-4F77-8A3A-117B42495EE1}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>Franklin
+Gabriela
+Kevin
+Leonardo
+Lucas</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="128">
   <si>
@@ -372,9 +453,6 @@
     <t>Consciência Negra</t>
   </si>
   <si>
-    <t>Apresentação</t>
-  </si>
-  <si>
     <t>BlockTime</t>
   </si>
   <si>
@@ -409,13 +487,16 @@
   </si>
   <si>
     <t>Apresentação do entendimento do escopo, construção do cronograma no Azure DevOps e levantamento de questões para a empresa</t>
+  </si>
+  <si>
+    <t>Apresentação dos Projetos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="14" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -491,20 +572,53 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="27">
+  <fills count="28">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -661,8 +775,14 @@
         <bgColor rgb="FF993366"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF5B2484"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -670,11 +790,89 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -879,9 +1077,6 @@
     <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -890,6 +1085,9 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -912,17 +1110,38 @@
     <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1305,7 +1524,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMK942"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -7115,11 +7334,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:CR39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="CF5" sqref="CF5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -7136,538 +7355,538 @@
     <col min="73" max="74" width="5.77734375" customWidth="1"/>
     <col min="75" max="75" width="3.77734375" style="80" customWidth="1"/>
     <col min="76" max="92" width="5.77734375" customWidth="1"/>
-    <col min="93" max="93" width="5.77734375" style="81" customWidth="1"/>
+    <col min="93" max="93" width="3.77734375" style="81" customWidth="1"/>
     <col min="94" max="96" width="5.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A1" s="95" t="s">
+      <c r="A1" s="97" t="s">
         <v>102</v>
       </c>
-      <c r="B1" s="78" t="s">
+      <c r="B1" s="96" t="s">
         <v>103</v>
       </c>
-      <c r="C1" s="78">
+      <c r="C1" s="100">
         <v>14</v>
       </c>
-      <c r="D1" s="78">
+      <c r="D1" s="100">
         <v>15</v>
       </c>
-      <c r="E1" s="78">
+      <c r="E1" s="100">
         <v>16</v>
       </c>
-      <c r="F1" s="78">
+      <c r="F1" s="100">
         <v>17</v>
       </c>
-      <c r="G1" s="78">
+      <c r="G1" s="100">
         <v>18</v>
       </c>
-      <c r="H1" s="78">
+      <c r="H1" s="100">
         <v>19</v>
       </c>
-      <c r="I1" s="78">
+      <c r="I1" s="100">
         <v>20</v>
       </c>
-      <c r="J1" s="78">
+      <c r="J1" s="100">
         <v>21</v>
       </c>
-      <c r="K1" s="78">
+      <c r="K1" s="100">
         <v>22</v>
       </c>
-      <c r="L1" s="78">
+      <c r="L1" s="100">
         <v>23</v>
       </c>
-      <c r="M1" s="78">
+      <c r="M1" s="100">
         <v>24</v>
       </c>
-      <c r="N1" s="78">
+      <c r="N1" s="100">
         <v>25</v>
       </c>
-      <c r="O1" s="78">
+      <c r="O1" s="100">
         <v>26</v>
       </c>
-      <c r="P1" s="78">
+      <c r="P1" s="100">
         <v>27</v>
       </c>
-      <c r="Q1" s="78">
+      <c r="Q1" s="100">
         <v>28</v>
       </c>
-      <c r="R1" s="78">
+      <c r="R1" s="100">
         <v>29</v>
       </c>
-      <c r="S1" s="78">
+      <c r="S1" s="100">
         <v>30</v>
       </c>
-      <c r="T1" s="78">
+      <c r="T1" s="100">
         <v>31</v>
       </c>
-      <c r="U1" s="78">
+      <c r="U1" s="100">
         <v>32</v>
       </c>
-      <c r="V1" s="78">
+      <c r="V1" s="100">
         <v>33</v>
       </c>
-      <c r="W1" s="78">
+      <c r="W1" s="100">
         <v>34</v>
       </c>
-      <c r="X1" s="78">
+      <c r="X1" s="100">
         <v>35</v>
       </c>
-      <c r="Y1" s="78">
+      <c r="Y1" s="100">
         <v>36</v>
       </c>
-      <c r="Z1" s="78">
+      <c r="Z1" s="100">
         <v>37</v>
       </c>
-      <c r="AA1" s="78">
+      <c r="AA1" s="100">
         <v>38</v>
       </c>
-      <c r="AB1" s="78">
+      <c r="AB1" s="100">
         <v>39</v>
       </c>
-      <c r="AC1" s="78">
+      <c r="AC1" s="100">
         <v>40</v>
       </c>
-      <c r="AD1" s="78">
+      <c r="AD1" s="100">
         <v>41</v>
       </c>
-      <c r="AE1" s="78">
+      <c r="AE1" s="100">
         <v>42</v>
       </c>
-      <c r="AF1" s="78">
+      <c r="AF1" s="100">
         <v>43</v>
       </c>
-      <c r="AG1" s="78">
+      <c r="AG1" s="100">
         <v>44</v>
       </c>
-      <c r="AH1" s="78">
+      <c r="AH1" s="100">
         <v>45</v>
       </c>
-      <c r="AI1" s="78">
+      <c r="AI1" s="100">
         <v>46</v>
       </c>
-      <c r="AJ1" s="78">
+      <c r="AJ1" s="100">
         <v>47</v>
       </c>
-      <c r="AK1" s="78">
+      <c r="AK1" s="100">
         <v>48</v>
       </c>
-      <c r="AL1" s="78">
+      <c r="AL1" s="100">
         <v>49</v>
       </c>
-      <c r="AM1" s="78">
+      <c r="AM1" s="100">
         <v>50</v>
       </c>
-      <c r="AN1" s="78">
+      <c r="AN1" s="100">
         <v>51</v>
       </c>
-      <c r="AO1" s="78">
+      <c r="AO1" s="100">
         <v>52</v>
       </c>
-      <c r="AP1" s="78">
+      <c r="AP1" s="100">
         <v>53</v>
       </c>
-      <c r="AQ1" s="78">
+      <c r="AQ1" s="100">
         <v>54</v>
       </c>
-      <c r="AR1" s="78">
+      <c r="AR1" s="100">
         <v>55</v>
       </c>
-      <c r="AS1" s="78">
+      <c r="AS1" s="100">
         <v>56</v>
       </c>
-      <c r="AT1" s="78">
+      <c r="AT1" s="100">
         <v>57</v>
       </c>
-      <c r="AU1" s="78">
+      <c r="AU1" s="100">
         <v>58</v>
       </c>
       <c r="AV1" s="82"/>
       <c r="AW1" s="82"/>
-      <c r="AX1" s="78">
+      <c r="AX1" s="100">
         <v>59</v>
       </c>
-      <c r="AY1" s="78">
+      <c r="AY1" s="100">
         <v>60</v>
       </c>
-      <c r="AZ1" s="78">
+      <c r="AZ1" s="100">
         <v>61</v>
       </c>
-      <c r="BA1" s="78">
+      <c r="BA1" s="100">
         <v>62</v>
       </c>
-      <c r="BB1" s="78">
+      <c r="BB1" s="100">
         <v>63</v>
       </c>
-      <c r="BC1" s="78">
+      <c r="BC1" s="100">
         <v>64</v>
       </c>
-      <c r="BD1" s="78">
+      <c r="BD1" s="100">
         <v>65</v>
       </c>
-      <c r="BE1" s="78">
+      <c r="BE1" s="100">
         <v>66</v>
       </c>
-      <c r="BF1" s="78">
+      <c r="BF1" s="100">
         <v>67</v>
       </c>
-      <c r="BG1" s="78">
+      <c r="BG1" s="100">
         <v>68</v>
       </c>
-      <c r="BH1" s="78">
+      <c r="BH1" s="100">
         <v>69</v>
       </c>
-      <c r="BI1" s="78">
+      <c r="BI1" s="100">
         <v>70</v>
       </c>
-      <c r="BJ1" s="78">
+      <c r="BJ1" s="100">
         <v>71</v>
       </c>
-      <c r="BK1" s="78">
+      <c r="BK1" s="100">
         <v>72</v>
       </c>
-      <c r="BL1" s="78">
+      <c r="BL1" s="100">
         <v>73</v>
       </c>
-      <c r="BM1" s="78">
+      <c r="BM1" s="100">
         <v>74</v>
       </c>
-      <c r="BN1" s="78">
+      <c r="BN1" s="100">
         <v>75</v>
       </c>
-      <c r="BO1" s="78">
+      <c r="BO1" s="100">
         <v>76</v>
       </c>
-      <c r="BP1" s="78">
+      <c r="BP1" s="100">
         <v>77</v>
       </c>
-      <c r="BQ1" s="78">
+      <c r="BQ1" s="100">
         <v>78</v>
       </c>
-      <c r="BR1" s="78">
+      <c r="BR1" s="100">
         <v>79</v>
       </c>
-      <c r="BS1" s="78">
+      <c r="BS1" s="100">
         <v>80</v>
       </c>
       <c r="BT1" s="82"/>
-      <c r="BU1" s="78">
+      <c r="BU1" s="100">
         <v>81</v>
       </c>
-      <c r="BV1" s="78">
+      <c r="BV1" s="100">
         <v>82</v>
       </c>
       <c r="BW1" s="82"/>
-      <c r="BX1" s="78">
+      <c r="BX1" s="100">
         <v>83</v>
       </c>
-      <c r="BY1" s="78">
+      <c r="BY1" s="100">
         <v>84</v>
       </c>
-      <c r="BZ1" s="78">
+      <c r="BZ1" s="100">
         <v>85</v>
       </c>
-      <c r="CA1" s="78">
+      <c r="CA1" s="100">
         <v>86</v>
       </c>
-      <c r="CB1" s="78">
+      <c r="CB1" s="100">
         <v>87</v>
       </c>
-      <c r="CC1" s="78">
+      <c r="CC1" s="100">
         <v>88</v>
       </c>
-      <c r="CD1" s="78">
+      <c r="CD1" s="100">
         <v>89</v>
       </c>
-      <c r="CE1" s="78">
+      <c r="CE1" s="100">
         <v>90</v>
       </c>
-      <c r="CF1" s="78">
+      <c r="CF1" s="100">
         <v>91</v>
       </c>
-      <c r="CG1" s="78">
+      <c r="CG1" s="100">
         <v>92</v>
       </c>
-      <c r="CH1" s="78">
+      <c r="CH1" s="100">
         <v>93</v>
       </c>
-      <c r="CI1" s="78">
+      <c r="CI1" s="100">
         <v>94</v>
       </c>
-      <c r="CJ1" s="78">
+      <c r="CJ1" s="100">
         <v>95</v>
       </c>
-      <c r="CK1" s="78">
+      <c r="CK1" s="100">
         <v>96</v>
       </c>
-      <c r="CL1" s="78">
+      <c r="CL1" s="100">
         <v>97</v>
       </c>
-      <c r="CM1" s="78">
+      <c r="CM1" s="100">
         <v>98</v>
       </c>
-      <c r="CN1" s="78">
+      <c r="CN1" s="100">
         <v>99</v>
       </c>
       <c r="CO1" s="83"/>
-      <c r="CP1" s="78">
+      <c r="CP1" s="100">
         <v>100</v>
       </c>
-      <c r="CQ1" s="78">
+      <c r="CQ1" s="100">
         <v>101</v>
       </c>
-      <c r="CR1" s="78">
+      <c r="CR1" s="100">
         <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:96" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="95"/>
-      <c r="B2" s="78" t="s">
+      <c r="A2" s="98"/>
+      <c r="B2" s="96" t="s">
         <v>104</v>
       </c>
-      <c r="C2" s="97" t="s">
+      <c r="C2" s="101" t="s">
         <v>105</v>
       </c>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="97"/>
-      <c r="K2" s="97"/>
-      <c r="L2" s="97"/>
-      <c r="M2" s="97"/>
-      <c r="N2" s="97"/>
-      <c r="O2" s="97"/>
-      <c r="P2" s="97"/>
-      <c r="Q2" s="97"/>
-      <c r="R2" s="95" t="s">
+      <c r="D2" s="101"/>
+      <c r="E2" s="101"/>
+      <c r="F2" s="101"/>
+      <c r="G2" s="101"/>
+      <c r="H2" s="101"/>
+      <c r="I2" s="101"/>
+      <c r="J2" s="101"/>
+      <c r="K2" s="101"/>
+      <c r="L2" s="101"/>
+      <c r="M2" s="101"/>
+      <c r="N2" s="101"/>
+      <c r="O2" s="101"/>
+      <c r="P2" s="101"/>
+      <c r="Q2" s="101"/>
+      <c r="R2" s="101" t="s">
         <v>106</v>
       </c>
-      <c r="S2" s="95"/>
-      <c r="T2" s="95"/>
-      <c r="U2" s="95"/>
-      <c r="V2" s="95"/>
-      <c r="W2" s="95"/>
-      <c r="X2" s="95"/>
-      <c r="Y2" s="95"/>
-      <c r="Z2" s="95"/>
-      <c r="AA2" s="95"/>
-      <c r="AB2" s="95"/>
-      <c r="AC2" s="95"/>
-      <c r="AD2" s="95"/>
-      <c r="AE2" s="95"/>
-      <c r="AF2" s="95"/>
-      <c r="AG2" s="95"/>
-      <c r="AH2" s="95"/>
-      <c r="AI2" s="95"/>
-      <c r="AJ2" s="95"/>
-      <c r="AK2" s="95"/>
-      <c r="AL2" s="95"/>
-      <c r="AM2" s="95" t="s">
+      <c r="S2" s="101"/>
+      <c r="T2" s="101"/>
+      <c r="U2" s="101"/>
+      <c r="V2" s="101"/>
+      <c r="W2" s="101"/>
+      <c r="X2" s="101"/>
+      <c r="Y2" s="101"/>
+      <c r="Z2" s="101"/>
+      <c r="AA2" s="101"/>
+      <c r="AB2" s="101"/>
+      <c r="AC2" s="101"/>
+      <c r="AD2" s="101"/>
+      <c r="AE2" s="101"/>
+      <c r="AF2" s="101"/>
+      <c r="AG2" s="101"/>
+      <c r="AH2" s="101"/>
+      <c r="AI2" s="101"/>
+      <c r="AJ2" s="101"/>
+      <c r="AK2" s="101"/>
+      <c r="AL2" s="101"/>
+      <c r="AM2" s="101" t="s">
         <v>107</v>
       </c>
-      <c r="AN2" s="95"/>
-      <c r="AO2" s="95"/>
-      <c r="AP2" s="95"/>
-      <c r="AQ2" s="95"/>
-      <c r="AR2" s="95"/>
-      <c r="AS2" s="95"/>
-      <c r="AT2" s="95"/>
-      <c r="AU2" s="95"/>
-      <c r="AV2" s="95"/>
-      <c r="AW2" s="95"/>
-      <c r="AX2" s="95"/>
-      <c r="AY2" s="95"/>
-      <c r="AZ2" s="95"/>
-      <c r="BA2" s="95"/>
-      <c r="BB2" s="95"/>
-      <c r="BC2" s="95"/>
-      <c r="BD2" s="95"/>
-      <c r="BE2" s="95"/>
-      <c r="BF2" s="95"/>
-      <c r="BG2" s="95"/>
-      <c r="BH2" s="95"/>
-      <c r="BI2" s="95"/>
-      <c r="BJ2" s="95" t="s">
+      <c r="AN2" s="101"/>
+      <c r="AO2" s="101"/>
+      <c r="AP2" s="101"/>
+      <c r="AQ2" s="101"/>
+      <c r="AR2" s="101"/>
+      <c r="AS2" s="101"/>
+      <c r="AT2" s="101"/>
+      <c r="AU2" s="101"/>
+      <c r="AV2" s="101"/>
+      <c r="AW2" s="101"/>
+      <c r="AX2" s="101"/>
+      <c r="AY2" s="101"/>
+      <c r="AZ2" s="101"/>
+      <c r="BA2" s="101"/>
+      <c r="BB2" s="101"/>
+      <c r="BC2" s="101"/>
+      <c r="BD2" s="101"/>
+      <c r="BE2" s="101"/>
+      <c r="BF2" s="101"/>
+      <c r="BG2" s="101"/>
+      <c r="BH2" s="101"/>
+      <c r="BI2" s="101"/>
+      <c r="BJ2" s="101" t="s">
         <v>108</v>
       </c>
-      <c r="BK2" s="95"/>
-      <c r="BL2" s="95"/>
-      <c r="BM2" s="95"/>
-      <c r="BN2" s="95"/>
-      <c r="BO2" s="95"/>
-      <c r="BP2" s="95"/>
-      <c r="BQ2" s="95"/>
-      <c r="BR2" s="95"/>
-      <c r="BS2" s="95"/>
-      <c r="BT2" s="95"/>
-      <c r="BU2" s="95"/>
-      <c r="BV2" s="95"/>
-      <c r="BW2" s="95"/>
-      <c r="BX2" s="95"/>
-      <c r="BY2" s="95"/>
-      <c r="BZ2" s="95"/>
-      <c r="CA2" s="95"/>
-      <c r="CB2" s="95"/>
-      <c r="CC2" s="95"/>
-      <c r="CD2" s="95"/>
-      <c r="CE2" s="95" t="s">
+      <c r="BK2" s="101"/>
+      <c r="BL2" s="101"/>
+      <c r="BM2" s="101"/>
+      <c r="BN2" s="101"/>
+      <c r="BO2" s="101"/>
+      <c r="BP2" s="101"/>
+      <c r="BQ2" s="101"/>
+      <c r="BR2" s="101"/>
+      <c r="BS2" s="101"/>
+      <c r="BT2" s="101"/>
+      <c r="BU2" s="101"/>
+      <c r="BV2" s="101"/>
+      <c r="BW2" s="101"/>
+      <c r="BX2" s="101"/>
+      <c r="BY2" s="101"/>
+      <c r="BZ2" s="101"/>
+      <c r="CA2" s="101"/>
+      <c r="CB2" s="101"/>
+      <c r="CC2" s="101"/>
+      <c r="CD2" s="101"/>
+      <c r="CE2" s="101" t="s">
         <v>109</v>
       </c>
-      <c r="CF2" s="95"/>
-      <c r="CG2" s="95"/>
-      <c r="CH2" s="95"/>
-      <c r="CI2" s="95"/>
-      <c r="CJ2" s="95"/>
-      <c r="CK2" s="95"/>
-      <c r="CL2" s="95"/>
-      <c r="CM2" s="95"/>
-      <c r="CN2" s="95"/>
-      <c r="CO2" s="95"/>
-      <c r="CP2" s="95"/>
-      <c r="CQ2" s="95"/>
-      <c r="CR2" s="95"/>
+      <c r="CF2" s="101"/>
+      <c r="CG2" s="101"/>
+      <c r="CH2" s="101"/>
+      <c r="CI2" s="101"/>
+      <c r="CJ2" s="101"/>
+      <c r="CK2" s="101"/>
+      <c r="CL2" s="101"/>
+      <c r="CM2" s="101"/>
+      <c r="CN2" s="101"/>
+      <c r="CO2" s="101"/>
+      <c r="CP2" s="101"/>
+      <c r="CQ2" s="101"/>
+      <c r="CR2" s="101"/>
     </row>
     <row r="3" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A3" s="95"/>
-      <c r="B3" s="78" t="s">
+      <c r="A3" s="99"/>
+      <c r="B3" s="96" t="s">
         <v>110</v>
       </c>
-      <c r="C3" s="78">
+      <c r="C3" s="100">
         <v>12</v>
       </c>
-      <c r="D3" s="78">
+      <c r="D3" s="100">
         <v>13</v>
       </c>
-      <c r="E3" s="78">
+      <c r="E3" s="100">
         <v>14</v>
       </c>
-      <c r="F3" s="78">
+      <c r="F3" s="100">
         <v>15</v>
       </c>
-      <c r="G3" s="78">
+      <c r="G3" s="100">
         <v>16</v>
       </c>
-      <c r="H3" s="78">
+      <c r="H3" s="100">
         <v>19</v>
       </c>
-      <c r="I3" s="78">
+      <c r="I3" s="100">
         <v>20</v>
       </c>
-      <c r="J3" s="78">
+      <c r="J3" s="100">
         <v>21</v>
       </c>
-      <c r="K3" s="78">
+      <c r="K3" s="100">
         <v>22</v>
       </c>
-      <c r="L3" s="78">
+      <c r="L3" s="100">
         <v>23</v>
       </c>
-      <c r="M3" s="78">
+      <c r="M3" s="100">
         <v>26</v>
       </c>
-      <c r="N3" s="78">
+      <c r="N3" s="100">
         <v>27</v>
       </c>
-      <c r="O3" s="78">
+      <c r="O3" s="100">
         <v>28</v>
       </c>
-      <c r="P3" s="78">
+      <c r="P3" s="100">
         <v>29</v>
       </c>
-      <c r="Q3" s="78">
+      <c r="Q3" s="100">
         <v>30</v>
       </c>
-      <c r="R3" s="78">
+      <c r="R3" s="100">
         <v>2</v>
       </c>
-      <c r="S3" s="78">
+      <c r="S3" s="100">
         <v>3</v>
       </c>
-      <c r="T3" s="78">
+      <c r="T3" s="100">
         <v>4</v>
       </c>
-      <c r="U3" s="78">
+      <c r="U3" s="100">
         <v>5</v>
       </c>
-      <c r="V3" s="78">
+      <c r="V3" s="100">
         <v>6</v>
       </c>
-      <c r="W3" s="78">
+      <c r="W3" s="100">
         <v>9</v>
       </c>
-      <c r="X3" s="78">
+      <c r="X3" s="100">
         <v>10</v>
       </c>
-      <c r="Y3" s="78">
+      <c r="Y3" s="100">
         <v>11</v>
       </c>
-      <c r="Z3" s="78">
+      <c r="Z3" s="100">
         <v>12</v>
       </c>
-      <c r="AA3" s="78">
+      <c r="AA3" s="100">
         <v>13</v>
       </c>
-      <c r="AB3" s="78">
+      <c r="AB3" s="100">
         <v>16</v>
       </c>
-      <c r="AC3" s="78">
+      <c r="AC3" s="100">
         <v>17</v>
       </c>
-      <c r="AD3" s="78">
+      <c r="AD3" s="100">
         <v>18</v>
       </c>
-      <c r="AE3" s="78">
+      <c r="AE3" s="100">
         <v>19</v>
       </c>
-      <c r="AF3" s="78">
+      <c r="AF3" s="100">
         <v>20</v>
       </c>
-      <c r="AG3" s="78">
+      <c r="AG3" s="100">
         <v>23</v>
       </c>
-      <c r="AH3" s="78">
+      <c r="AH3" s="100">
         <v>24</v>
       </c>
-      <c r="AI3" s="78">
+      <c r="AI3" s="100">
         <v>25</v>
       </c>
-      <c r="AJ3" s="78">
+      <c r="AJ3" s="100">
         <v>26</v>
       </c>
-      <c r="AK3" s="78">
+      <c r="AK3" s="100">
         <v>27</v>
       </c>
-      <c r="AL3" s="78">
+      <c r="AL3" s="100">
         <v>30</v>
       </c>
-      <c r="AM3" s="78">
+      <c r="AM3" s="100">
         <v>1</v>
       </c>
-      <c r="AN3" s="78">
+      <c r="AN3" s="100">
         <v>2</v>
       </c>
-      <c r="AO3" s="78">
+      <c r="AO3" s="100">
         <v>3</v>
       </c>
-      <c r="AP3" s="78">
+      <c r="AP3" s="100">
         <v>4</v>
       </c>
-      <c r="AQ3" s="78">
+      <c r="AQ3" s="100">
         <v>7</v>
       </c>
-      <c r="AR3" s="78">
+      <c r="AR3" s="100">
         <v>8</v>
       </c>
-      <c r="AS3" s="78">
+      <c r="AS3" s="100">
         <v>9</v>
       </c>
-      <c r="AT3" s="78">
+      <c r="AT3" s="100">
         <v>10</v>
       </c>
-      <c r="AU3" s="78">
+      <c r="AU3" s="100">
         <v>11</v>
       </c>
       <c r="AV3" s="83">
@@ -7676,473 +7895,482 @@
       <c r="AW3" s="83">
         <v>15</v>
       </c>
-      <c r="AX3" s="78">
+      <c r="AX3" s="100">
         <v>16</v>
       </c>
-      <c r="AY3" s="78">
+      <c r="AY3" s="100">
         <v>17</v>
       </c>
-      <c r="AZ3" s="78">
+      <c r="AZ3" s="100">
         <v>18</v>
       </c>
-      <c r="BA3" s="78">
+      <c r="BA3" s="100">
         <v>21</v>
       </c>
-      <c r="BB3" s="78">
+      <c r="BB3" s="100">
         <v>22</v>
       </c>
-      <c r="BC3" s="78">
+      <c r="BC3" s="100">
         <v>23</v>
       </c>
-      <c r="BD3" s="78">
+      <c r="BD3" s="100">
         <v>24</v>
       </c>
-      <c r="BE3" s="78">
+      <c r="BE3" s="100">
         <v>25</v>
       </c>
-      <c r="BF3" s="78">
+      <c r="BF3" s="100">
         <v>28</v>
       </c>
-      <c r="BG3" s="78">
+      <c r="BG3" s="100">
         <v>29</v>
       </c>
-      <c r="BH3" s="78">
+      <c r="BH3" s="100">
         <v>30</v>
       </c>
-      <c r="BI3" s="78">
+      <c r="BI3" s="100">
         <v>31</v>
       </c>
-      <c r="BJ3" s="78">
+      <c r="BJ3" s="100">
         <v>1</v>
       </c>
-      <c r="BK3" s="78">
+      <c r="BK3" s="100">
         <v>4</v>
       </c>
-      <c r="BL3" s="78">
+      <c r="BL3" s="100">
         <v>5</v>
       </c>
-      <c r="BM3" s="78">
+      <c r="BM3" s="100">
         <v>6</v>
       </c>
-      <c r="BN3" s="78">
+      <c r="BN3" s="100">
         <v>7</v>
       </c>
-      <c r="BO3" s="78">
+      <c r="BO3" s="100">
         <v>8</v>
       </c>
-      <c r="BP3" s="78">
+      <c r="BP3" s="100">
         <v>11</v>
       </c>
-      <c r="BQ3" s="78">
+      <c r="BQ3" s="100">
         <v>12</v>
       </c>
-      <c r="BR3" s="78">
+      <c r="BR3" s="100">
         <v>13</v>
       </c>
-      <c r="BS3" s="78">
+      <c r="BS3" s="100">
         <v>14</v>
       </c>
       <c r="BT3" s="83">
         <v>15</v>
       </c>
-      <c r="BU3" s="78">
+      <c r="BU3" s="100">
         <v>18</v>
       </c>
-      <c r="BV3" s="78">
+      <c r="BV3" s="100">
         <v>19</v>
       </c>
       <c r="BW3" s="83">
         <v>20</v>
       </c>
-      <c r="BX3" s="78">
+      <c r="BX3" s="100">
         <v>21</v>
       </c>
-      <c r="BY3" s="78">
+      <c r="BY3" s="100">
         <v>22</v>
       </c>
-      <c r="BZ3" s="78">
+      <c r="BZ3" s="100">
         <v>25</v>
       </c>
-      <c r="CA3" s="78">
+      <c r="CA3" s="100">
         <v>26</v>
       </c>
-      <c r="CB3" s="78">
+      <c r="CB3" s="100">
         <v>27</v>
       </c>
-      <c r="CC3" s="78">
+      <c r="CC3" s="100">
         <v>28</v>
       </c>
-      <c r="CD3" s="78">
+      <c r="CD3" s="100">
         <v>29</v>
       </c>
-      <c r="CE3" s="78">
+      <c r="CE3" s="100">
         <v>2</v>
       </c>
-      <c r="CF3" s="78">
+      <c r="CF3" s="100">
         <v>3</v>
       </c>
-      <c r="CG3" s="78">
+      <c r="CG3" s="100">
         <v>4</v>
       </c>
-      <c r="CH3" s="78">
+      <c r="CH3" s="100">
         <v>5</v>
       </c>
-      <c r="CI3" s="78">
+      <c r="CI3" s="100">
         <v>6</v>
       </c>
-      <c r="CJ3" s="78">
+      <c r="CJ3" s="100">
         <v>9</v>
       </c>
-      <c r="CK3" s="78">
+      <c r="CK3" s="100">
         <v>10</v>
       </c>
-      <c r="CL3" s="78">
+      <c r="CL3" s="100">
         <v>11</v>
       </c>
-      <c r="CM3" s="78">
+      <c r="CM3" s="100">
         <v>12</v>
       </c>
-      <c r="CN3" s="78">
+      <c r="CN3" s="100">
         <v>13</v>
       </c>
       <c r="CO3" s="83">
         <v>14</v>
       </c>
-      <c r="CP3" s="78">
+      <c r="CP3" s="95">
         <v>16</v>
       </c>
-      <c r="CQ3" s="78">
+      <c r="CQ3" s="95">
         <v>17</v>
       </c>
-      <c r="CR3" s="78">
+      <c r="CR3" s="95">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:96" s="85" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="84" t="s">
+    <row r="4" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="102" t="s">
         <v>111</v>
       </c>
-      <c r="C4" s="98" t="s">
+      <c r="B4" s="103"/>
+      <c r="C4" s="87" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" s="87" t="s">
+        <v>122</v>
+      </c>
+      <c r="E4" s="87" t="s">
+        <v>123</v>
+      </c>
+      <c r="F4" s="87"/>
+      <c r="G4" s="87"/>
+      <c r="H4" s="87"/>
+      <c r="I4" s="87"/>
+      <c r="J4" s="87"/>
+      <c r="K4" s="87"/>
+      <c r="L4" s="87"/>
+      <c r="M4" s="87"/>
+      <c r="N4" s="87"/>
+      <c r="O4" s="85"/>
+      <c r="P4" s="85"/>
+      <c r="Q4" s="85"/>
+      <c r="AV4" s="105" t="s">
+        <v>112</v>
+      </c>
+      <c r="AW4" s="105" t="s">
+        <v>112</v>
+      </c>
+      <c r="BT4" s="105" t="s">
+        <v>113</v>
+      </c>
+      <c r="BW4" s="105" t="s">
+        <v>114</v>
+      </c>
+      <c r="CO4" s="105" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="5" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="102" t="s">
+        <v>115</v>
+      </c>
+      <c r="B5" s="103"/>
+      <c r="C5" s="87" t="s">
+        <v>118</v>
+      </c>
+      <c r="D5" s="87" t="s">
         <v>119</v>
       </c>
-      <c r="D4" s="98" t="s">
-        <v>123</v>
-      </c>
-      <c r="E4" s="98" t="s">
+      <c r="E5" s="87" t="s">
         <v>124</v>
       </c>
-      <c r="F4" s="98"/>
-      <c r="G4" s="98"/>
-      <c r="H4" s="98"/>
-      <c r="I4" s="98"/>
-      <c r="J4" s="98"/>
-      <c r="K4" s="98"/>
-      <c r="L4" s="98"/>
-      <c r="M4" s="98"/>
-      <c r="N4" s="98"/>
-      <c r="O4" s="86"/>
-      <c r="P4" s="86"/>
-      <c r="Q4" s="86"/>
-      <c r="AV4" s="96" t="s">
-        <v>112</v>
-      </c>
-      <c r="AW4" s="96" t="s">
-        <v>112</v>
-      </c>
-      <c r="BT4" s="96" t="s">
-        <v>113</v>
-      </c>
-      <c r="BW4" s="96" t="s">
-        <v>114</v>
-      </c>
-      <c r="CO4" s="96" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="5" spans="1:96" s="85" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="84" t="s">
+      <c r="F5" s="87"/>
+      <c r="G5" s="87"/>
+      <c r="H5" s="87"/>
+      <c r="I5" s="87"/>
+      <c r="J5" s="87"/>
+      <c r="K5" s="87"/>
+      <c r="L5" s="87"/>
+      <c r="M5" s="87"/>
+      <c r="N5" s="87"/>
+      <c r="O5" s="85"/>
+      <c r="P5" s="85"/>
+      <c r="Q5" s="85"/>
+      <c r="AV5" s="105"/>
+      <c r="AW5" s="105"/>
+      <c r="BT5" s="105"/>
+      <c r="BW5" s="105"/>
+      <c r="CO5" s="105"/>
+    </row>
+    <row r="6" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="102" t="s">
         <v>116</v>
       </c>
-      <c r="C5" s="98" t="s">
-        <v>119</v>
-      </c>
-      <c r="D5" s="98" t="s">
+      <c r="B6" s="103"/>
+      <c r="C6" s="87" t="s">
+        <v>118</v>
+      </c>
+      <c r="D6" s="87" t="s">
         <v>120</v>
       </c>
-      <c r="E5" s="98" t="s">
+      <c r="E6" s="87" t="s">
         <v>125</v>
       </c>
-      <c r="F5" s="98"/>
-      <c r="G5" s="98"/>
-      <c r="H5" s="98"/>
-      <c r="I5" s="98"/>
-      <c r="J5" s="98"/>
-      <c r="K5" s="98"/>
-      <c r="L5" s="98"/>
-      <c r="M5" s="98"/>
-      <c r="N5" s="98"/>
-      <c r="O5" s="86"/>
-      <c r="P5" s="86"/>
-      <c r="Q5" s="86"/>
-      <c r="AV5" s="96"/>
-      <c r="AW5" s="96"/>
-      <c r="BT5" s="96"/>
-      <c r="BW5" s="96"/>
-      <c r="CO5" s="96"/>
-    </row>
-    <row r="6" spans="1:96" s="85" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="84" t="s">
+      <c r="F6" s="87"/>
+      <c r="G6" s="87"/>
+      <c r="H6" s="87"/>
+      <c r="I6" s="87"/>
+      <c r="J6" s="87"/>
+      <c r="K6" s="87"/>
+      <c r="L6" s="87"/>
+      <c r="M6" s="87"/>
+      <c r="N6" s="87"/>
+      <c r="O6" s="85"/>
+      <c r="P6" s="85"/>
+      <c r="Q6" s="85"/>
+      <c r="AV6" s="105"/>
+      <c r="AW6" s="105"/>
+      <c r="BT6" s="105"/>
+      <c r="BW6" s="105"/>
+      <c r="CO6" s="105"/>
+    </row>
+    <row r="7" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="102" t="s">
         <v>117</v>
       </c>
-      <c r="C6" s="98" t="s">
-        <v>119</v>
-      </c>
-      <c r="D6" s="98" t="s">
+      <c r="B7" s="103"/>
+      <c r="C7" s="87" t="s">
+        <v>118</v>
+      </c>
+      <c r="D7" s="87" t="s">
         <v>121</v>
       </c>
-      <c r="E6" s="98" t="s">
+      <c r="E7" s="87" t="s">
         <v>126</v>
       </c>
-      <c r="F6" s="98"/>
-      <c r="G6" s="98"/>
-      <c r="H6" s="98"/>
-      <c r="I6" s="98"/>
-      <c r="J6" s="98"/>
-      <c r="K6" s="98"/>
-      <c r="L6" s="98"/>
-      <c r="M6" s="98"/>
-      <c r="N6" s="98"/>
-      <c r="O6" s="86"/>
-      <c r="P6" s="86"/>
-      <c r="Q6" s="86"/>
-      <c r="AV6" s="96"/>
-      <c r="AW6" s="96"/>
-      <c r="BT6" s="96"/>
-      <c r="BW6" s="96"/>
-      <c r="CO6" s="96"/>
-    </row>
-    <row r="7" spans="1:96" s="85" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="84" t="s">
-        <v>118</v>
-      </c>
-      <c r="C7" s="98" t="s">
-        <v>119</v>
-      </c>
-      <c r="D7" s="98" t="s">
-        <v>122</v>
-      </c>
-      <c r="E7" s="98" t="s">
-        <v>127</v>
-      </c>
-      <c r="F7" s="98"/>
-      <c r="G7" s="98"/>
-      <c r="H7" s="98"/>
-      <c r="I7" s="98"/>
-      <c r="J7" s="98"/>
-      <c r="K7" s="98"/>
-      <c r="L7" s="98"/>
-      <c r="M7" s="98"/>
-      <c r="N7" s="98"/>
-      <c r="O7" s="86"/>
-      <c r="P7" s="86"/>
-      <c r="Q7" s="86"/>
-      <c r="AV7" s="96"/>
-      <c r="AW7" s="96"/>
-      <c r="BT7" s="96"/>
-      <c r="BW7" s="96"/>
-      <c r="CO7" s="96"/>
+      <c r="F7" s="87"/>
+      <c r="G7" s="87"/>
+      <c r="H7" s="87"/>
+      <c r="I7" s="87"/>
+      <c r="J7" s="87"/>
+      <c r="K7" s="87"/>
+      <c r="L7" s="87"/>
+      <c r="M7" s="87"/>
+      <c r="N7" s="87"/>
+      <c r="O7" s="85"/>
+      <c r="P7" s="85"/>
+      <c r="Q7" s="85"/>
+      <c r="AV7" s="105"/>
+      <c r="AW7" s="105"/>
+      <c r="BT7" s="105"/>
+      <c r="BW7" s="105"/>
+      <c r="CO7" s="105"/>
     </row>
     <row r="8" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="AV8" s="96"/>
-      <c r="AW8" s="96"/>
-      <c r="BT8" s="96"/>
-      <c r="BW8" s="96"/>
-      <c r="CO8" s="96"/>
+      <c r="AV8" s="104"/>
+      <c r="AW8" s="104"/>
+      <c r="BT8" s="104"/>
+      <c r="BW8" s="104"/>
+      <c r="CO8" s="104"/>
     </row>
     <row r="9" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="AV9" s="96"/>
-      <c r="AW9" s="96"/>
-      <c r="BT9" s="96"/>
-      <c r="BW9" s="96"/>
-      <c r="CO9" s="96"/>
+      <c r="AV9" s="104"/>
+      <c r="AW9" s="104"/>
+      <c r="BT9" s="104"/>
+      <c r="BW9" s="104"/>
+      <c r="CO9" s="104"/>
     </row>
     <row r="10" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="AV10" s="96"/>
-      <c r="AW10" s="96"/>
-      <c r="BT10" s="96"/>
-      <c r="BW10" s="96"/>
-      <c r="CO10" s="96"/>
+      <c r="AV10" s="104"/>
+      <c r="AW10" s="104"/>
+      <c r="BT10" s="104"/>
+      <c r="BW10" s="104"/>
+      <c r="CO10" s="104"/>
     </row>
     <row r="11" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="AV11" s="96"/>
-      <c r="AW11" s="96"/>
-      <c r="BT11" s="96"/>
-      <c r="BW11" s="96"/>
-      <c r="CO11" s="96"/>
+      <c r="AV11" s="104"/>
+      <c r="AW11" s="104"/>
+      <c r="BT11" s="104"/>
+      <c r="BW11" s="104"/>
+      <c r="CO11" s="104"/>
     </row>
     <row r="12" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="AV12" s="96"/>
-      <c r="AW12" s="96"/>
-      <c r="BT12" s="96"/>
-      <c r="BW12" s="96"/>
-      <c r="CO12" s="96"/>
+      <c r="AV12" s="104"/>
+      <c r="AW12" s="104"/>
+      <c r="BT12" s="104"/>
+      <c r="BW12" s="104"/>
+      <c r="CO12" s="104"/>
     </row>
     <row r="13" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="AV13" s="96"/>
-      <c r="AW13" s="96"/>
-      <c r="BT13" s="96"/>
-      <c r="BW13" s="96"/>
-      <c r="CO13" s="96"/>
+      <c r="AV13" s="104"/>
+      <c r="AW13" s="104"/>
+      <c r="BT13" s="104"/>
+      <c r="BW13" s="104"/>
+      <c r="CO13" s="104"/>
     </row>
     <row r="14" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="AV14" s="96"/>
-      <c r="AW14" s="96"/>
-      <c r="BT14" s="96"/>
-      <c r="BW14" s="96"/>
-      <c r="CO14" s="96"/>
+      <c r="AV14" s="104"/>
+      <c r="AW14" s="104"/>
+      <c r="BT14" s="104"/>
+      <c r="BW14" s="104"/>
+      <c r="CO14" s="104"/>
     </row>
     <row r="15" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="AV15" s="96"/>
-      <c r="AW15" s="96"/>
-      <c r="BT15" s="96"/>
-      <c r="BW15" s="96"/>
-      <c r="CO15" s="96"/>
+      <c r="AV15" s="104"/>
+      <c r="AW15" s="104"/>
+      <c r="BT15" s="104"/>
+      <c r="BW15" s="104"/>
+      <c r="CO15" s="104"/>
     </row>
     <row r="16" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="AV16" s="96"/>
-      <c r="AW16" s="96"/>
-      <c r="BT16" s="96"/>
-      <c r="BW16" s="96"/>
-      <c r="CO16" s="96"/>
+      <c r="AV16" s="104"/>
+      <c r="AW16" s="104"/>
+      <c r="BT16" s="104"/>
+      <c r="BW16" s="104"/>
+      <c r="CO16" s="104"/>
     </row>
     <row r="17" spans="48:93" x14ac:dyDescent="0.25">
-      <c r="AV17" s="96"/>
-      <c r="AW17" s="96"/>
-      <c r="BT17" s="96"/>
-      <c r="BW17" s="96"/>
-      <c r="CO17" s="96"/>
+      <c r="AV17" s="104"/>
+      <c r="AW17" s="104"/>
+      <c r="BT17" s="104"/>
+      <c r="BW17" s="104"/>
+      <c r="CO17" s="104"/>
     </row>
     <row r="18" spans="48:93" x14ac:dyDescent="0.25">
-      <c r="AV18" s="96"/>
-      <c r="AW18" s="96"/>
-      <c r="BT18" s="96"/>
-      <c r="BW18" s="96"/>
-      <c r="CO18" s="96"/>
+      <c r="AV18" s="104"/>
+      <c r="AW18" s="104"/>
+      <c r="BT18" s="104"/>
+      <c r="BW18" s="104"/>
+      <c r="CO18" s="104"/>
     </row>
     <row r="19" spans="48:93" x14ac:dyDescent="0.25">
-      <c r="AV19" s="96"/>
-      <c r="AW19" s="96"/>
-      <c r="BT19" s="96"/>
-      <c r="BW19" s="96"/>
-      <c r="CO19" s="96"/>
+      <c r="AV19" s="104"/>
+      <c r="AW19" s="104"/>
+      <c r="BT19" s="104"/>
+      <c r="BW19" s="104"/>
+      <c r="CO19" s="104"/>
     </row>
     <row r="20" spans="48:93" x14ac:dyDescent="0.25">
-      <c r="AV20" s="96"/>
-      <c r="AW20" s="96"/>
-      <c r="BT20" s="96"/>
-      <c r="BW20" s="96"/>
-      <c r="CO20" s="96"/>
+      <c r="AV20" s="104"/>
+      <c r="AW20" s="104"/>
+      <c r="BT20" s="104"/>
+      <c r="BW20" s="104"/>
+      <c r="CO20" s="104"/>
     </row>
     <row r="21" spans="48:93" x14ac:dyDescent="0.25">
-      <c r="AV21" s="96"/>
-      <c r="AW21" s="96"/>
-      <c r="BT21" s="96"/>
-      <c r="BW21" s="96"/>
-      <c r="CO21" s="96"/>
+      <c r="AV21" s="104"/>
+      <c r="AW21" s="104"/>
+      <c r="BT21" s="104"/>
+      <c r="BW21" s="104"/>
+      <c r="CO21" s="104"/>
     </row>
     <row r="22" spans="48:93" x14ac:dyDescent="0.25">
-      <c r="AV22" s="96"/>
-      <c r="AW22" s="96"/>
-      <c r="BT22" s="96"/>
-      <c r="BW22" s="96"/>
-      <c r="CO22" s="96"/>
+      <c r="AV22" s="104"/>
+      <c r="AW22" s="104"/>
+      <c r="BT22" s="104"/>
+      <c r="BW22" s="104"/>
+      <c r="CO22" s="104"/>
     </row>
     <row r="23" spans="48:93" x14ac:dyDescent="0.25">
-      <c r="AV23" s="96"/>
-      <c r="AW23" s="96"/>
-      <c r="BT23" s="96"/>
-      <c r="BW23" s="96"/>
-      <c r="CO23" s="96"/>
+      <c r="AV23" s="104"/>
+      <c r="AW23" s="104"/>
+      <c r="BT23" s="104"/>
+      <c r="BW23" s="104"/>
+      <c r="CO23" s="104"/>
     </row>
     <row r="24" spans="48:93" x14ac:dyDescent="0.25">
-      <c r="AV24" s="96"/>
-      <c r="AW24" s="96"/>
-      <c r="BT24" s="96"/>
-      <c r="BW24" s="96"/>
-      <c r="CO24" s="96"/>
+      <c r="AV24" s="104"/>
+      <c r="AW24" s="104"/>
+      <c r="BT24" s="104"/>
+      <c r="BW24" s="104"/>
+      <c r="CO24" s="104"/>
     </row>
     <row r="25" spans="48:93" x14ac:dyDescent="0.25">
-      <c r="AV25" s="96"/>
-      <c r="AW25" s="96"/>
-      <c r="BT25" s="96"/>
-      <c r="BW25" s="96"/>
-      <c r="CO25" s="96"/>
+      <c r="AV25" s="104"/>
+      <c r="AW25" s="104"/>
+      <c r="BT25" s="104"/>
+      <c r="BW25" s="104"/>
+      <c r="CO25" s="104"/>
     </row>
     <row r="26" spans="48:93" x14ac:dyDescent="0.25">
-      <c r="AV26" s="96"/>
-      <c r="AW26" s="96"/>
-      <c r="BT26" s="96"/>
-      <c r="BW26" s="96"/>
-      <c r="CO26" s="96"/>
+      <c r="AV26" s="104"/>
+      <c r="AW26" s="104"/>
+      <c r="BT26" s="104"/>
+      <c r="BW26" s="104"/>
+      <c r="CO26" s="104"/>
     </row>
     <row r="27" spans="48:93" x14ac:dyDescent="0.25">
-      <c r="AV27" s="96"/>
-      <c r="AW27" s="96"/>
-      <c r="BT27" s="96"/>
-      <c r="BW27" s="96"/>
-      <c r="CO27" s="96"/>
+      <c r="AV27" s="104"/>
+      <c r="AW27" s="104"/>
+      <c r="BT27" s="104"/>
+      <c r="BW27" s="104"/>
+      <c r="CO27" s="104"/>
     </row>
     <row r="28" spans="48:93" x14ac:dyDescent="0.25">
-      <c r="AV28" s="87"/>
+      <c r="AV28" s="86"/>
     </row>
     <row r="29" spans="48:93" x14ac:dyDescent="0.25">
-      <c r="AV29" s="87"/>
+      <c r="AV29" s="86"/>
     </row>
     <row r="30" spans="48:93" x14ac:dyDescent="0.25">
-      <c r="AV30" s="87"/>
+      <c r="AV30" s="86"/>
     </row>
     <row r="31" spans="48:93" x14ac:dyDescent="0.25">
-      <c r="AV31" s="87"/>
+      <c r="AV31" s="86"/>
     </row>
     <row r="32" spans="48:93" x14ac:dyDescent="0.25">
-      <c r="AV32" s="87"/>
+      <c r="AV32" s="86"/>
     </row>
     <row r="33" spans="48:48" x14ac:dyDescent="0.25">
-      <c r="AV33" s="87"/>
+      <c r="AV33" s="86"/>
     </row>
     <row r="34" spans="48:48" x14ac:dyDescent="0.25">
-      <c r="AV34" s="87"/>
+      <c r="AV34" s="86"/>
     </row>
     <row r="35" spans="48:48" x14ac:dyDescent="0.25">
-      <c r="AV35" s="87"/>
+      <c r="AV35" s="86"/>
     </row>
     <row r="36" spans="48:48" x14ac:dyDescent="0.25">
-      <c r="AV36" s="87"/>
+      <c r="AV36" s="86"/>
     </row>
     <row r="37" spans="48:48" x14ac:dyDescent="0.25">
-      <c r="AV37" s="87"/>
+      <c r="AV37" s="86"/>
     </row>
     <row r="38" spans="48:48" x14ac:dyDescent="0.25">
-      <c r="AV38" s="87"/>
+      <c r="AV38" s="86"/>
     </row>
     <row r="39" spans="48:48" x14ac:dyDescent="0.25">
-      <c r="AV39" s="87"/>
+      <c r="AV39" s="86"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="15">
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="AV4:AV7"/>
+    <mergeCell ref="CE2:CR2"/>
+    <mergeCell ref="AW4:AW7"/>
+    <mergeCell ref="BT4:BT7"/>
+    <mergeCell ref="BW4:BW7"/>
+    <mergeCell ref="CO4:CO7"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="C2:Q2"/>
     <mergeCell ref="R2:AL2"/>
     <mergeCell ref="AM2:BI2"/>
     <mergeCell ref="BJ2:CD2"/>
-    <mergeCell ref="CE2:CR2"/>
-    <mergeCell ref="AV4:AV27"/>
-    <mergeCell ref="AW4:AW27"/>
-    <mergeCell ref="BT4:BT27"/>
-    <mergeCell ref="BW4:BW27"/>
-    <mergeCell ref="CO4:CO27"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adiciona daily realizada em 16-08
</commit_message>
<xml_diff>
--- a/Cronograma/Projeto-Cronograma - Acompanhamento.xlsx
+++ b/Cronograma/Projeto-Cronograma - Acompanhamento.xlsx
@@ -1,20 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Works\Cursos\senai_desenvolvimento\2s2019\2s2019-t3-mentoria\Cronograma\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\39893838843\Downloads\2s2019-t3-mentoria\Cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C89556BB-515D-4698-9B10-4FD3A9570D18}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Proj-Cronograma" sheetId="1" r:id="rId1"/>
-    <sheet name="Dailys" sheetId="2" r:id="rId2"/>
+    <sheet name="Dailies" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -26,12 +25,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Saulo Santos</author>
   </authors>
   <commentList>
-    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{B823D240-44A1-4AA8-AD85-B98BE0488E33}">
+    <comment ref="A4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -48,7 +47,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{EFDCB323-A12C-4FE4-999F-BA8C5695F98E}">
+    <comment ref="A5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -65,7 +64,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{37BAB12C-F1E4-410F-9AC0-AAB1C84CED66}">
+    <comment ref="A6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -83,7 +82,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{79CF17A7-FE5A-4F77-8A3A-117B42495EE1}">
+    <comment ref="A7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -106,7 +105,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="132">
   <si>
     <t>REDES</t>
   </si>
@@ -490,12 +489,24 @@
   </si>
   <si>
     <t>Apresentação dos Projetos</t>
+  </si>
+  <si>
+    <t>Definição do roteiro de perguntas, criação do modelo de apresentações, divisão de quem fará as perguntas</t>
+  </si>
+  <si>
+    <t>Roteiro de perguntas, ínicio do projeto 1 com algumas funcionalidades</t>
+  </si>
+  <si>
+    <t>Roteiro e formulário com as perguntas, filtrando-as. Início da modelagem do banco de dados</t>
+  </si>
+  <si>
+    <t>Finalizaram as perguntas que serão feitas, pesquisa de mercado com sistemas semelhantes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -1122,18 +1133,6 @@
     <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1142,6 +1141,18 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="27" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1524,11 +1535,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK942"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="S4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="T4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
       <selection pane="bottomRight" activeCell="Q11" sqref="Q11"/>
@@ -7334,11 +7345,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CR39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -7360,7 +7371,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A1" s="103" t="s">
+      <c r="A1" s="99" t="s">
         <v>102</v>
       </c>
       <c r="B1" s="89" t="s">
@@ -7640,7 +7651,7 @@
       </c>
     </row>
     <row r="2" spans="1:96" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="104"/>
+      <c r="A2" s="100"/>
       <c r="B2" s="89" t="s">
         <v>104</v>
       </c>
@@ -7750,7 +7761,7 @@
       <c r="CR2" s="102"/>
     </row>
     <row r="3" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A3" s="105"/>
+      <c r="A3" s="101"/>
       <c r="B3" s="89" t="s">
         <v>110</v>
       </c>
@@ -8038,10 +8049,10 @@
       </c>
     </row>
     <row r="4" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="99" t="s">
+      <c r="A4" s="104" t="s">
         <v>111</v>
       </c>
-      <c r="B4" s="100"/>
+      <c r="B4" s="105"/>
       <c r="C4" s="87" t="s">
         <v>118</v>
       </c>
@@ -8051,7 +8062,9 @@
       <c r="E4" s="87" t="s">
         <v>123</v>
       </c>
-      <c r="F4" s="87"/>
+      <c r="F4" s="87" t="s">
+        <v>128</v>
+      </c>
       <c r="G4" s="87"/>
       <c r="H4" s="87"/>
       <c r="I4" s="87"/>
@@ -8063,27 +8076,27 @@
       <c r="O4" s="85"/>
       <c r="P4" s="85"/>
       <c r="Q4" s="85"/>
-      <c r="AV4" s="101" t="s">
+      <c r="AV4" s="103" t="s">
         <v>112</v>
       </c>
-      <c r="AW4" s="101" t="s">
+      <c r="AW4" s="103" t="s">
         <v>112</v>
       </c>
-      <c r="BT4" s="101" t="s">
+      <c r="BT4" s="103" t="s">
         <v>113</v>
       </c>
-      <c r="BW4" s="101" t="s">
+      <c r="BW4" s="103" t="s">
         <v>114</v>
       </c>
-      <c r="CO4" s="101" t="s">
+      <c r="CO4" s="103" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="99" t="s">
+      <c r="A5" s="104" t="s">
         <v>115</v>
       </c>
-      <c r="B5" s="100"/>
+      <c r="B5" s="105"/>
       <c r="C5" s="87" t="s">
         <v>118</v>
       </c>
@@ -8093,7 +8106,9 @@
       <c r="E5" s="87" t="s">
         <v>124</v>
       </c>
-      <c r="F5" s="87"/>
+      <c r="F5" s="87" t="s">
+        <v>129</v>
+      </c>
       <c r="G5" s="87"/>
       <c r="H5" s="87"/>
       <c r="I5" s="87"/>
@@ -8105,17 +8120,17 @@
       <c r="O5" s="85"/>
       <c r="P5" s="85"/>
       <c r="Q5" s="85"/>
-      <c r="AV5" s="101"/>
-      <c r="AW5" s="101"/>
-      <c r="BT5" s="101"/>
-      <c r="BW5" s="101"/>
-      <c r="CO5" s="101"/>
+      <c r="AV5" s="103"/>
+      <c r="AW5" s="103"/>
+      <c r="BT5" s="103"/>
+      <c r="BW5" s="103"/>
+      <c r="CO5" s="103"/>
     </row>
     <row r="6" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="99" t="s">
+      <c r="A6" s="104" t="s">
         <v>116</v>
       </c>
-      <c r="B6" s="100"/>
+      <c r="B6" s="105"/>
       <c r="C6" s="87" t="s">
         <v>118</v>
       </c>
@@ -8125,7 +8140,9 @@
       <c r="E6" s="87" t="s">
         <v>125</v>
       </c>
-      <c r="F6" s="87"/>
+      <c r="F6" s="87" t="s">
+        <v>130</v>
+      </c>
       <c r="G6" s="87"/>
       <c r="H6" s="87"/>
       <c r="I6" s="87"/>
@@ -8137,17 +8154,17 @@
       <c r="O6" s="85"/>
       <c r="P6" s="85"/>
       <c r="Q6" s="85"/>
-      <c r="AV6" s="101"/>
-      <c r="AW6" s="101"/>
-      <c r="BT6" s="101"/>
-      <c r="BW6" s="101"/>
-      <c r="CO6" s="101"/>
+      <c r="AV6" s="103"/>
+      <c r="AW6" s="103"/>
+      <c r="BT6" s="103"/>
+      <c r="BW6" s="103"/>
+      <c r="CO6" s="103"/>
     </row>
     <row r="7" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="99" t="s">
+      <c r="A7" s="104" t="s">
         <v>117</v>
       </c>
-      <c r="B7" s="100"/>
+      <c r="B7" s="105"/>
       <c r="C7" s="87" t="s">
         <v>118</v>
       </c>
@@ -8157,7 +8174,9 @@
       <c r="E7" s="87" t="s">
         <v>126</v>
       </c>
-      <c r="F7" s="87"/>
+      <c r="F7" s="87" t="s">
+        <v>131</v>
+      </c>
       <c r="G7" s="87"/>
       <c r="H7" s="87"/>
       <c r="I7" s="87"/>
@@ -8169,11 +8188,11 @@
       <c r="O7" s="85"/>
       <c r="P7" s="85"/>
       <c r="Q7" s="85"/>
-      <c r="AV7" s="101"/>
-      <c r="AW7" s="101"/>
-      <c r="BT7" s="101"/>
-      <c r="BW7" s="101"/>
-      <c r="CO7" s="101"/>
+      <c r="AV7" s="103"/>
+      <c r="AW7" s="103"/>
+      <c r="BT7" s="103"/>
+      <c r="BW7" s="103"/>
+      <c r="CO7" s="103"/>
     </row>
     <row r="8" spans="1:96" x14ac:dyDescent="0.25">
       <c r="AV8" s="91"/>
@@ -8353,21 +8372,21 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="AV4:AV7"/>
+    <mergeCell ref="CE2:CR2"/>
+    <mergeCell ref="AW4:AW7"/>
+    <mergeCell ref="BT4:BT7"/>
+    <mergeCell ref="BW4:BW7"/>
+    <mergeCell ref="CO4:CO7"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="C2:Q2"/>
     <mergeCell ref="R2:AL2"/>
     <mergeCell ref="AM2:BI2"/>
     <mergeCell ref="BJ2:CD2"/>
-    <mergeCell ref="CE2:CR2"/>
-    <mergeCell ref="AW4:AW7"/>
-    <mergeCell ref="BT4:BT7"/>
-    <mergeCell ref="BW4:BW7"/>
-    <mergeCell ref="CO4:CO7"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="AV4:AV7"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Melhora estilização da planilha
</commit_message>
<xml_diff>
--- a/Cronograma/Projeto-Cronograma - Acompanhamento.xlsx
+++ b/Cronograma/Projeto-Cronograma - Acompanhamento.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\39893838843\Downloads\2s2019-t3-mentoria\Cronograma\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Works\Cursos\senai_desenvolvimento\2s2019\2s2019-t3-mentoria\Cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{449CD73E-C075-4711-BE1E-747C328E9EC0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Proj-Cronograma" sheetId="1" r:id="rId1"/>
@@ -25,12 +26,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Saulo Santos</author>
   </authors>
   <commentList>
-    <comment ref="A4" authorId="0" shapeId="0">
+    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -47,7 +48,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A5" authorId="0" shapeId="0">
+    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -64,7 +65,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A6" authorId="0" shapeId="0">
+    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
       <text>
         <r>
           <rPr>
@@ -82,7 +83,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A7" authorId="0" shapeId="0">
+    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
       <text>
         <r>
           <rPr>
@@ -506,7 +507,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -883,7 +884,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1094,9 +1095,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" textRotation="255"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1108,9 +1106,6 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="255"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1133,6 +1128,18 @@
     <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1141,18 +1148,6 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="27" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1535,7 +1530,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMK942"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -1557,7 +1552,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:116" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="94" t="s">
+      <c r="A1" s="92" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -1897,7 +1892,7 @@
       </c>
     </row>
     <row r="2" spans="1:116" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="94"/>
+      <c r="A2" s="92"/>
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
@@ -2223,15 +2218,15 @@
         <v>12</v>
       </c>
       <c r="DF2" s="11"/>
-      <c r="DG2" s="95"/>
-      <c r="DH2" s="95"/>
-      <c r="DI2" s="95"/>
-      <c r="DJ2" s="95"/>
+      <c r="DG2" s="93"/>
+      <c r="DH2" s="93"/>
+      <c r="DI2" s="93"/>
+      <c r="DJ2" s="93"/>
       <c r="DK2" s="12"/>
       <c r="DL2" s="12"/>
     </row>
     <row r="3" spans="1:116" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="94"/>
+      <c r="A3" s="92"/>
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
@@ -2568,7 +2563,7 @@
       <c r="A4" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="96" t="s">
+      <c r="B4" s="94" t="s">
         <v>38</v>
       </c>
       <c r="C4" s="20" t="s">
@@ -2710,7 +2705,7 @@
       <c r="A5" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="96"/>
+      <c r="B5" s="94"/>
       <c r="C5" s="22"/>
       <c r="D5" s="22"/>
       <c r="E5" s="22"/>
@@ -2850,7 +2845,7 @@
       <c r="A6" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="B6" s="96"/>
+      <c r="B6" s="94"/>
       <c r="C6" s="22"/>
       <c r="D6" s="22"/>
       <c r="E6" s="22"/>
@@ -2990,7 +2985,7 @@
       <c r="A7" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="B7" s="96"/>
+      <c r="B7" s="94"/>
       <c r="C7" s="22"/>
       <c r="D7" s="22"/>
       <c r="E7" s="22"/>
@@ -3128,7 +3123,7 @@
       <c r="A8" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="B8" s="96"/>
+      <c r="B8" s="94"/>
       <c r="C8" s="22"/>
       <c r="D8" s="22"/>
       <c r="E8" s="22"/>
@@ -3268,7 +3263,7 @@
       <c r="A9" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="B9" s="97" t="s">
+      <c r="B9" s="95" t="s">
         <v>58</v>
       </c>
       <c r="C9" s="22"/>
@@ -3410,7 +3405,7 @@
       <c r="A10" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="B10" s="97"/>
+      <c r="B10" s="95"/>
       <c r="C10" s="22"/>
       <c r="D10" s="22"/>
       <c r="E10" s="22"/>
@@ -3550,7 +3545,7 @@
       <c r="A11" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="B11" s="98" t="s">
+      <c r="B11" s="96" t="s">
         <v>66</v>
       </c>
       <c r="C11" s="22"/>
@@ -3680,7 +3675,7 @@
       <c r="A12" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="B12" s="98"/>
+      <c r="B12" s="96"/>
       <c r="C12" s="22"/>
       <c r="D12" s="22"/>
       <c r="E12" s="22"/>
@@ -3818,7 +3813,7 @@
       <c r="A13" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="B13" s="98"/>
+      <c r="B13" s="96"/>
       <c r="C13" s="22"/>
       <c r="D13" s="22"/>
       <c r="E13" s="22"/>
@@ -3958,7 +3953,7 @@
       <c r="A14" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="B14" s="98"/>
+      <c r="B14" s="96"/>
       <c r="C14" s="22"/>
       <c r="D14" s="22"/>
       <c r="E14" s="22"/>
@@ -4094,7 +4089,7 @@
       <c r="A15" s="35" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="98"/>
+      <c r="B15" s="96"/>
       <c r="C15" s="22"/>
       <c r="D15" s="22"/>
       <c r="E15" s="22"/>
@@ -4230,7 +4225,7 @@
       <c r="A16" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="B16" s="98"/>
+      <c r="B16" s="96"/>
       <c r="C16" s="22"/>
       <c r="D16" s="22"/>
       <c r="E16" s="22"/>
@@ -4366,7 +4361,7 @@
       <c r="A17" s="35" t="s">
         <v>78</v>
       </c>
-      <c r="B17" s="98"/>
+      <c r="B17" s="96"/>
       <c r="C17" s="22"/>
       <c r="D17" s="22"/>
       <c r="E17" s="22"/>
@@ -4502,7 +4497,7 @@
       <c r="A18" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="B18" s="98"/>
+      <c r="B18" s="96"/>
       <c r="C18" s="22"/>
       <c r="D18" s="22"/>
       <c r="E18" s="22"/>
@@ -4642,7 +4637,7 @@
       <c r="A19" s="40" t="s">
         <v>81</v>
       </c>
-      <c r="B19" s="98"/>
+      <c r="B19" s="96"/>
       <c r="C19" s="22"/>
       <c r="D19" s="22"/>
       <c r="E19" s="22"/>
@@ -4778,7 +4773,7 @@
       <c r="A20" s="43" t="s">
         <v>82</v>
       </c>
-      <c r="B20" s="98"/>
+      <c r="B20" s="96"/>
       <c r="C20" s="22"/>
       <c r="D20" s="22"/>
       <c r="E20" s="22"/>
@@ -4914,7 +4909,7 @@
       <c r="A21" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="B21" s="92" t="s">
+      <c r="B21" s="90" t="s">
         <v>86</v>
       </c>
       <c r="C21" s="22"/>
@@ -5048,7 +5043,7 @@
       <c r="A22" s="50" t="s">
         <v>88</v>
       </c>
-      <c r="B22" s="92"/>
+      <c r="B22" s="90"/>
       <c r="C22" s="22"/>
       <c r="D22" s="22"/>
       <c r="E22" s="22"/>
@@ -5184,7 +5179,7 @@
       <c r="A23" s="54" t="s">
         <v>89</v>
       </c>
-      <c r="B23" s="92"/>
+      <c r="B23" s="90"/>
       <c r="C23" s="22"/>
       <c r="D23" s="22"/>
       <c r="E23" s="22"/>
@@ -5316,7 +5311,7 @@
       <c r="A24" s="57" t="s">
         <v>90</v>
       </c>
-      <c r="B24" s="92"/>
+      <c r="B24" s="90"/>
       <c r="C24" s="22"/>
       <c r="D24" s="22"/>
       <c r="E24" s="22"/>
@@ -5450,7 +5445,7 @@
       <c r="A25" s="60" t="s">
         <v>92</v>
       </c>
-      <c r="B25" s="92"/>
+      <c r="B25" s="90"/>
       <c r="C25" s="22"/>
       <c r="D25" s="22"/>
       <c r="E25" s="22"/>
@@ -5594,7 +5589,7 @@
       <c r="A26" s="62" t="s">
         <v>93</v>
       </c>
-      <c r="B26" s="93" t="s">
+      <c r="B26" s="91" t="s">
         <v>58</v>
       </c>
       <c r="C26" s="22"/>
@@ -5728,7 +5723,7 @@
       <c r="A27" s="65" t="s">
         <v>95</v>
       </c>
-      <c r="B27" s="93"/>
+      <c r="B27" s="91"/>
       <c r="C27" s="22"/>
       <c r="D27" s="22"/>
       <c r="E27" s="22"/>
@@ -5868,7 +5863,7 @@
       <c r="A28" s="68" t="s">
         <v>97</v>
       </c>
-      <c r="B28" s="93"/>
+      <c r="B28" s="91"/>
       <c r="C28" s="22"/>
       <c r="D28" s="22"/>
       <c r="E28" s="22"/>
@@ -6000,7 +5995,7 @@
       <c r="A29" s="71" t="s">
         <v>99</v>
       </c>
-      <c r="B29" s="93"/>
+      <c r="B29" s="91"/>
       <c r="C29" s="22"/>
       <c r="D29" s="22"/>
       <c r="E29" s="22"/>
@@ -6128,7 +6123,7 @@
       <c r="A30" s="74" t="s">
         <v>100</v>
       </c>
-      <c r="B30" s="93"/>
+      <c r="B30" s="91"/>
       <c r="C30" s="22"/>
       <c r="D30" s="22"/>
       <c r="E30" s="22"/>
@@ -6254,7 +6249,7 @@
       <c r="A31" s="62" t="s">
         <v>101</v>
       </c>
-      <c r="B31" s="93"/>
+      <c r="B31" s="91"/>
       <c r="C31" s="22"/>
       <c r="D31" s="22"/>
       <c r="E31" s="22"/>
@@ -7345,11 +7340,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CR39"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:CR7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="CS1" sqref="CS1:GO1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -7371,533 +7366,533 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A1" s="99" t="s">
+      <c r="A1" s="101" t="s">
         <v>102</v>
       </c>
-      <c r="B1" s="89" t="s">
+      <c r="B1" s="88" t="s">
         <v>103</v>
       </c>
-      <c r="C1" s="90">
+      <c r="C1" s="89">
         <v>14</v>
       </c>
-      <c r="D1" s="90">
+      <c r="D1" s="89">
         <v>15</v>
       </c>
-      <c r="E1" s="90">
+      <c r="E1" s="89">
         <v>16</v>
       </c>
-      <c r="F1" s="90">
+      <c r="F1" s="89">
         <v>17</v>
       </c>
-      <c r="G1" s="90">
+      <c r="G1" s="89">
         <v>18</v>
       </c>
-      <c r="H1" s="90">
+      <c r="H1" s="89">
         <v>19</v>
       </c>
-      <c r="I1" s="90">
+      <c r="I1" s="89">
         <v>20</v>
       </c>
-      <c r="J1" s="90">
+      <c r="J1" s="89">
         <v>21</v>
       </c>
-      <c r="K1" s="90">
+      <c r="K1" s="89">
         <v>22</v>
       </c>
-      <c r="L1" s="90">
+      <c r="L1" s="89">
         <v>23</v>
       </c>
-      <c r="M1" s="90">
+      <c r="M1" s="89">
         <v>24</v>
       </c>
-      <c r="N1" s="90">
+      <c r="N1" s="89">
         <v>25</v>
       </c>
-      <c r="O1" s="90">
+      <c r="O1" s="89">
         <v>26</v>
       </c>
-      <c r="P1" s="90">
+      <c r="P1" s="89">
         <v>27</v>
       </c>
-      <c r="Q1" s="90">
+      <c r="Q1" s="89">
         <v>28</v>
       </c>
-      <c r="R1" s="90">
+      <c r="R1" s="89">
         <v>29</v>
       </c>
-      <c r="S1" s="90">
+      <c r="S1" s="89">
         <v>30</v>
       </c>
-      <c r="T1" s="90">
+      <c r="T1" s="89">
         <v>31</v>
       </c>
-      <c r="U1" s="90">
+      <c r="U1" s="89">
         <v>32</v>
       </c>
-      <c r="V1" s="90">
+      <c r="V1" s="89">
         <v>33</v>
       </c>
-      <c r="W1" s="90">
+      <c r="W1" s="89">
         <v>34</v>
       </c>
-      <c r="X1" s="90">
+      <c r="X1" s="89">
         <v>35</v>
       </c>
-      <c r="Y1" s="90">
+      <c r="Y1" s="89">
         <v>36</v>
       </c>
-      <c r="Z1" s="90">
+      <c r="Z1" s="89">
         <v>37</v>
       </c>
-      <c r="AA1" s="90">
+      <c r="AA1" s="89">
         <v>38</v>
       </c>
-      <c r="AB1" s="90">
+      <c r="AB1" s="89">
         <v>39</v>
       </c>
-      <c r="AC1" s="90">
+      <c r="AC1" s="89">
         <v>40</v>
       </c>
-      <c r="AD1" s="90">
+      <c r="AD1" s="89">
         <v>41</v>
       </c>
-      <c r="AE1" s="90">
+      <c r="AE1" s="89">
         <v>42</v>
       </c>
-      <c r="AF1" s="90">
+      <c r="AF1" s="89">
         <v>43</v>
       </c>
-      <c r="AG1" s="90">
+      <c r="AG1" s="89">
         <v>44</v>
       </c>
-      <c r="AH1" s="90">
+      <c r="AH1" s="89">
         <v>45</v>
       </c>
-      <c r="AI1" s="90">
+      <c r="AI1" s="89">
         <v>46</v>
       </c>
-      <c r="AJ1" s="90">
+      <c r="AJ1" s="89">
         <v>47</v>
       </c>
-      <c r="AK1" s="90">
+      <c r="AK1" s="89">
         <v>48</v>
       </c>
-      <c r="AL1" s="90">
+      <c r="AL1" s="89">
         <v>49</v>
       </c>
-      <c r="AM1" s="90">
+      <c r="AM1" s="89">
         <v>50</v>
       </c>
-      <c r="AN1" s="90">
+      <c r="AN1" s="89">
         <v>51</v>
       </c>
-      <c r="AO1" s="90">
+      <c r="AO1" s="89">
         <v>52</v>
       </c>
-      <c r="AP1" s="90">
+      <c r="AP1" s="89">
         <v>53</v>
       </c>
-      <c r="AQ1" s="90">
+      <c r="AQ1" s="89">
         <v>54</v>
       </c>
-      <c r="AR1" s="90">
+      <c r="AR1" s="89">
         <v>55</v>
       </c>
-      <c r="AS1" s="90">
+      <c r="AS1" s="89">
         <v>56</v>
       </c>
-      <c r="AT1" s="90">
+      <c r="AT1" s="89">
         <v>57</v>
       </c>
-      <c r="AU1" s="90">
+      <c r="AU1" s="89">
         <v>58</v>
       </c>
       <c r="AV1" s="82"/>
       <c r="AW1" s="82"/>
-      <c r="AX1" s="90">
+      <c r="AX1" s="89">
         <v>59</v>
       </c>
-      <c r="AY1" s="90">
+      <c r="AY1" s="89">
         <v>60</v>
       </c>
-      <c r="AZ1" s="90">
+      <c r="AZ1" s="89">
         <v>61</v>
       </c>
-      <c r="BA1" s="90">
+      <c r="BA1" s="89">
         <v>62</v>
       </c>
-      <c r="BB1" s="90">
+      <c r="BB1" s="89">
         <v>63</v>
       </c>
-      <c r="BC1" s="90">
+      <c r="BC1" s="89">
         <v>64</v>
       </c>
-      <c r="BD1" s="90">
+      <c r="BD1" s="89">
         <v>65</v>
       </c>
-      <c r="BE1" s="90">
+      <c r="BE1" s="89">
         <v>66</v>
       </c>
-      <c r="BF1" s="90">
+      <c r="BF1" s="89">
         <v>67</v>
       </c>
-      <c r="BG1" s="90">
+      <c r="BG1" s="89">
         <v>68</v>
       </c>
-      <c r="BH1" s="90">
+      <c r="BH1" s="89">
         <v>69</v>
       </c>
-      <c r="BI1" s="90">
+      <c r="BI1" s="89">
         <v>70</v>
       </c>
-      <c r="BJ1" s="90">
+      <c r="BJ1" s="89">
         <v>71</v>
       </c>
-      <c r="BK1" s="90">
+      <c r="BK1" s="89">
         <v>72</v>
       </c>
-      <c r="BL1" s="90">
+      <c r="BL1" s="89">
         <v>73</v>
       </c>
-      <c r="BM1" s="90">
+      <c r="BM1" s="89">
         <v>74</v>
       </c>
-      <c r="BN1" s="90">
+      <c r="BN1" s="89">
         <v>75</v>
       </c>
-      <c r="BO1" s="90">
+      <c r="BO1" s="89">
         <v>76</v>
       </c>
-      <c r="BP1" s="90">
+      <c r="BP1" s="89">
         <v>77</v>
       </c>
-      <c r="BQ1" s="90">
+      <c r="BQ1" s="89">
         <v>78</v>
       </c>
-      <c r="BR1" s="90">
+      <c r="BR1" s="89">
         <v>79</v>
       </c>
-      <c r="BS1" s="90">
+      <c r="BS1" s="89">
         <v>80</v>
       </c>
       <c r="BT1" s="82"/>
-      <c r="BU1" s="90">
+      <c r="BU1" s="89">
         <v>81</v>
       </c>
-      <c r="BV1" s="90">
+      <c r="BV1" s="89">
         <v>82</v>
       </c>
       <c r="BW1" s="82"/>
-      <c r="BX1" s="90">
+      <c r="BX1" s="89">
         <v>83</v>
       </c>
-      <c r="BY1" s="90">
+      <c r="BY1" s="89">
         <v>84</v>
       </c>
-      <c r="BZ1" s="90">
+      <c r="BZ1" s="89">
         <v>85</v>
       </c>
-      <c r="CA1" s="90">
+      <c r="CA1" s="89">
         <v>86</v>
       </c>
-      <c r="CB1" s="90">
+      <c r="CB1" s="89">
         <v>87</v>
       </c>
-      <c r="CC1" s="90">
+      <c r="CC1" s="89">
         <v>88</v>
       </c>
-      <c r="CD1" s="90">
+      <c r="CD1" s="89">
         <v>89</v>
       </c>
-      <c r="CE1" s="90">
+      <c r="CE1" s="89">
         <v>90</v>
       </c>
-      <c r="CF1" s="90">
+      <c r="CF1" s="89">
         <v>91</v>
       </c>
-      <c r="CG1" s="90">
+      <c r="CG1" s="89">
         <v>92</v>
       </c>
-      <c r="CH1" s="90">
+      <c r="CH1" s="89">
         <v>93</v>
       </c>
-      <c r="CI1" s="90">
+      <c r="CI1" s="89">
         <v>94</v>
       </c>
-      <c r="CJ1" s="90">
+      <c r="CJ1" s="89">
         <v>95</v>
       </c>
-      <c r="CK1" s="90">
+      <c r="CK1" s="89">
         <v>96</v>
       </c>
-      <c r="CL1" s="90">
+      <c r="CL1" s="89">
         <v>97</v>
       </c>
-      <c r="CM1" s="90">
+      <c r="CM1" s="89">
         <v>98</v>
       </c>
-      <c r="CN1" s="90">
+      <c r="CN1" s="89">
         <v>99</v>
       </c>
       <c r="CO1" s="83"/>
-      <c r="CP1" s="90">
+      <c r="CP1" s="89">
         <v>100</v>
       </c>
-      <c r="CQ1" s="90">
+      <c r="CQ1" s="89">
         <v>101</v>
       </c>
-      <c r="CR1" s="90">
+      <c r="CR1" s="89">
         <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:96" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="100"/>
-      <c r="B2" s="89" t="s">
+      <c r="A2" s="102"/>
+      <c r="B2" s="88" t="s">
         <v>104</v>
       </c>
-      <c r="C2" s="102" t="s">
+      <c r="C2" s="100" t="s">
         <v>105</v>
       </c>
-      <c r="D2" s="102"/>
-      <c r="E2" s="102"/>
-      <c r="F2" s="102"/>
-      <c r="G2" s="102"/>
-      <c r="H2" s="102"/>
-      <c r="I2" s="102"/>
-      <c r="J2" s="102"/>
-      <c r="K2" s="102"/>
-      <c r="L2" s="102"/>
-      <c r="M2" s="102"/>
-      <c r="N2" s="102"/>
-      <c r="O2" s="102"/>
-      <c r="P2" s="102"/>
-      <c r="Q2" s="102"/>
-      <c r="R2" s="102" t="s">
+      <c r="D2" s="100"/>
+      <c r="E2" s="100"/>
+      <c r="F2" s="100"/>
+      <c r="G2" s="100"/>
+      <c r="H2" s="100"/>
+      <c r="I2" s="100"/>
+      <c r="J2" s="100"/>
+      <c r="K2" s="100"/>
+      <c r="L2" s="100"/>
+      <c r="M2" s="100"/>
+      <c r="N2" s="100"/>
+      <c r="O2" s="100"/>
+      <c r="P2" s="100"/>
+      <c r="Q2" s="100"/>
+      <c r="R2" s="100" t="s">
         <v>106</v>
       </c>
-      <c r="S2" s="102"/>
-      <c r="T2" s="102"/>
-      <c r="U2" s="102"/>
-      <c r="V2" s="102"/>
-      <c r="W2" s="102"/>
-      <c r="X2" s="102"/>
-      <c r="Y2" s="102"/>
-      <c r="Z2" s="102"/>
-      <c r="AA2" s="102"/>
-      <c r="AB2" s="102"/>
-      <c r="AC2" s="102"/>
-      <c r="AD2" s="102"/>
-      <c r="AE2" s="102"/>
-      <c r="AF2" s="102"/>
-      <c r="AG2" s="102"/>
-      <c r="AH2" s="102"/>
-      <c r="AI2" s="102"/>
-      <c r="AJ2" s="102"/>
-      <c r="AK2" s="102"/>
-      <c r="AL2" s="102"/>
-      <c r="AM2" s="102" t="s">
+      <c r="S2" s="100"/>
+      <c r="T2" s="100"/>
+      <c r="U2" s="100"/>
+      <c r="V2" s="100"/>
+      <c r="W2" s="100"/>
+      <c r="X2" s="100"/>
+      <c r="Y2" s="100"/>
+      <c r="Z2" s="100"/>
+      <c r="AA2" s="100"/>
+      <c r="AB2" s="100"/>
+      <c r="AC2" s="100"/>
+      <c r="AD2" s="100"/>
+      <c r="AE2" s="100"/>
+      <c r="AF2" s="100"/>
+      <c r="AG2" s="100"/>
+      <c r="AH2" s="100"/>
+      <c r="AI2" s="100"/>
+      <c r="AJ2" s="100"/>
+      <c r="AK2" s="100"/>
+      <c r="AL2" s="100"/>
+      <c r="AM2" s="100" t="s">
         <v>107</v>
       </c>
-      <c r="AN2" s="102"/>
-      <c r="AO2" s="102"/>
-      <c r="AP2" s="102"/>
-      <c r="AQ2" s="102"/>
-      <c r="AR2" s="102"/>
-      <c r="AS2" s="102"/>
-      <c r="AT2" s="102"/>
-      <c r="AU2" s="102"/>
-      <c r="AV2" s="102"/>
-      <c r="AW2" s="102"/>
-      <c r="AX2" s="102"/>
-      <c r="AY2" s="102"/>
-      <c r="AZ2" s="102"/>
-      <c r="BA2" s="102"/>
-      <c r="BB2" s="102"/>
-      <c r="BC2" s="102"/>
-      <c r="BD2" s="102"/>
-      <c r="BE2" s="102"/>
-      <c r="BF2" s="102"/>
-      <c r="BG2" s="102"/>
-      <c r="BH2" s="102"/>
-      <c r="BI2" s="102"/>
-      <c r="BJ2" s="102" t="s">
+      <c r="AN2" s="100"/>
+      <c r="AO2" s="100"/>
+      <c r="AP2" s="100"/>
+      <c r="AQ2" s="100"/>
+      <c r="AR2" s="100"/>
+      <c r="AS2" s="100"/>
+      <c r="AT2" s="100"/>
+      <c r="AU2" s="100"/>
+      <c r="AV2" s="100"/>
+      <c r="AW2" s="100"/>
+      <c r="AX2" s="100"/>
+      <c r="AY2" s="100"/>
+      <c r="AZ2" s="100"/>
+      <c r="BA2" s="100"/>
+      <c r="BB2" s="100"/>
+      <c r="BC2" s="100"/>
+      <c r="BD2" s="100"/>
+      <c r="BE2" s="100"/>
+      <c r="BF2" s="100"/>
+      <c r="BG2" s="100"/>
+      <c r="BH2" s="100"/>
+      <c r="BI2" s="100"/>
+      <c r="BJ2" s="100" t="s">
         <v>108</v>
       </c>
-      <c r="BK2" s="102"/>
-      <c r="BL2" s="102"/>
-      <c r="BM2" s="102"/>
-      <c r="BN2" s="102"/>
-      <c r="BO2" s="102"/>
-      <c r="BP2" s="102"/>
-      <c r="BQ2" s="102"/>
-      <c r="BR2" s="102"/>
-      <c r="BS2" s="102"/>
-      <c r="BT2" s="102"/>
-      <c r="BU2" s="102"/>
-      <c r="BV2" s="102"/>
-      <c r="BW2" s="102"/>
-      <c r="BX2" s="102"/>
-      <c r="BY2" s="102"/>
-      <c r="BZ2" s="102"/>
-      <c r="CA2" s="102"/>
-      <c r="CB2" s="102"/>
-      <c r="CC2" s="102"/>
-      <c r="CD2" s="102"/>
-      <c r="CE2" s="102" t="s">
+      <c r="BK2" s="100"/>
+      <c r="BL2" s="100"/>
+      <c r="BM2" s="100"/>
+      <c r="BN2" s="100"/>
+      <c r="BO2" s="100"/>
+      <c r="BP2" s="100"/>
+      <c r="BQ2" s="100"/>
+      <c r="BR2" s="100"/>
+      <c r="BS2" s="100"/>
+      <c r="BT2" s="100"/>
+      <c r="BU2" s="100"/>
+      <c r="BV2" s="100"/>
+      <c r="BW2" s="100"/>
+      <c r="BX2" s="100"/>
+      <c r="BY2" s="100"/>
+      <c r="BZ2" s="100"/>
+      <c r="CA2" s="100"/>
+      <c r="CB2" s="100"/>
+      <c r="CC2" s="100"/>
+      <c r="CD2" s="100"/>
+      <c r="CE2" s="100" t="s">
         <v>109</v>
       </c>
-      <c r="CF2" s="102"/>
-      <c r="CG2" s="102"/>
-      <c r="CH2" s="102"/>
-      <c r="CI2" s="102"/>
-      <c r="CJ2" s="102"/>
-      <c r="CK2" s="102"/>
-      <c r="CL2" s="102"/>
-      <c r="CM2" s="102"/>
-      <c r="CN2" s="102"/>
-      <c r="CO2" s="102"/>
-      <c r="CP2" s="102"/>
-      <c r="CQ2" s="102"/>
-      <c r="CR2" s="102"/>
+      <c r="CF2" s="100"/>
+      <c r="CG2" s="100"/>
+      <c r="CH2" s="100"/>
+      <c r="CI2" s="100"/>
+      <c r="CJ2" s="100"/>
+      <c r="CK2" s="100"/>
+      <c r="CL2" s="100"/>
+      <c r="CM2" s="100"/>
+      <c r="CN2" s="100"/>
+      <c r="CO2" s="100"/>
+      <c r="CP2" s="100"/>
+      <c r="CQ2" s="100"/>
+      <c r="CR2" s="100"/>
     </row>
     <row r="3" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A3" s="101"/>
-      <c r="B3" s="89" t="s">
+      <c r="A3" s="103"/>
+      <c r="B3" s="88" t="s">
         <v>110</v>
       </c>
-      <c r="C3" s="90">
+      <c r="C3" s="89">
         <v>12</v>
       </c>
-      <c r="D3" s="90">
+      <c r="D3" s="89">
         <v>13</v>
       </c>
-      <c r="E3" s="90">
+      <c r="E3" s="89">
         <v>14</v>
       </c>
-      <c r="F3" s="90">
+      <c r="F3" s="89">
         <v>15</v>
       </c>
-      <c r="G3" s="90">
+      <c r="G3" s="89">
         <v>16</v>
       </c>
-      <c r="H3" s="90">
+      <c r="H3" s="89">
         <v>19</v>
       </c>
-      <c r="I3" s="90">
+      <c r="I3" s="89">
         <v>20</v>
       </c>
-      <c r="J3" s="90">
+      <c r="J3" s="89">
         <v>21</v>
       </c>
-      <c r="K3" s="90">
+      <c r="K3" s="89">
         <v>22</v>
       </c>
-      <c r="L3" s="90">
+      <c r="L3" s="89">
         <v>23</v>
       </c>
-      <c r="M3" s="90">
+      <c r="M3" s="89">
         <v>26</v>
       </c>
-      <c r="N3" s="90">
+      <c r="N3" s="89">
         <v>27</v>
       </c>
-      <c r="O3" s="90">
+      <c r="O3" s="89">
         <v>28</v>
       </c>
-      <c r="P3" s="90">
+      <c r="P3" s="89">
         <v>29</v>
       </c>
-      <c r="Q3" s="90">
+      <c r="Q3" s="89">
         <v>30</v>
       </c>
-      <c r="R3" s="90">
+      <c r="R3" s="89">
         <v>2</v>
       </c>
-      <c r="S3" s="90">
+      <c r="S3" s="89">
         <v>3</v>
       </c>
-      <c r="T3" s="90">
+      <c r="T3" s="89">
         <v>4</v>
       </c>
-      <c r="U3" s="90">
+      <c r="U3" s="89">
         <v>5</v>
       </c>
-      <c r="V3" s="90">
+      <c r="V3" s="89">
         <v>6</v>
       </c>
-      <c r="W3" s="90">
+      <c r="W3" s="89">
         <v>9</v>
       </c>
-      <c r="X3" s="90">
+      <c r="X3" s="89">
         <v>10</v>
       </c>
-      <c r="Y3" s="90">
+      <c r="Y3" s="89">
         <v>11</v>
       </c>
-      <c r="Z3" s="90">
+      <c r="Z3" s="89">
         <v>12</v>
       </c>
-      <c r="AA3" s="90">
+      <c r="AA3" s="89">
         <v>13</v>
       </c>
-      <c r="AB3" s="90">
+      <c r="AB3" s="89">
         <v>16</v>
       </c>
-      <c r="AC3" s="90">
+      <c r="AC3" s="89">
         <v>17</v>
       </c>
-      <c r="AD3" s="90">
+      <c r="AD3" s="89">
         <v>18</v>
       </c>
-      <c r="AE3" s="90">
+      <c r="AE3" s="89">
         <v>19</v>
       </c>
-      <c r="AF3" s="90">
+      <c r="AF3" s="89">
         <v>20</v>
       </c>
-      <c r="AG3" s="90">
+      <c r="AG3" s="89">
         <v>23</v>
       </c>
-      <c r="AH3" s="90">
+      <c r="AH3" s="89">
         <v>24</v>
       </c>
-      <c r="AI3" s="90">
+      <c r="AI3" s="89">
         <v>25</v>
       </c>
-      <c r="AJ3" s="90">
+      <c r="AJ3" s="89">
         <v>26</v>
       </c>
-      <c r="AK3" s="90">
+      <c r="AK3" s="89">
         <v>27</v>
       </c>
-      <c r="AL3" s="90">
+      <c r="AL3" s="89">
         <v>30</v>
       </c>
-      <c r="AM3" s="90">
+      <c r="AM3" s="89">
         <v>1</v>
       </c>
-      <c r="AN3" s="90">
+      <c r="AN3" s="89">
         <v>2</v>
       </c>
-      <c r="AO3" s="90">
+      <c r="AO3" s="89">
         <v>3</v>
       </c>
-      <c r="AP3" s="90">
+      <c r="AP3" s="89">
         <v>4</v>
       </c>
-      <c r="AQ3" s="90">
+      <c r="AQ3" s="89">
         <v>7</v>
       </c>
-      <c r="AR3" s="90">
+      <c r="AR3" s="89">
         <v>8</v>
       </c>
-      <c r="AS3" s="90">
+      <c r="AS3" s="89">
         <v>9</v>
       </c>
-      <c r="AT3" s="90">
+      <c r="AT3" s="89">
         <v>10</v>
       </c>
-      <c r="AU3" s="90">
+      <c r="AU3" s="89">
         <v>11</v>
       </c>
       <c r="AV3" s="83">
@@ -7906,487 +7901,311 @@
       <c r="AW3" s="83">
         <v>15</v>
       </c>
-      <c r="AX3" s="90">
+      <c r="AX3" s="89">
         <v>16</v>
       </c>
-      <c r="AY3" s="90">
+      <c r="AY3" s="89">
         <v>17</v>
       </c>
-      <c r="AZ3" s="90">
+      <c r="AZ3" s="89">
         <v>18</v>
       </c>
-      <c r="BA3" s="90">
+      <c r="BA3" s="89">
         <v>21</v>
       </c>
-      <c r="BB3" s="90">
+      <c r="BB3" s="89">
         <v>22</v>
       </c>
-      <c r="BC3" s="90">
+      <c r="BC3" s="89">
         <v>23</v>
       </c>
-      <c r="BD3" s="90">
+      <c r="BD3" s="89">
         <v>24</v>
       </c>
-      <c r="BE3" s="90">
+      <c r="BE3" s="89">
         <v>25</v>
       </c>
-      <c r="BF3" s="90">
+      <c r="BF3" s="89">
         <v>28</v>
       </c>
-      <c r="BG3" s="90">
+      <c r="BG3" s="89">
         <v>29</v>
       </c>
-      <c r="BH3" s="90">
+      <c r="BH3" s="89">
         <v>30</v>
       </c>
-      <c r="BI3" s="90">
+      <c r="BI3" s="89">
         <v>31</v>
       </c>
-      <c r="BJ3" s="90">
+      <c r="BJ3" s="89">
         <v>1</v>
       </c>
-      <c r="BK3" s="90">
+      <c r="BK3" s="89">
         <v>4</v>
       </c>
-      <c r="BL3" s="90">
+      <c r="BL3" s="89">
         <v>5</v>
       </c>
-      <c r="BM3" s="90">
+      <c r="BM3" s="89">
         <v>6</v>
       </c>
-      <c r="BN3" s="90">
+      <c r="BN3" s="89">
         <v>7</v>
       </c>
-      <c r="BO3" s="90">
+      <c r="BO3" s="89">
         <v>8</v>
       </c>
-      <c r="BP3" s="90">
+      <c r="BP3" s="89">
         <v>11</v>
       </c>
-      <c r="BQ3" s="90">
+      <c r="BQ3" s="89">
         <v>12</v>
       </c>
-      <c r="BR3" s="90">
+      <c r="BR3" s="89">
         <v>13</v>
       </c>
-      <c r="BS3" s="90">
+      <c r="BS3" s="89">
         <v>14</v>
       </c>
       <c r="BT3" s="83">
         <v>15</v>
       </c>
-      <c r="BU3" s="90">
+      <c r="BU3" s="89">
         <v>18</v>
       </c>
-      <c r="BV3" s="90">
+      <c r="BV3" s="89">
         <v>19</v>
       </c>
       <c r="BW3" s="83">
         <v>20</v>
       </c>
-      <c r="BX3" s="90">
+      <c r="BX3" s="89">
         <v>21</v>
       </c>
-      <c r="BY3" s="90">
+      <c r="BY3" s="89">
         <v>22</v>
       </c>
-      <c r="BZ3" s="90">
+      <c r="BZ3" s="89">
         <v>25</v>
       </c>
-      <c r="CA3" s="90">
+      <c r="CA3" s="89">
         <v>26</v>
       </c>
-      <c r="CB3" s="90">
+      <c r="CB3" s="89">
         <v>27</v>
       </c>
-      <c r="CC3" s="90">
+      <c r="CC3" s="89">
         <v>28</v>
       </c>
-      <c r="CD3" s="90">
+      <c r="CD3" s="89">
         <v>29</v>
       </c>
-      <c r="CE3" s="90">
+      <c r="CE3" s="89">
         <v>2</v>
       </c>
-      <c r="CF3" s="90">
+      <c r="CF3" s="89">
         <v>3</v>
       </c>
-      <c r="CG3" s="90">
+      <c r="CG3" s="89">
         <v>4</v>
       </c>
-      <c r="CH3" s="90">
+      <c r="CH3" s="89">
         <v>5</v>
       </c>
-      <c r="CI3" s="90">
+      <c r="CI3" s="89">
         <v>6</v>
       </c>
-      <c r="CJ3" s="90">
+      <c r="CJ3" s="89">
         <v>9</v>
       </c>
-      <c r="CK3" s="90">
+      <c r="CK3" s="89">
         <v>10</v>
       </c>
-      <c r="CL3" s="90">
+      <c r="CL3" s="89">
         <v>11</v>
       </c>
-      <c r="CM3" s="90">
+      <c r="CM3" s="89">
         <v>12</v>
       </c>
-      <c r="CN3" s="90">
+      <c r="CN3" s="89">
         <v>13</v>
       </c>
       <c r="CO3" s="83">
         <v>14</v>
       </c>
-      <c r="CP3" s="88">
+      <c r="CP3" s="87">
         <v>16</v>
       </c>
-      <c r="CQ3" s="88">
+      <c r="CQ3" s="87">
         <v>17</v>
       </c>
-      <c r="CR3" s="88">
+      <c r="CR3" s="87">
         <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="104" t="s">
+      <c r="A4" s="97" t="s">
         <v>111</v>
       </c>
-      <c r="B4" s="105"/>
-      <c r="C4" s="87" t="s">
+      <c r="B4" s="98"/>
+      <c r="C4" s="86" t="s">
         <v>118</v>
       </c>
-      <c r="D4" s="87" t="s">
+      <c r="D4" s="86" t="s">
         <v>122</v>
       </c>
-      <c r="E4" s="87" t="s">
+      <c r="E4" s="86" t="s">
         <v>123</v>
       </c>
-      <c r="F4" s="87" t="s">
+      <c r="F4" s="86" t="s">
         <v>128</v>
       </c>
-      <c r="G4" s="87"/>
-      <c r="H4" s="87"/>
-      <c r="I4" s="87"/>
-      <c r="J4" s="87"/>
-      <c r="K4" s="87"/>
-      <c r="L4" s="87"/>
-      <c r="M4" s="87"/>
-      <c r="N4" s="87"/>
+      <c r="G4" s="86"/>
+      <c r="H4" s="86"/>
+      <c r="I4" s="86"/>
+      <c r="J4" s="86"/>
+      <c r="K4" s="86"/>
+      <c r="L4" s="86"/>
+      <c r="M4" s="86"/>
+      <c r="N4" s="86"/>
       <c r="O4" s="85"/>
       <c r="P4" s="85"/>
       <c r="Q4" s="85"/>
-      <c r="AV4" s="103" t="s">
+      <c r="AV4" s="99" t="s">
         <v>112</v>
       </c>
-      <c r="AW4" s="103" t="s">
+      <c r="AW4" s="99" t="s">
         <v>112</v>
       </c>
-      <c r="BT4" s="103" t="s">
+      <c r="BT4" s="99" t="s">
         <v>113</v>
       </c>
-      <c r="BW4" s="103" t="s">
+      <c r="BW4" s="99" t="s">
         <v>114</v>
       </c>
-      <c r="CO4" s="103" t="s">
+      <c r="CO4" s="99" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="104" t="s">
+      <c r="A5" s="97" t="s">
         <v>115</v>
       </c>
-      <c r="B5" s="105"/>
-      <c r="C5" s="87" t="s">
+      <c r="B5" s="98"/>
+      <c r="C5" s="86" t="s">
         <v>118</v>
       </c>
-      <c r="D5" s="87" t="s">
+      <c r="D5" s="86" t="s">
         <v>119</v>
       </c>
-      <c r="E5" s="87" t="s">
+      <c r="E5" s="86" t="s">
         <v>124</v>
       </c>
-      <c r="F5" s="87" t="s">
+      <c r="F5" s="86" t="s">
         <v>129</v>
       </c>
-      <c r="G5" s="87"/>
-      <c r="H5" s="87"/>
-      <c r="I5" s="87"/>
-      <c r="J5" s="87"/>
-      <c r="K5" s="87"/>
-      <c r="L5" s="87"/>
-      <c r="M5" s="87"/>
-      <c r="N5" s="87"/>
+      <c r="G5" s="86"/>
+      <c r="H5" s="86"/>
+      <c r="I5" s="86"/>
+      <c r="J5" s="86"/>
+      <c r="K5" s="86"/>
+      <c r="L5" s="86"/>
+      <c r="M5" s="86"/>
+      <c r="N5" s="86"/>
       <c r="O5" s="85"/>
       <c r="P5" s="85"/>
       <c r="Q5" s="85"/>
-      <c r="AV5" s="103"/>
-      <c r="AW5" s="103"/>
-      <c r="BT5" s="103"/>
-      <c r="BW5" s="103"/>
-      <c r="CO5" s="103"/>
+      <c r="AV5" s="99"/>
+      <c r="AW5" s="99"/>
+      <c r="BT5" s="99"/>
+      <c r="BW5" s="99"/>
+      <c r="CO5" s="99"/>
     </row>
     <row r="6" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="104" t="s">
+      <c r="A6" s="97" t="s">
         <v>116</v>
       </c>
-      <c r="B6" s="105"/>
-      <c r="C6" s="87" t="s">
+      <c r="B6" s="98"/>
+      <c r="C6" s="86" t="s">
         <v>118</v>
       </c>
-      <c r="D6" s="87" t="s">
+      <c r="D6" s="86" t="s">
         <v>120</v>
       </c>
-      <c r="E6" s="87" t="s">
+      <c r="E6" s="86" t="s">
         <v>125</v>
       </c>
-      <c r="F6" s="87" t="s">
+      <c r="F6" s="86" t="s">
         <v>130</v>
       </c>
-      <c r="G6" s="87"/>
-      <c r="H6" s="87"/>
-      <c r="I6" s="87"/>
-      <c r="J6" s="87"/>
-      <c r="K6" s="87"/>
-      <c r="L6" s="87"/>
-      <c r="M6" s="87"/>
-      <c r="N6" s="87"/>
+      <c r="G6" s="86"/>
+      <c r="H6" s="86"/>
+      <c r="I6" s="86"/>
+      <c r="J6" s="86"/>
+      <c r="K6" s="86"/>
+      <c r="L6" s="86"/>
+      <c r="M6" s="86"/>
+      <c r="N6" s="86"/>
       <c r="O6" s="85"/>
       <c r="P6" s="85"/>
       <c r="Q6" s="85"/>
-      <c r="AV6" s="103"/>
-      <c r="AW6" s="103"/>
-      <c r="BT6" s="103"/>
-      <c r="BW6" s="103"/>
-      <c r="CO6" s="103"/>
+      <c r="AV6" s="99"/>
+      <c r="AW6" s="99"/>
+      <c r="BT6" s="99"/>
+      <c r="BW6" s="99"/>
+      <c r="CO6" s="99"/>
     </row>
     <row r="7" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="104" t="s">
+      <c r="A7" s="97" t="s">
         <v>117</v>
       </c>
-      <c r="B7" s="105"/>
-      <c r="C7" s="87" t="s">
+      <c r="B7" s="98"/>
+      <c r="C7" s="86" t="s">
         <v>118</v>
       </c>
-      <c r="D7" s="87" t="s">
+      <c r="D7" s="86" t="s">
         <v>121</v>
       </c>
-      <c r="E7" s="87" t="s">
+      <c r="E7" s="86" t="s">
         <v>126</v>
       </c>
-      <c r="F7" s="87" t="s">
+      <c r="F7" s="86" t="s">
         <v>131</v>
       </c>
-      <c r="G7" s="87"/>
-      <c r="H7" s="87"/>
-      <c r="I7" s="87"/>
-      <c r="J7" s="87"/>
-      <c r="K7" s="87"/>
-      <c r="L7" s="87"/>
-      <c r="M7" s="87"/>
-      <c r="N7" s="87"/>
+      <c r="G7" s="86"/>
+      <c r="H7" s="86"/>
+      <c r="I7" s="86"/>
+      <c r="J7" s="86"/>
+      <c r="K7" s="86"/>
+      <c r="L7" s="86"/>
+      <c r="M7" s="86"/>
+      <c r="N7" s="86"/>
       <c r="O7" s="85"/>
       <c r="P7" s="85"/>
       <c r="Q7" s="85"/>
-      <c r="AV7" s="103"/>
-      <c r="AW7" s="103"/>
-      <c r="BT7" s="103"/>
-      <c r="BW7" s="103"/>
-      <c r="CO7" s="103"/>
-    </row>
-    <row r="8" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="AV8" s="91"/>
-      <c r="AW8" s="91"/>
-      <c r="BT8" s="91"/>
-      <c r="BW8" s="91"/>
-      <c r="CO8" s="91"/>
-    </row>
-    <row r="9" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="AV9" s="91"/>
-      <c r="AW9" s="91"/>
-      <c r="BT9" s="91"/>
-      <c r="BW9" s="91"/>
-      <c r="CO9" s="91"/>
-    </row>
-    <row r="10" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="AV10" s="91"/>
-      <c r="AW10" s="91"/>
-      <c r="BT10" s="91"/>
-      <c r="BW10" s="91"/>
-      <c r="CO10" s="91"/>
-    </row>
-    <row r="11" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="AV11" s="91"/>
-      <c r="AW11" s="91"/>
-      <c r="BT11" s="91"/>
-      <c r="BW11" s="91"/>
-      <c r="CO11" s="91"/>
-    </row>
-    <row r="12" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="AV12" s="91"/>
-      <c r="AW12" s="91"/>
-      <c r="BT12" s="91"/>
-      <c r="BW12" s="91"/>
-      <c r="CO12" s="91"/>
-    </row>
-    <row r="13" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="AV13" s="91"/>
-      <c r="AW13" s="91"/>
-      <c r="BT13" s="91"/>
-      <c r="BW13" s="91"/>
-      <c r="CO13" s="91"/>
-    </row>
-    <row r="14" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="AV14" s="91"/>
-      <c r="AW14" s="91"/>
-      <c r="BT14" s="91"/>
-      <c r="BW14" s="91"/>
-      <c r="CO14" s="91"/>
-    </row>
-    <row r="15" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="AV15" s="91"/>
-      <c r="AW15" s="91"/>
-      <c r="BT15" s="91"/>
-      <c r="BW15" s="91"/>
-      <c r="CO15" s="91"/>
-    </row>
-    <row r="16" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="AV16" s="91"/>
-      <c r="AW16" s="91"/>
-      <c r="BT16" s="91"/>
-      <c r="BW16" s="91"/>
-      <c r="CO16" s="91"/>
-    </row>
-    <row r="17" spans="48:93" x14ac:dyDescent="0.25">
-      <c r="AV17" s="91"/>
-      <c r="AW17" s="91"/>
-      <c r="BT17" s="91"/>
-      <c r="BW17" s="91"/>
-      <c r="CO17" s="91"/>
-    </row>
-    <row r="18" spans="48:93" x14ac:dyDescent="0.25">
-      <c r="AV18" s="91"/>
-      <c r="AW18" s="91"/>
-      <c r="BT18" s="91"/>
-      <c r="BW18" s="91"/>
-      <c r="CO18" s="91"/>
-    </row>
-    <row r="19" spans="48:93" x14ac:dyDescent="0.25">
-      <c r="AV19" s="91"/>
-      <c r="AW19" s="91"/>
-      <c r="BT19" s="91"/>
-      <c r="BW19" s="91"/>
-      <c r="CO19" s="91"/>
-    </row>
-    <row r="20" spans="48:93" x14ac:dyDescent="0.25">
-      <c r="AV20" s="91"/>
-      <c r="AW20" s="91"/>
-      <c r="BT20" s="91"/>
-      <c r="BW20" s="91"/>
-      <c r="CO20" s="91"/>
-    </row>
-    <row r="21" spans="48:93" x14ac:dyDescent="0.25">
-      <c r="AV21" s="91"/>
-      <c r="AW21" s="91"/>
-      <c r="BT21" s="91"/>
-      <c r="BW21" s="91"/>
-      <c r="CO21" s="91"/>
-    </row>
-    <row r="22" spans="48:93" x14ac:dyDescent="0.25">
-      <c r="AV22" s="91"/>
-      <c r="AW22" s="91"/>
-      <c r="BT22" s="91"/>
-      <c r="BW22" s="91"/>
-      <c r="CO22" s="91"/>
-    </row>
-    <row r="23" spans="48:93" x14ac:dyDescent="0.25">
-      <c r="AV23" s="91"/>
-      <c r="AW23" s="91"/>
-      <c r="BT23" s="91"/>
-      <c r="BW23" s="91"/>
-      <c r="CO23" s="91"/>
-    </row>
-    <row r="24" spans="48:93" x14ac:dyDescent="0.25">
-      <c r="AV24" s="91"/>
-      <c r="AW24" s="91"/>
-      <c r="BT24" s="91"/>
-      <c r="BW24" s="91"/>
-      <c r="CO24" s="91"/>
-    </row>
-    <row r="25" spans="48:93" x14ac:dyDescent="0.25">
-      <c r="AV25" s="91"/>
-      <c r="AW25" s="91"/>
-      <c r="BT25" s="91"/>
-      <c r="BW25" s="91"/>
-      <c r="CO25" s="91"/>
-    </row>
-    <row r="26" spans="48:93" x14ac:dyDescent="0.25">
-      <c r="AV26" s="91"/>
-      <c r="AW26" s="91"/>
-      <c r="BT26" s="91"/>
-      <c r="BW26" s="91"/>
-      <c r="CO26" s="91"/>
-    </row>
-    <row r="27" spans="48:93" x14ac:dyDescent="0.25">
-      <c r="AV27" s="91"/>
-      <c r="AW27" s="91"/>
-      <c r="BT27" s="91"/>
-      <c r="BW27" s="91"/>
-      <c r="CO27" s="91"/>
-    </row>
-    <row r="28" spans="48:93" x14ac:dyDescent="0.25">
-      <c r="AV28" s="86"/>
-    </row>
-    <row r="29" spans="48:93" x14ac:dyDescent="0.25">
-      <c r="AV29" s="86"/>
-    </row>
-    <row r="30" spans="48:93" x14ac:dyDescent="0.25">
-      <c r="AV30" s="86"/>
-    </row>
-    <row r="31" spans="48:93" x14ac:dyDescent="0.25">
-      <c r="AV31" s="86"/>
-    </row>
-    <row r="32" spans="48:93" x14ac:dyDescent="0.25">
-      <c r="AV32" s="86"/>
-    </row>
-    <row r="33" spans="48:48" x14ac:dyDescent="0.25">
-      <c r="AV33" s="86"/>
-    </row>
-    <row r="34" spans="48:48" x14ac:dyDescent="0.25">
-      <c r="AV34" s="86"/>
-    </row>
-    <row r="35" spans="48:48" x14ac:dyDescent="0.25">
-      <c r="AV35" s="86"/>
-    </row>
-    <row r="36" spans="48:48" x14ac:dyDescent="0.25">
-      <c r="AV36" s="86"/>
-    </row>
-    <row r="37" spans="48:48" x14ac:dyDescent="0.25">
-      <c r="AV37" s="86"/>
-    </row>
-    <row r="38" spans="48:48" x14ac:dyDescent="0.25">
-      <c r="AV38" s="86"/>
-    </row>
-    <row r="39" spans="48:48" x14ac:dyDescent="0.25">
-      <c r="AV39" s="86"/>
+      <c r="AV7" s="99"/>
+      <c r="AW7" s="99"/>
+      <c r="BT7" s="99"/>
+      <c r="BW7" s="99"/>
+      <c r="CO7" s="99"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="C2:Q2"/>
+    <mergeCell ref="R2:AL2"/>
+    <mergeCell ref="AM2:BI2"/>
+    <mergeCell ref="BJ2:CD2"/>
+    <mergeCell ref="CE2:CR2"/>
+    <mergeCell ref="AW4:AW7"/>
+    <mergeCell ref="BT4:BT7"/>
+    <mergeCell ref="BW4:BW7"/>
+    <mergeCell ref="CO4:CO7"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="AV4:AV7"/>
-    <mergeCell ref="CE2:CR2"/>
-    <mergeCell ref="AW4:AW7"/>
-    <mergeCell ref="BT4:BT7"/>
-    <mergeCell ref="BW4:BW7"/>
-    <mergeCell ref="CO4:CO7"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="C2:Q2"/>
-    <mergeCell ref="R2:AL2"/>
-    <mergeCell ref="AM2:BI2"/>
-    <mergeCell ref="BJ2:CD2"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Adiciona daily realizada no dia 19-08
</commit_message>
<xml_diff>
--- a/Cronograma/Projeto-Cronograma - Acompanhamento.xlsx
+++ b/Cronograma/Projeto-Cronograma - Acompanhamento.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Works\Cursos\senai_desenvolvimento\2s2019\2s2019-t3-mentoria\Cronograma\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\39893838843\Downloads\2s2019-t3-mentoria\Cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{449CD73E-C075-4711-BE1E-747C328E9EC0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Proj-Cronograma" sheetId="1" r:id="rId1"/>
@@ -26,12 +25,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Saulo Santos</author>
   </authors>
   <commentList>
-    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
+    <comment ref="A4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -48,7 +47,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
+    <comment ref="A5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -65,7 +64,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
+    <comment ref="A6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -83,7 +82,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
+    <comment ref="A7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -106,7 +105,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="136">
   <si>
     <t>REDES</t>
   </si>
@@ -502,12 +501,24 @@
   </si>
   <si>
     <t>Finalizaram as perguntas que serão feitas, pesquisa de mercado com sistemas semelhantes</t>
+  </si>
+  <si>
+    <t>Preparação e reunião com o cliente</t>
+  </si>
+  <si>
+    <t>Reunião com o cliente e alinhamento de ideias e propostas para o projeto</t>
+  </si>
+  <si>
+    <t>Reunião com o cliente e definição das prioridades</t>
+  </si>
+  <si>
+    <t>Planejamento da sprint 1, preparação para a reunião com cliente e criaram um template para reunir os documentos compartilhados com os integrantes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -1128,18 +1139,6 @@
     <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1148,6 +1147,18 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="27" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1530,7 +1541,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK942"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -7340,11 +7351,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CR7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="CS1" sqref="CS1:GO1048576"/>
+      <selection activeCell="G4" sqref="G4:G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -7366,7 +7377,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A1" s="101" t="s">
+      <c r="A1" s="97" t="s">
         <v>102</v>
       </c>
       <c r="B1" s="88" t="s">
@@ -7646,7 +7657,7 @@
       </c>
     </row>
     <row r="2" spans="1:96" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="102"/>
+      <c r="A2" s="98"/>
       <c r="B2" s="88" t="s">
         <v>104</v>
       </c>
@@ -7756,7 +7767,7 @@
       <c r="CR2" s="100"/>
     </row>
     <row r="3" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A3" s="103"/>
+      <c r="A3" s="99"/>
       <c r="B3" s="88" t="s">
         <v>110</v>
       </c>
@@ -8044,10 +8055,10 @@
       </c>
     </row>
     <row r="4" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="97" t="s">
+      <c r="A4" s="102" t="s">
         <v>111</v>
       </c>
-      <c r="B4" s="98"/>
+      <c r="B4" s="103"/>
       <c r="C4" s="86" t="s">
         <v>118</v>
       </c>
@@ -8060,7 +8071,9 @@
       <c r="F4" s="86" t="s">
         <v>128</v>
       </c>
-      <c r="G4" s="86"/>
+      <c r="G4" s="86" t="s">
+        <v>132</v>
+      </c>
       <c r="H4" s="86"/>
       <c r="I4" s="86"/>
       <c r="J4" s="86"/>
@@ -8071,27 +8084,27 @@
       <c r="O4" s="85"/>
       <c r="P4" s="85"/>
       <c r="Q4" s="85"/>
-      <c r="AV4" s="99" t="s">
+      <c r="AV4" s="101" t="s">
         <v>112</v>
       </c>
-      <c r="AW4" s="99" t="s">
+      <c r="AW4" s="101" t="s">
         <v>112</v>
       </c>
-      <c r="BT4" s="99" t="s">
+      <c r="BT4" s="101" t="s">
         <v>113</v>
       </c>
-      <c r="BW4" s="99" t="s">
+      <c r="BW4" s="101" t="s">
         <v>114</v>
       </c>
-      <c r="CO4" s="99" t="s">
+      <c r="CO4" s="101" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="97" t="s">
+      <c r="A5" s="102" t="s">
         <v>115</v>
       </c>
-      <c r="B5" s="98"/>
+      <c r="B5" s="103"/>
       <c r="C5" s="86" t="s">
         <v>118</v>
       </c>
@@ -8104,7 +8117,9 @@
       <c r="F5" s="86" t="s">
         <v>129</v>
       </c>
-      <c r="G5" s="86"/>
+      <c r="G5" s="86" t="s">
+        <v>133</v>
+      </c>
       <c r="H5" s="86"/>
       <c r="I5" s="86"/>
       <c r="J5" s="86"/>
@@ -8115,17 +8130,17 @@
       <c r="O5" s="85"/>
       <c r="P5" s="85"/>
       <c r="Q5" s="85"/>
-      <c r="AV5" s="99"/>
-      <c r="AW5" s="99"/>
-      <c r="BT5" s="99"/>
-      <c r="BW5" s="99"/>
-      <c r="CO5" s="99"/>
+      <c r="AV5" s="101"/>
+      <c r="AW5" s="101"/>
+      <c r="BT5" s="101"/>
+      <c r="BW5" s="101"/>
+      <c r="CO5" s="101"/>
     </row>
     <row r="6" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="97" t="s">
+      <c r="A6" s="102" t="s">
         <v>116</v>
       </c>
-      <c r="B6" s="98"/>
+      <c r="B6" s="103"/>
       <c r="C6" s="86" t="s">
         <v>118</v>
       </c>
@@ -8138,7 +8153,9 @@
       <c r="F6" s="86" t="s">
         <v>130</v>
       </c>
-      <c r="G6" s="86"/>
+      <c r="G6" s="86" t="s">
+        <v>134</v>
+      </c>
       <c r="H6" s="86"/>
       <c r="I6" s="86"/>
       <c r="J6" s="86"/>
@@ -8149,17 +8166,17 @@
       <c r="O6" s="85"/>
       <c r="P6" s="85"/>
       <c r="Q6" s="85"/>
-      <c r="AV6" s="99"/>
-      <c r="AW6" s="99"/>
-      <c r="BT6" s="99"/>
-      <c r="BW6" s="99"/>
-      <c r="CO6" s="99"/>
+      <c r="AV6" s="101"/>
+      <c r="AW6" s="101"/>
+      <c r="BT6" s="101"/>
+      <c r="BW6" s="101"/>
+      <c r="CO6" s="101"/>
     </row>
     <row r="7" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="97" t="s">
+      <c r="A7" s="102" t="s">
         <v>117</v>
       </c>
-      <c r="B7" s="98"/>
+      <c r="B7" s="103"/>
       <c r="C7" s="86" t="s">
         <v>118</v>
       </c>
@@ -8172,7 +8189,9 @@
       <c r="F7" s="86" t="s">
         <v>131</v>
       </c>
-      <c r="G7" s="86"/>
+      <c r="G7" s="86" t="s">
+        <v>135</v>
+      </c>
       <c r="H7" s="86"/>
       <c r="I7" s="86"/>
       <c r="J7" s="86"/>
@@ -8183,29 +8202,29 @@
       <c r="O7" s="85"/>
       <c r="P7" s="85"/>
       <c r="Q7" s="85"/>
-      <c r="AV7" s="99"/>
-      <c r="AW7" s="99"/>
-      <c r="BT7" s="99"/>
-      <c r="BW7" s="99"/>
-      <c r="CO7" s="99"/>
+      <c r="AV7" s="101"/>
+      <c r="AW7" s="101"/>
+      <c r="BT7" s="101"/>
+      <c r="BW7" s="101"/>
+      <c r="CO7" s="101"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="AV4:AV7"/>
+    <mergeCell ref="CE2:CR2"/>
+    <mergeCell ref="AW4:AW7"/>
+    <mergeCell ref="BT4:BT7"/>
+    <mergeCell ref="BW4:BW7"/>
+    <mergeCell ref="CO4:CO7"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="C2:Q2"/>
     <mergeCell ref="R2:AL2"/>
     <mergeCell ref="AM2:BI2"/>
     <mergeCell ref="BJ2:CD2"/>
-    <mergeCell ref="CE2:CR2"/>
-    <mergeCell ref="AW4:AW7"/>
-    <mergeCell ref="BT4:BT7"/>
-    <mergeCell ref="BW4:BW7"/>
-    <mergeCell ref="CO4:CO7"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="AV4:AV7"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Adiciona daily realizada no dia 20-08
</commit_message>
<xml_diff>
--- a/Cronograma/Projeto-Cronograma - Acompanhamento.xlsx
+++ b/Cronograma/Projeto-Cronograma - Acompanhamento.xlsx
@@ -105,7 +105,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="140">
   <si>
     <t>REDES</t>
   </si>
@@ -513,6 +513,18 @@
   </si>
   <si>
     <t>Planejamento da sprint 1, preparação para a reunião com cliente e criaram um template para reunir os documentos compartilhados com os integrantes</t>
+  </si>
+  <si>
+    <t>Definição de funcionalidades de usuários, Apresentação SpaceNeedle e background da tela de login</t>
+  </si>
+  <si>
+    <t>Modelo lógico do banco de dados e Apresentação SpaceNeedle</t>
+  </si>
+  <si>
+    <t>Apresentação SpaceNeedle e pesquisa de tecnologias que serão utilizadas</t>
+  </si>
+  <si>
+    <t>Apresentação SpaceNeedle, criação de formulário de pesquisa para definir a persona de usuários e entrevista com o cliente</t>
   </si>
 </sst>
 </file>
@@ -1139,6 +1151,18 @@
     <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1147,18 +1171,6 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="27" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -7355,7 +7367,7 @@
   <dimension ref="A1:CR7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4:G7"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -7377,7 +7389,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A1" s="97" t="s">
+      <c r="A1" s="101" t="s">
         <v>102</v>
       </c>
       <c r="B1" s="88" t="s">
@@ -7657,7 +7669,7 @@
       </c>
     </row>
     <row r="2" spans="1:96" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="98"/>
+      <c r="A2" s="102"/>
       <c r="B2" s="88" t="s">
         <v>104</v>
       </c>
@@ -7767,7 +7779,7 @@
       <c r="CR2" s="100"/>
     </row>
     <row r="3" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A3" s="99"/>
+      <c r="A3" s="103"/>
       <c r="B3" s="88" t="s">
         <v>110</v>
       </c>
@@ -8055,10 +8067,10 @@
       </c>
     </row>
     <row r="4" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="102" t="s">
+      <c r="A4" s="97" t="s">
         <v>111</v>
       </c>
-      <c r="B4" s="103"/>
+      <c r="B4" s="98"/>
       <c r="C4" s="86" t="s">
         <v>118</v>
       </c>
@@ -8074,7 +8086,9 @@
       <c r="G4" s="86" t="s">
         <v>132</v>
       </c>
-      <c r="H4" s="86"/>
+      <c r="H4" s="86" t="s">
+        <v>136</v>
+      </c>
       <c r="I4" s="86"/>
       <c r="J4" s="86"/>
       <c r="K4" s="86"/>
@@ -8084,27 +8098,27 @@
       <c r="O4" s="85"/>
       <c r="P4" s="85"/>
       <c r="Q4" s="85"/>
-      <c r="AV4" s="101" t="s">
+      <c r="AV4" s="99" t="s">
         <v>112</v>
       </c>
-      <c r="AW4" s="101" t="s">
+      <c r="AW4" s="99" t="s">
         <v>112</v>
       </c>
-      <c r="BT4" s="101" t="s">
+      <c r="BT4" s="99" t="s">
         <v>113</v>
       </c>
-      <c r="BW4" s="101" t="s">
+      <c r="BW4" s="99" t="s">
         <v>114</v>
       </c>
-      <c r="CO4" s="101" t="s">
+      <c r="CO4" s="99" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="102" t="s">
+      <c r="A5" s="97" t="s">
         <v>115</v>
       </c>
-      <c r="B5" s="103"/>
+      <c r="B5" s="98"/>
       <c r="C5" s="86" t="s">
         <v>118</v>
       </c>
@@ -8120,7 +8134,9 @@
       <c r="G5" s="86" t="s">
         <v>133</v>
       </c>
-      <c r="H5" s="86"/>
+      <c r="H5" s="86" t="s">
+        <v>138</v>
+      </c>
       <c r="I5" s="86"/>
       <c r="J5" s="86"/>
       <c r="K5" s="86"/>
@@ -8130,17 +8146,17 @@
       <c r="O5" s="85"/>
       <c r="P5" s="85"/>
       <c r="Q5" s="85"/>
-      <c r="AV5" s="101"/>
-      <c r="AW5" s="101"/>
-      <c r="BT5" s="101"/>
-      <c r="BW5" s="101"/>
-      <c r="CO5" s="101"/>
+      <c r="AV5" s="99"/>
+      <c r="AW5" s="99"/>
+      <c r="BT5" s="99"/>
+      <c r="BW5" s="99"/>
+      <c r="CO5" s="99"/>
     </row>
     <row r="6" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="102" t="s">
+      <c r="A6" s="97" t="s">
         <v>116</v>
       </c>
-      <c r="B6" s="103"/>
+      <c r="B6" s="98"/>
       <c r="C6" s="86" t="s">
         <v>118</v>
       </c>
@@ -8156,7 +8172,9 @@
       <c r="G6" s="86" t="s">
         <v>134</v>
       </c>
-      <c r="H6" s="86"/>
+      <c r="H6" s="86" t="s">
+        <v>137</v>
+      </c>
       <c r="I6" s="86"/>
       <c r="J6" s="86"/>
       <c r="K6" s="86"/>
@@ -8166,17 +8184,17 @@
       <c r="O6" s="85"/>
       <c r="P6" s="85"/>
       <c r="Q6" s="85"/>
-      <c r="AV6" s="101"/>
-      <c r="AW6" s="101"/>
-      <c r="BT6" s="101"/>
-      <c r="BW6" s="101"/>
-      <c r="CO6" s="101"/>
+      <c r="AV6" s="99"/>
+      <c r="AW6" s="99"/>
+      <c r="BT6" s="99"/>
+      <c r="BW6" s="99"/>
+      <c r="CO6" s="99"/>
     </row>
     <row r="7" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="102" t="s">
+      <c r="A7" s="97" t="s">
         <v>117</v>
       </c>
-      <c r="B7" s="103"/>
+      <c r="B7" s="98"/>
       <c r="C7" s="86" t="s">
         <v>118</v>
       </c>
@@ -8192,7 +8210,9 @@
       <c r="G7" s="86" t="s">
         <v>135</v>
       </c>
-      <c r="H7" s="86"/>
+      <c r="H7" s="86" t="s">
+        <v>139</v>
+      </c>
       <c r="I7" s="86"/>
       <c r="J7" s="86"/>
       <c r="K7" s="86"/>
@@ -8202,29 +8222,29 @@
       <c r="O7" s="85"/>
       <c r="P7" s="85"/>
       <c r="Q7" s="85"/>
-      <c r="AV7" s="101"/>
-      <c r="AW7" s="101"/>
-      <c r="BT7" s="101"/>
-      <c r="BW7" s="101"/>
-      <c r="CO7" s="101"/>
+      <c r="AV7" s="99"/>
+      <c r="AW7" s="99"/>
+      <c r="BT7" s="99"/>
+      <c r="BW7" s="99"/>
+      <c r="CO7" s="99"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="C2:Q2"/>
+    <mergeCell ref="R2:AL2"/>
+    <mergeCell ref="AM2:BI2"/>
+    <mergeCell ref="BJ2:CD2"/>
+    <mergeCell ref="CE2:CR2"/>
+    <mergeCell ref="AW4:AW7"/>
+    <mergeCell ref="BT4:BT7"/>
+    <mergeCell ref="BW4:BW7"/>
+    <mergeCell ref="CO4:CO7"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="AV4:AV7"/>
-    <mergeCell ref="CE2:CR2"/>
-    <mergeCell ref="AW4:AW7"/>
-    <mergeCell ref="BT4:BT7"/>
-    <mergeCell ref="BW4:BW7"/>
-    <mergeCell ref="CO4:CO7"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="C2:Q2"/>
-    <mergeCell ref="R2:AL2"/>
-    <mergeCell ref="AM2:BI2"/>
-    <mergeCell ref="BJ2:CD2"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Adiciona daily realizada no dia 21-08, Altera nome dos diarios de bordo turma A e B
</commit_message>
<xml_diff>
--- a/Cronograma/Projeto-Cronograma - Acompanhamento.xlsx
+++ b/Cronograma/Projeto-Cronograma - Acompanhamento.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Works\Cursos\senai_desenvolvimento\2s2019\2s2019-t3-mentoria\Cronograma\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\39893838843\Downloads\2s2019-t3-mentoria\Cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5010DCC1-13BF-4D53-A15A-15066D2C484F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Proj-Cronograma" sheetId="1" r:id="rId1"/>
@@ -26,12 +25,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Saulo Santos</author>
   </authors>
   <commentList>
-    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
+    <comment ref="A4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -48,7 +47,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
+    <comment ref="A5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -65,7 +64,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
+    <comment ref="A6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -83,7 +82,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
+    <comment ref="A7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -106,7 +105,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="144">
   <si>
     <t>REDES</t>
   </si>
@@ -526,12 +525,24 @@
   </si>
   <si>
     <t>Apresentação SpaceNeedle, criação de formulário de pesquisa para definir a persona de usuários e entrevista com o cliente</t>
+  </si>
+  <si>
+    <t>Criação de três opções de layout de login, diagrama de classes do usuário e melhor organização do planejamento da sprint</t>
+  </si>
+  <si>
+    <t>Executaram comandos do projeto 1 e analisaram os retornos. Planejamento da sprint 1 no Azure DevOps</t>
+  </si>
+  <si>
+    <t>Planejaram o projeto como um todo dividindo todas as sprints e estudo da estrutura do banco de dados</t>
+  </si>
+  <si>
+    <t>Formulários para definição de personas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -1137,6 +1148,9 @@
     <xf numFmtId="0" fontId="13" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1158,6 +1172,18 @@
     <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1165,21 +1191,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="27" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1567,7 +1578,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK942"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -1589,7 +1600,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:116" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="92" t="s">
+      <c r="A1" s="93" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -1929,7 +1940,7 @@
       </c>
     </row>
     <row r="2" spans="1:116" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="92"/>
+      <c r="A2" s="93"/>
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
@@ -2255,15 +2266,15 @@
         <v>12</v>
       </c>
       <c r="DF2" s="11"/>
-      <c r="DG2" s="93"/>
-      <c r="DH2" s="93"/>
-      <c r="DI2" s="93"/>
-      <c r="DJ2" s="93"/>
+      <c r="DG2" s="94"/>
+      <c r="DH2" s="94"/>
+      <c r="DI2" s="94"/>
+      <c r="DJ2" s="94"/>
       <c r="DK2" s="12"/>
       <c r="DL2" s="12"/>
     </row>
     <row r="3" spans="1:116" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="92"/>
+      <c r="A3" s="93"/>
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
@@ -2600,7 +2611,7 @@
       <c r="A4" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="94" t="s">
+      <c r="B4" s="95" t="s">
         <v>38</v>
       </c>
       <c r="C4" s="20" t="s">
@@ -2742,7 +2753,7 @@
       <c r="A5" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="94"/>
+      <c r="B5" s="95"/>
       <c r="C5" s="22"/>
       <c r="D5" s="22"/>
       <c r="E5" s="22"/>
@@ -2882,7 +2893,7 @@
       <c r="A6" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="B6" s="94"/>
+      <c r="B6" s="95"/>
       <c r="C6" s="22"/>
       <c r="D6" s="22"/>
       <c r="E6" s="22"/>
@@ -3022,7 +3033,7 @@
       <c r="A7" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="B7" s="94"/>
+      <c r="B7" s="95"/>
       <c r="C7" s="22"/>
       <c r="D7" s="22"/>
       <c r="E7" s="22"/>
@@ -3160,7 +3171,7 @@
       <c r="A8" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="B8" s="94"/>
+      <c r="B8" s="95"/>
       <c r="C8" s="22"/>
       <c r="D8" s="22"/>
       <c r="E8" s="22"/>
@@ -3300,7 +3311,7 @@
       <c r="A9" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="B9" s="95" t="s">
+      <c r="B9" s="96" t="s">
         <v>58</v>
       </c>
       <c r="C9" s="22"/>
@@ -3442,7 +3453,7 @@
       <c r="A10" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="B10" s="95"/>
+      <c r="B10" s="96"/>
       <c r="C10" s="22"/>
       <c r="D10" s="22"/>
       <c r="E10" s="22"/>
@@ -3582,7 +3593,7 @@
       <c r="A11" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="B11" s="96" t="s">
+      <c r="B11" s="97" t="s">
         <v>66</v>
       </c>
       <c r="C11" s="22"/>
@@ -3712,7 +3723,7 @@
       <c r="A12" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="B12" s="96"/>
+      <c r="B12" s="97"/>
       <c r="C12" s="22"/>
       <c r="D12" s="22"/>
       <c r="E12" s="22"/>
@@ -3850,7 +3861,7 @@
       <c r="A13" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="B13" s="96"/>
+      <c r="B13" s="97"/>
       <c r="C13" s="22"/>
       <c r="D13" s="22"/>
       <c r="E13" s="22"/>
@@ -3990,7 +4001,7 @@
       <c r="A14" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="B14" s="96"/>
+      <c r="B14" s="97"/>
       <c r="C14" s="22"/>
       <c r="D14" s="22"/>
       <c r="E14" s="22"/>
@@ -4126,7 +4137,7 @@
       <c r="A15" s="35" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="96"/>
+      <c r="B15" s="97"/>
       <c r="C15" s="22"/>
       <c r="D15" s="22"/>
       <c r="E15" s="22"/>
@@ -4262,7 +4273,7 @@
       <c r="A16" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="B16" s="96"/>
+      <c r="B16" s="97"/>
       <c r="C16" s="22"/>
       <c r="D16" s="22"/>
       <c r="E16" s="22"/>
@@ -4398,7 +4409,7 @@
       <c r="A17" s="35" t="s">
         <v>78</v>
       </c>
-      <c r="B17" s="96"/>
+      <c r="B17" s="97"/>
       <c r="C17" s="22"/>
       <c r="D17" s="22"/>
       <c r="E17" s="22"/>
@@ -4534,7 +4545,7 @@
       <c r="A18" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="B18" s="96"/>
+      <c r="B18" s="97"/>
       <c r="C18" s="22"/>
       <c r="D18" s="22"/>
       <c r="E18" s="22"/>
@@ -4674,7 +4685,7 @@
       <c r="A19" s="40" t="s">
         <v>81</v>
       </c>
-      <c r="B19" s="96"/>
+      <c r="B19" s="97"/>
       <c r="C19" s="22"/>
       <c r="D19" s="22"/>
       <c r="E19" s="22"/>
@@ -4810,7 +4821,7 @@
       <c r="A20" s="43" t="s">
         <v>82</v>
       </c>
-      <c r="B20" s="96"/>
+      <c r="B20" s="97"/>
       <c r="C20" s="22"/>
       <c r="D20" s="22"/>
       <c r="E20" s="22"/>
@@ -4946,7 +4957,7 @@
       <c r="A21" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="B21" s="90" t="s">
+      <c r="B21" s="91" t="s">
         <v>86</v>
       </c>
       <c r="C21" s="22"/>
@@ -5080,7 +5091,7 @@
       <c r="A22" s="50" t="s">
         <v>88</v>
       </c>
-      <c r="B22" s="90"/>
+      <c r="B22" s="91"/>
       <c r="C22" s="22"/>
       <c r="D22" s="22"/>
       <c r="E22" s="22"/>
@@ -5216,7 +5227,7 @@
       <c r="A23" s="54" t="s">
         <v>89</v>
       </c>
-      <c r="B23" s="90"/>
+      <c r="B23" s="91"/>
       <c r="C23" s="22"/>
       <c r="D23" s="22"/>
       <c r="E23" s="22"/>
@@ -5348,7 +5359,7 @@
       <c r="A24" s="57" t="s">
         <v>90</v>
       </c>
-      <c r="B24" s="90"/>
+      <c r="B24" s="91"/>
       <c r="C24" s="22"/>
       <c r="D24" s="22"/>
       <c r="E24" s="22"/>
@@ -5482,7 +5493,7 @@
       <c r="A25" s="60" t="s">
         <v>92</v>
       </c>
-      <c r="B25" s="90"/>
+      <c r="B25" s="91"/>
       <c r="C25" s="22"/>
       <c r="D25" s="22"/>
       <c r="E25" s="22"/>
@@ -5626,7 +5637,7 @@
       <c r="A26" s="62" t="s">
         <v>93</v>
       </c>
-      <c r="B26" s="91" t="s">
+      <c r="B26" s="92" t="s">
         <v>58</v>
       </c>
       <c r="C26" s="22"/>
@@ -5760,7 +5771,7 @@
       <c r="A27" s="65" t="s">
         <v>95</v>
       </c>
-      <c r="B27" s="91"/>
+      <c r="B27" s="92"/>
       <c r="C27" s="22"/>
       <c r="D27" s="22"/>
       <c r="E27" s="22"/>
@@ -5900,7 +5911,7 @@
       <c r="A28" s="68" t="s">
         <v>97</v>
       </c>
-      <c r="B28" s="91"/>
+      <c r="B28" s="92"/>
       <c r="C28" s="22"/>
       <c r="D28" s="22"/>
       <c r="E28" s="22"/>
@@ -6032,7 +6043,7 @@
       <c r="A29" s="71" t="s">
         <v>99</v>
       </c>
-      <c r="B29" s="91"/>
+      <c r="B29" s="92"/>
       <c r="C29" s="22"/>
       <c r="D29" s="22"/>
       <c r="E29" s="22"/>
@@ -6160,7 +6171,7 @@
       <c r="A30" s="74" t="s">
         <v>100</v>
       </c>
-      <c r="B30" s="91"/>
+      <c r="B30" s="92"/>
       <c r="C30" s="22"/>
       <c r="D30" s="22"/>
       <c r="E30" s="22"/>
@@ -6286,7 +6297,7 @@
       <c r="A31" s="62" t="s">
         <v>101</v>
       </c>
-      <c r="B31" s="91"/>
+      <c r="B31" s="92"/>
       <c r="C31" s="22"/>
       <c r="D31" s="22"/>
       <c r="E31" s="22"/>
@@ -7377,11 +7388,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CR7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -7403,7 +7414,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A1" s="97" t="s">
+      <c r="A1" s="102" t="s">
         <v>102</v>
       </c>
       <c r="B1" s="88" t="s">
@@ -7683,121 +7694,121 @@
       </c>
     </row>
     <row r="2" spans="1:96" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="98"/>
+      <c r="A2" s="103"/>
       <c r="B2" s="88" t="s">
         <v>104</v>
       </c>
-      <c r="C2" s="100" t="s">
+      <c r="C2" s="101" t="s">
         <v>105</v>
       </c>
-      <c r="D2" s="100"/>
-      <c r="E2" s="100"/>
-      <c r="F2" s="100"/>
-      <c r="G2" s="100"/>
-      <c r="H2" s="100"/>
-      <c r="I2" s="100"/>
-      <c r="J2" s="100"/>
-      <c r="K2" s="100"/>
-      <c r="L2" s="100"/>
-      <c r="M2" s="100"/>
-      <c r="N2" s="100"/>
-      <c r="O2" s="100"/>
-      <c r="P2" s="100"/>
-      <c r="Q2" s="100"/>
-      <c r="R2" s="100" t="s">
+      <c r="D2" s="101"/>
+      <c r="E2" s="101"/>
+      <c r="F2" s="101"/>
+      <c r="G2" s="101"/>
+      <c r="H2" s="101"/>
+      <c r="I2" s="101"/>
+      <c r="J2" s="101"/>
+      <c r="K2" s="101"/>
+      <c r="L2" s="101"/>
+      <c r="M2" s="101"/>
+      <c r="N2" s="101"/>
+      <c r="O2" s="101"/>
+      <c r="P2" s="101"/>
+      <c r="Q2" s="101"/>
+      <c r="R2" s="101" t="s">
         <v>106</v>
       </c>
-      <c r="S2" s="100"/>
-      <c r="T2" s="100"/>
-      <c r="U2" s="100"/>
-      <c r="V2" s="100"/>
-      <c r="W2" s="100"/>
-      <c r="X2" s="100"/>
-      <c r="Y2" s="100"/>
-      <c r="Z2" s="100"/>
-      <c r="AA2" s="100"/>
-      <c r="AB2" s="100"/>
-      <c r="AC2" s="100"/>
-      <c r="AD2" s="100"/>
-      <c r="AE2" s="100"/>
-      <c r="AF2" s="100"/>
-      <c r="AG2" s="100"/>
-      <c r="AH2" s="100"/>
-      <c r="AI2" s="100"/>
-      <c r="AJ2" s="100"/>
-      <c r="AK2" s="100"/>
-      <c r="AL2" s="100"/>
-      <c r="AM2" s="100" t="s">
+      <c r="S2" s="101"/>
+      <c r="T2" s="101"/>
+      <c r="U2" s="101"/>
+      <c r="V2" s="101"/>
+      <c r="W2" s="101"/>
+      <c r="X2" s="101"/>
+      <c r="Y2" s="101"/>
+      <c r="Z2" s="101"/>
+      <c r="AA2" s="101"/>
+      <c r="AB2" s="101"/>
+      <c r="AC2" s="101"/>
+      <c r="AD2" s="101"/>
+      <c r="AE2" s="101"/>
+      <c r="AF2" s="101"/>
+      <c r="AG2" s="101"/>
+      <c r="AH2" s="101"/>
+      <c r="AI2" s="101"/>
+      <c r="AJ2" s="101"/>
+      <c r="AK2" s="101"/>
+      <c r="AL2" s="101"/>
+      <c r="AM2" s="101" t="s">
         <v>107</v>
       </c>
-      <c r="AN2" s="100"/>
-      <c r="AO2" s="100"/>
-      <c r="AP2" s="100"/>
-      <c r="AQ2" s="100"/>
-      <c r="AR2" s="100"/>
-      <c r="AS2" s="100"/>
-      <c r="AT2" s="100"/>
-      <c r="AU2" s="100"/>
-      <c r="AV2" s="100"/>
-      <c r="AW2" s="100"/>
-      <c r="AX2" s="100"/>
-      <c r="AY2" s="100"/>
-      <c r="AZ2" s="100"/>
-      <c r="BA2" s="100"/>
-      <c r="BB2" s="100"/>
-      <c r="BC2" s="100"/>
-      <c r="BD2" s="100"/>
-      <c r="BE2" s="100"/>
-      <c r="BF2" s="100"/>
-      <c r="BG2" s="100"/>
-      <c r="BH2" s="100"/>
-      <c r="BI2" s="100"/>
-      <c r="BJ2" s="100" t="s">
+      <c r="AN2" s="101"/>
+      <c r="AO2" s="101"/>
+      <c r="AP2" s="101"/>
+      <c r="AQ2" s="101"/>
+      <c r="AR2" s="101"/>
+      <c r="AS2" s="101"/>
+      <c r="AT2" s="101"/>
+      <c r="AU2" s="101"/>
+      <c r="AV2" s="101"/>
+      <c r="AW2" s="101"/>
+      <c r="AX2" s="101"/>
+      <c r="AY2" s="101"/>
+      <c r="AZ2" s="101"/>
+      <c r="BA2" s="101"/>
+      <c r="BB2" s="101"/>
+      <c r="BC2" s="101"/>
+      <c r="BD2" s="101"/>
+      <c r="BE2" s="101"/>
+      <c r="BF2" s="101"/>
+      <c r="BG2" s="101"/>
+      <c r="BH2" s="101"/>
+      <c r="BI2" s="101"/>
+      <c r="BJ2" s="101" t="s">
         <v>108</v>
       </c>
-      <c r="BK2" s="100"/>
-      <c r="BL2" s="100"/>
-      <c r="BM2" s="100"/>
-      <c r="BN2" s="100"/>
-      <c r="BO2" s="100"/>
-      <c r="BP2" s="100"/>
-      <c r="BQ2" s="100"/>
-      <c r="BR2" s="100"/>
-      <c r="BS2" s="100"/>
-      <c r="BT2" s="100"/>
-      <c r="BU2" s="100"/>
-      <c r="BV2" s="100"/>
-      <c r="BW2" s="100"/>
-      <c r="BX2" s="100"/>
-      <c r="BY2" s="100"/>
-      <c r="BZ2" s="100"/>
-      <c r="CA2" s="100"/>
-      <c r="CB2" s="100"/>
-      <c r="CC2" s="100"/>
-      <c r="CD2" s="100"/>
-      <c r="CE2" s="100" t="s">
+      <c r="BK2" s="101"/>
+      <c r="BL2" s="101"/>
+      <c r="BM2" s="101"/>
+      <c r="BN2" s="101"/>
+      <c r="BO2" s="101"/>
+      <c r="BP2" s="101"/>
+      <c r="BQ2" s="101"/>
+      <c r="BR2" s="101"/>
+      <c r="BS2" s="101"/>
+      <c r="BT2" s="101"/>
+      <c r="BU2" s="101"/>
+      <c r="BV2" s="101"/>
+      <c r="BW2" s="101"/>
+      <c r="BX2" s="101"/>
+      <c r="BY2" s="101"/>
+      <c r="BZ2" s="101"/>
+      <c r="CA2" s="101"/>
+      <c r="CB2" s="101"/>
+      <c r="CC2" s="101"/>
+      <c r="CD2" s="101"/>
+      <c r="CE2" s="101" t="s">
         <v>109</v>
       </c>
-      <c r="CF2" s="100"/>
-      <c r="CG2" s="100"/>
-      <c r="CH2" s="100"/>
-      <c r="CI2" s="100"/>
-      <c r="CJ2" s="100"/>
-      <c r="CK2" s="100"/>
-      <c r="CL2" s="100"/>
-      <c r="CM2" s="100"/>
-      <c r="CN2" s="100"/>
-      <c r="CO2" s="100"/>
-      <c r="CP2" s="100"/>
-      <c r="CQ2" s="100"/>
-      <c r="CR2" s="100"/>
+      <c r="CF2" s="101"/>
+      <c r="CG2" s="101"/>
+      <c r="CH2" s="101"/>
+      <c r="CI2" s="101"/>
+      <c r="CJ2" s="101"/>
+      <c r="CK2" s="101"/>
+      <c r="CL2" s="101"/>
+      <c r="CM2" s="101"/>
+      <c r="CN2" s="101"/>
+      <c r="CO2" s="101"/>
+      <c r="CP2" s="101"/>
+      <c r="CQ2" s="101"/>
+      <c r="CR2" s="101"/>
     </row>
     <row r="3" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A3" s="99"/>
+      <c r="A3" s="104"/>
       <c r="B3" s="88" t="s">
         <v>110</v>
       </c>
-      <c r="C3" s="104">
+      <c r="C3" s="90">
         <v>12</v>
       </c>
       <c r="D3" s="89">
@@ -7809,10 +7820,10 @@
       <c r="F3" s="89">
         <v>15</v>
       </c>
-      <c r="G3" s="104">
+      <c r="G3" s="90">
         <v>16</v>
       </c>
-      <c r="H3" s="104">
+      <c r="H3" s="90">
         <v>19</v>
       </c>
       <c r="I3" s="89">
@@ -7824,10 +7835,10 @@
       <c r="K3" s="89">
         <v>22</v>
       </c>
-      <c r="L3" s="104">
+      <c r="L3" s="90">
         <v>23</v>
       </c>
-      <c r="M3" s="104">
+      <c r="M3" s="90">
         <v>26</v>
       </c>
       <c r="N3" s="89">
@@ -8081,10 +8092,10 @@
       </c>
     </row>
     <row r="4" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="102" t="s">
+      <c r="A4" s="98" t="s">
         <v>111</v>
       </c>
-      <c r="B4" s="103"/>
+      <c r="B4" s="99"/>
       <c r="C4" s="86" t="s">
         <v>118</v>
       </c>
@@ -8103,7 +8114,9 @@
       <c r="H4" s="86" t="s">
         <v>136</v>
       </c>
-      <c r="I4" s="86"/>
+      <c r="I4" s="86" t="s">
+        <v>140</v>
+      </c>
       <c r="J4" s="86"/>
       <c r="K4" s="86"/>
       <c r="L4" s="86"/>
@@ -8112,27 +8125,27 @@
       <c r="O4" s="85"/>
       <c r="P4" s="85"/>
       <c r="Q4" s="85"/>
-      <c r="AV4" s="101" t="s">
+      <c r="AV4" s="100" t="s">
         <v>112</v>
       </c>
-      <c r="AW4" s="101" t="s">
+      <c r="AW4" s="100" t="s">
         <v>112</v>
       </c>
-      <c r="BT4" s="101" t="s">
+      <c r="BT4" s="100" t="s">
         <v>113</v>
       </c>
-      <c r="BW4" s="101" t="s">
+      <c r="BW4" s="100" t="s">
         <v>114</v>
       </c>
-      <c r="CO4" s="101" t="s">
+      <c r="CO4" s="100" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="102" t="s">
+      <c r="A5" s="98" t="s">
         <v>115</v>
       </c>
-      <c r="B5" s="103"/>
+      <c r="B5" s="99"/>
       <c r="C5" s="86" t="s">
         <v>118</v>
       </c>
@@ -8151,7 +8164,9 @@
       <c r="H5" s="86" t="s">
         <v>138</v>
       </c>
-      <c r="I5" s="86"/>
+      <c r="I5" s="86" t="s">
+        <v>141</v>
+      </c>
       <c r="J5" s="86"/>
       <c r="K5" s="86"/>
       <c r="L5" s="86"/>
@@ -8160,17 +8175,17 @@
       <c r="O5" s="85"/>
       <c r="P5" s="85"/>
       <c r="Q5" s="85"/>
-      <c r="AV5" s="101"/>
-      <c r="AW5" s="101"/>
-      <c r="BT5" s="101"/>
-      <c r="BW5" s="101"/>
-      <c r="CO5" s="101"/>
+      <c r="AV5" s="100"/>
+      <c r="AW5" s="100"/>
+      <c r="BT5" s="100"/>
+      <c r="BW5" s="100"/>
+      <c r="CO5" s="100"/>
     </row>
     <row r="6" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="102" t="s">
+      <c r="A6" s="98" t="s">
         <v>116</v>
       </c>
-      <c r="B6" s="103"/>
+      <c r="B6" s="99"/>
       <c r="C6" s="86" t="s">
         <v>118</v>
       </c>
@@ -8189,7 +8204,9 @@
       <c r="H6" s="86" t="s">
         <v>137</v>
       </c>
-      <c r="I6" s="86"/>
+      <c r="I6" s="86" t="s">
+        <v>142</v>
+      </c>
       <c r="J6" s="86"/>
       <c r="K6" s="86"/>
       <c r="L6" s="86"/>
@@ -8198,17 +8215,17 @@
       <c r="O6" s="85"/>
       <c r="P6" s="85"/>
       <c r="Q6" s="85"/>
-      <c r="AV6" s="101"/>
-      <c r="AW6" s="101"/>
-      <c r="BT6" s="101"/>
-      <c r="BW6" s="101"/>
-      <c r="CO6" s="101"/>
+      <c r="AV6" s="100"/>
+      <c r="AW6" s="100"/>
+      <c r="BT6" s="100"/>
+      <c r="BW6" s="100"/>
+      <c r="CO6" s="100"/>
     </row>
     <row r="7" spans="1:96" s="84" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="102" t="s">
+      <c r="A7" s="98" t="s">
         <v>117</v>
       </c>
-      <c r="B7" s="103"/>
+      <c r="B7" s="99"/>
       <c r="C7" s="86" t="s">
         <v>118</v>
       </c>
@@ -8227,7 +8244,9 @@
       <c r="H7" s="86" t="s">
         <v>139</v>
       </c>
-      <c r="I7" s="86"/>
+      <c r="I7" s="86" t="s">
+        <v>143</v>
+      </c>
       <c r="J7" s="86"/>
       <c r="K7" s="86"/>
       <c r="L7" s="86"/>
@@ -8236,29 +8255,29 @@
       <c r="O7" s="85"/>
       <c r="P7" s="85"/>
       <c r="Q7" s="85"/>
-      <c r="AV7" s="101"/>
-      <c r="AW7" s="101"/>
-      <c r="BT7" s="101"/>
-      <c r="BW7" s="101"/>
-      <c r="CO7" s="101"/>
+      <c r="AV7" s="100"/>
+      <c r="AW7" s="100"/>
+      <c r="BT7" s="100"/>
+      <c r="BW7" s="100"/>
+      <c r="CO7" s="100"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="C2:Q2"/>
+    <mergeCell ref="R2:AL2"/>
+    <mergeCell ref="AM2:BI2"/>
+    <mergeCell ref="BJ2:CD2"/>
+    <mergeCell ref="CE2:CR2"/>
+    <mergeCell ref="AW4:AW7"/>
+    <mergeCell ref="BT4:BT7"/>
+    <mergeCell ref="BW4:BW7"/>
+    <mergeCell ref="CO4:CO7"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="AV4:AV7"/>
-    <mergeCell ref="CE2:CR2"/>
-    <mergeCell ref="AW4:AW7"/>
-    <mergeCell ref="BT4:BT7"/>
-    <mergeCell ref="BW4:BW7"/>
-    <mergeCell ref="CO4:CO7"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="C2:Q2"/>
-    <mergeCell ref="R2:AL2"/>
-    <mergeCell ref="AM2:BI2"/>
-    <mergeCell ref="BJ2:CD2"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>